<commit_message>
Update Realisasi SP2D (6,01%)
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="454">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -998,6 +998,18 @@
     <t>Penggantian Uang Persediaan KKP untuk keperluan Belanja Barang (BPP 001 Set. BRSDM).</t>
   </si>
   <si>
+    <t>16-FEB-23</t>
+  </si>
+  <si>
+    <t>'00077T</t>
+  </si>
+  <si>
+    <t>'231751303001729</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.88/BRSDM/KP.440/I/2023 Tgl.17 Januari 2023,Surat Tugas Nomor:B.451/BRSDM.1/KP.440/I/2023 Tgl.18 Januari 2023</t>
+  </si>
+  <si>
     <t>'00025T</t>
   </si>
   <si>
@@ -1289,6 +1301,18 @@
     <t>'626402.175.524114.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000907</t>
   </si>
   <si>
+    <t>'00076T</t>
+  </si>
+  <si>
+    <t>'231751301003224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai SPK No:241/PPK/BRSDM.1/I/2023 Tgl.18-1-2023,BAST No:BAST.281/PPK/BRSDM.1/I/2023 Tgl.20-1-2023,BAP NO:282/PPK/BRSDM.1/I/2023 Tgl.20-1-2023 </t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.001341</t>
+  </si>
+  <si>
     <t>'626402.175.524114.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.001342</t>
   </si>
   <si>
@@ -1344,6 +1368,15 @@
   </si>
   <si>
     <t>'626402.175.532111.03212WA.2378EBB.A000000001.00000.1.0151.2.000000.000000.951.102.0A.000785</t>
+  </si>
+  <si>
+    <t>'00075T</t>
+  </si>
+  <si>
+    <t>'231751303001715</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Modal Sesuai SPK No:342/PPK/BRSDM.1/I/2023 Tgl.26-1-2023,BAST No:BAST.383/PPK/BRSDM.1/I/2023 Tgl.30-1-2023,BAP No:384/PPK/BRSDM.1/I/2023 Tgl.30-1-2023 Pengadaan TV WALL</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1718,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L275"/>
+  <dimension ref="A1:L278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -9578,19 +9611,19 @@
         <v>13</v>
       </c>
       <c r="D210" t="s">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="E210" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F210" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G210" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H210" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="I210" t="s">
         <v>19</v>
@@ -9599,10 +9632,10 @@
         <v>1</v>
       </c>
       <c r="K210">
-        <v>45645400</v>
+        <v>1115000</v>
       </c>
       <c r="L210">
-        <v>45645400</v>
+        <v>1115000</v>
       </c>
     </row>
     <row r="211" spans="1:12">
@@ -9616,7 +9649,7 @@
         <v>13</v>
       </c>
       <c r="D211" t="s">
-        <v>62</v>
+        <v>297</v>
       </c>
       <c r="E211" t="s">
         <v>331</v>
@@ -9628,7 +9661,7 @@
         <v>333</v>
       </c>
       <c r="H211" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="I211" t="s">
         <v>19</v>
@@ -9637,10 +9670,10 @@
         <v>1</v>
       </c>
       <c r="K211">
-        <v>6775500</v>
+        <v>45645400</v>
       </c>
       <c r="L211">
-        <v>6775500</v>
+        <v>45645400</v>
       </c>
     </row>
     <row r="212" spans="1:12">
@@ -9654,20 +9687,20 @@
         <v>13</v>
       </c>
       <c r="D212" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="E212" t="s">
+        <v>335</v>
+      </c>
+      <c r="F212" t="s">
+        <v>336</v>
+      </c>
+      <c r="G212" t="s">
+        <v>337</v>
+      </c>
+      <c r="H212" t="s">
         <v>334</v>
       </c>
-      <c r="F212" t="s">
-        <v>335</v>
-      </c>
-      <c r="G212" t="s">
-        <v>336</v>
-      </c>
-      <c r="H212" t="s">
-        <v>337</v>
-      </c>
       <c r="I212" t="s">
         <v>19</v>
       </c>
@@ -9675,10 +9708,10 @@
         <v>1</v>
       </c>
       <c r="K212">
-        <v>7321500</v>
+        <v>6775500</v>
       </c>
       <c r="L212">
-        <v>7321500</v>
+        <v>6775500</v>
       </c>
     </row>
     <row r="213" spans="1:12">
@@ -9692,19 +9725,19 @@
         <v>13</v>
       </c>
       <c r="D213" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E213" t="s">
-        <v>129</v>
+        <v>338</v>
       </c>
       <c r="F213" t="s">
-        <v>130</v>
+        <v>339</v>
       </c>
       <c r="G213" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="H213" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I213" t="s">
         <v>19</v>
@@ -9713,10 +9746,10 @@
         <v>1</v>
       </c>
       <c r="K213">
-        <v>3652800</v>
+        <v>7321500</v>
       </c>
       <c r="L213">
-        <v>3652800</v>
+        <v>7321500</v>
       </c>
     </row>
     <row r="214" spans="1:12">
@@ -9742,7 +9775,7 @@
         <v>131</v>
       </c>
       <c r="H214" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="I214" t="s">
         <v>19</v>
@@ -9751,10 +9784,10 @@
         <v>1</v>
       </c>
       <c r="K214">
-        <v>280000</v>
+        <v>3652800</v>
       </c>
       <c r="L214">
-        <v>280000</v>
+        <v>3652800</v>
       </c>
     </row>
     <row r="215" spans="1:12">
@@ -9768,16 +9801,16 @@
         <v>13</v>
       </c>
       <c r="D215" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E215" t="s">
-        <v>340</v>
+        <v>129</v>
       </c>
       <c r="F215" t="s">
-        <v>341</v>
+        <v>130</v>
       </c>
       <c r="G215" t="s">
-        <v>342</v>
+        <v>131</v>
       </c>
       <c r="H215" t="s">
         <v>343</v>
@@ -9789,10 +9822,10 @@
         <v>1</v>
       </c>
       <c r="K215">
-        <v>50692502</v>
+        <v>280000</v>
       </c>
       <c r="L215">
-        <v>50692502</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="216" spans="1:12">
@@ -9806,7 +9839,7 @@
         <v>13</v>
       </c>
       <c r="D216" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="E216" t="s">
         <v>344</v>
@@ -9818,7 +9851,7 @@
         <v>346</v>
       </c>
       <c r="H216" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="I216" t="s">
         <v>19</v>
@@ -9827,10 +9860,10 @@
         <v>1</v>
       </c>
       <c r="K216">
-        <v>9800000</v>
+        <v>50692502</v>
       </c>
       <c r="L216">
-        <v>9800000</v>
+        <v>50692502</v>
       </c>
     </row>
     <row r="217" spans="1:12">
@@ -9844,16 +9877,16 @@
         <v>13</v>
       </c>
       <c r="D217" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="E217" t="s">
-        <v>141</v>
+        <v>348</v>
       </c>
       <c r="F217" t="s">
-        <v>142</v>
+        <v>349</v>
       </c>
       <c r="G217" t="s">
-        <v>143</v>
+        <v>350</v>
       </c>
       <c r="H217" t="s">
         <v>347</v>
@@ -9865,10 +9898,10 @@
         <v>1</v>
       </c>
       <c r="K217">
-        <v>7096000</v>
+        <v>9800000</v>
       </c>
       <c r="L217">
-        <v>7096000</v>
+        <v>9800000</v>
       </c>
     </row>
     <row r="218" spans="1:12">
@@ -9894,7 +9927,7 @@
         <v>143</v>
       </c>
       <c r="H218" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="I218" t="s">
         <v>19</v>
@@ -9903,10 +9936,10 @@
         <v>1</v>
       </c>
       <c r="K218">
-        <v>15310300</v>
+        <v>7096000</v>
       </c>
       <c r="L218">
-        <v>15310300</v>
+        <v>7096000</v>
       </c>
     </row>
     <row r="219" spans="1:12">
@@ -9932,7 +9965,7 @@
         <v>143</v>
       </c>
       <c r="H219" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I219" t="s">
         <v>19</v>
@@ -9941,10 +9974,10 @@
         <v>1</v>
       </c>
       <c r="K219">
-        <v>410000</v>
+        <v>15310300</v>
       </c>
       <c r="L219">
-        <v>410000</v>
+        <v>15310300</v>
       </c>
     </row>
     <row r="220" spans="1:12">
@@ -9970,7 +10003,7 @@
         <v>143</v>
       </c>
       <c r="H220" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="I220" t="s">
         <v>19</v>
@@ -9979,10 +10012,10 @@
         <v>1</v>
       </c>
       <c r="K220">
-        <v>1380000</v>
+        <v>410000</v>
       </c>
       <c r="L220">
-        <v>1380000</v>
+        <v>410000</v>
       </c>
     </row>
     <row r="221" spans="1:12">
@@ -9996,16 +10029,16 @@
         <v>13</v>
       </c>
       <c r="D221" t="s">
-        <v>212</v>
+        <v>24</v>
       </c>
       <c r="E221" t="s">
-        <v>351</v>
+        <v>141</v>
       </c>
       <c r="F221" t="s">
-        <v>352</v>
+        <v>142</v>
       </c>
       <c r="G221" t="s">
-        <v>353</v>
+        <v>143</v>
       </c>
       <c r="H221" t="s">
         <v>354</v>
@@ -10017,10 +10050,10 @@
         <v>1</v>
       </c>
       <c r="K221">
-        <v>16394000</v>
+        <v>1380000</v>
       </c>
       <c r="L221">
-        <v>16394000</v>
+        <v>1380000</v>
       </c>
     </row>
     <row r="222" spans="1:12">
@@ -10034,19 +10067,19 @@
         <v>13</v>
       </c>
       <c r="D222" t="s">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="E222" t="s">
-        <v>141</v>
+        <v>355</v>
       </c>
       <c r="F222" t="s">
-        <v>142</v>
+        <v>356</v>
       </c>
       <c r="G222" t="s">
-        <v>143</v>
+        <v>357</v>
       </c>
       <c r="H222" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="I222" t="s">
         <v>19</v>
@@ -10055,10 +10088,10 @@
         <v>1</v>
       </c>
       <c r="K222">
-        <v>3300000</v>
+        <v>16394000</v>
       </c>
       <c r="L222">
-        <v>3300000</v>
+        <v>16394000</v>
       </c>
     </row>
     <row r="223" spans="1:12">
@@ -10072,19 +10105,19 @@
         <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>297</v>
+        <v>24</v>
       </c>
       <c r="E223" t="s">
-        <v>356</v>
+        <v>141</v>
       </c>
       <c r="F223" t="s">
-        <v>357</v>
+        <v>142</v>
       </c>
       <c r="G223" t="s">
-        <v>307</v>
+        <v>143</v>
       </c>
       <c r="H223" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I223" t="s">
         <v>19</v>
@@ -10093,10 +10126,10 @@
         <v>1</v>
       </c>
       <c r="K223">
-        <v>93138974</v>
+        <v>3300000</v>
       </c>
       <c r="L223">
-        <v>93138974</v>
+        <v>3300000</v>
       </c>
     </row>
     <row r="224" spans="1:12">
@@ -10113,16 +10146,16 @@
         <v>297</v>
       </c>
       <c r="E224" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F224" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G224" t="s">
         <v>307</v>
       </c>
       <c r="H224" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I224" t="s">
         <v>19</v>
@@ -10131,10 +10164,10 @@
         <v>1</v>
       </c>
       <c r="K224">
-        <v>15082960</v>
+        <v>93138974</v>
       </c>
       <c r="L224">
-        <v>15082960</v>
+        <v>93138974</v>
       </c>
     </row>
     <row r="225" spans="1:12">
@@ -10148,19 +10181,19 @@
         <v>13</v>
       </c>
       <c r="D225" t="s">
-        <v>109</v>
+        <v>297</v>
       </c>
       <c r="E225" t="s">
-        <v>110</v>
+        <v>363</v>
       </c>
       <c r="F225" t="s">
-        <v>111</v>
+        <v>364</v>
       </c>
       <c r="G225" t="s">
-        <v>112</v>
+        <v>307</v>
       </c>
       <c r="H225" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="I225" t="s">
         <v>19</v>
@@ -10169,10 +10202,10 @@
         <v>1</v>
       </c>
       <c r="K225">
-        <v>450000</v>
+        <v>15082960</v>
       </c>
       <c r="L225">
-        <v>450000</v>
+        <v>15082960</v>
       </c>
     </row>
     <row r="226" spans="1:12">
@@ -10186,16 +10219,16 @@
         <v>13</v>
       </c>
       <c r="D226" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E226" t="s">
-        <v>362</v>
+        <v>110</v>
       </c>
       <c r="F226" t="s">
-        <v>363</v>
+        <v>111</v>
       </c>
       <c r="G226" t="s">
-        <v>364</v>
+        <v>112</v>
       </c>
       <c r="H226" t="s">
         <v>365</v>
@@ -10207,10 +10240,10 @@
         <v>1</v>
       </c>
       <c r="K226">
-        <v>8591000</v>
+        <v>450000</v>
       </c>
       <c r="L226">
-        <v>8591000</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="227" spans="1:12">
@@ -10224,19 +10257,19 @@
         <v>13</v>
       </c>
       <c r="D227" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E227" t="s">
-        <v>129</v>
+        <v>366</v>
       </c>
       <c r="F227" t="s">
-        <v>130</v>
+        <v>367</v>
       </c>
       <c r="G227" t="s">
-        <v>131</v>
+        <v>368</v>
       </c>
       <c r="H227" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I227" t="s">
         <v>19</v>
@@ -10245,10 +10278,10 @@
         <v>1</v>
       </c>
       <c r="K227">
-        <v>2258000</v>
+        <v>8591000</v>
       </c>
       <c r="L227">
-        <v>2258000</v>
+        <v>8591000</v>
       </c>
     </row>
     <row r="228" spans="1:12">
@@ -10274,7 +10307,7 @@
         <v>131</v>
       </c>
       <c r="H228" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I228" t="s">
         <v>19</v>
@@ -10283,10 +10316,10 @@
         <v>1</v>
       </c>
       <c r="K228">
-        <v>15828200</v>
+        <v>2258000</v>
       </c>
       <c r="L228">
-        <v>15828200</v>
+        <v>2258000</v>
       </c>
     </row>
     <row r="229" spans="1:12">
@@ -10300,19 +10333,19 @@
         <v>13</v>
       </c>
       <c r="D229" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E229" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="F229" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="G229" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="H229" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I229" t="s">
         <v>19</v>
@@ -10321,10 +10354,10 @@
         <v>1</v>
       </c>
       <c r="K229">
-        <v>2102330</v>
+        <v>15828200</v>
       </c>
       <c r="L229">
-        <v>2102330</v>
+        <v>15828200</v>
       </c>
     </row>
     <row r="230" spans="1:12">
@@ -10338,19 +10371,19 @@
         <v>13</v>
       </c>
       <c r="D230" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E230" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="F230" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="G230" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="H230" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="I230" t="s">
         <v>19</v>
@@ -10359,10 +10392,10 @@
         <v>1</v>
       </c>
       <c r="K230">
-        <v>14733600</v>
+        <v>2102330</v>
       </c>
       <c r="L230">
-        <v>14733600</v>
+        <v>2102330</v>
       </c>
     </row>
     <row r="231" spans="1:12">
@@ -10376,19 +10409,19 @@
         <v>13</v>
       </c>
       <c r="D231" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E231" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F231" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G231" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="H231" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="I231" t="s">
         <v>19</v>
@@ -10397,10 +10430,10 @@
         <v>1</v>
       </c>
       <c r="K231">
-        <v>9137000</v>
+        <v>14733600</v>
       </c>
       <c r="L231">
-        <v>9137000</v>
+        <v>14733600</v>
       </c>
     </row>
     <row r="232" spans="1:12">
@@ -10417,13 +10450,13 @@
         <v>24</v>
       </c>
       <c r="E232" t="s">
-        <v>371</v>
+        <v>141</v>
       </c>
       <c r="F232" t="s">
-        <v>372</v>
+        <v>142</v>
       </c>
       <c r="G232" t="s">
-        <v>373</v>
+        <v>143</v>
       </c>
       <c r="H232" t="s">
         <v>374</v>
@@ -10435,10 +10468,10 @@
         <v>1</v>
       </c>
       <c r="K232">
-        <v>16821479</v>
+        <v>9137000</v>
       </c>
       <c r="L232">
-        <v>16821479</v>
+        <v>9137000</v>
       </c>
     </row>
     <row r="233" spans="1:12">
@@ -10452,7 +10485,7 @@
         <v>13</v>
       </c>
       <c r="D233" t="s">
-        <v>176</v>
+        <v>24</v>
       </c>
       <c r="E233" t="s">
         <v>375</v>
@@ -10473,10 +10506,10 @@
         <v>1</v>
       </c>
       <c r="K233">
-        <v>320961489</v>
+        <v>16821479</v>
       </c>
       <c r="L233">
-        <v>320961489</v>
+        <v>16821479</v>
       </c>
     </row>
     <row r="234" spans="1:12">
@@ -10490,7 +10523,7 @@
         <v>13</v>
       </c>
       <c r="D234" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="E234" t="s">
         <v>379</v>
@@ -10502,7 +10535,7 @@
         <v>381</v>
       </c>
       <c r="H234" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="I234" t="s">
         <v>19</v>
@@ -10511,10 +10544,10 @@
         <v>1</v>
       </c>
       <c r="K234">
-        <v>4590000</v>
+        <v>320961489</v>
       </c>
       <c r="L234">
-        <v>4590000</v>
+        <v>320961489</v>
       </c>
     </row>
     <row r="235" spans="1:12">
@@ -10528,20 +10561,20 @@
         <v>13</v>
       </c>
       <c r="D235" t="s">
-        <v>297</v>
+        <v>62</v>
       </c>
       <c r="E235" t="s">
+        <v>383</v>
+      </c>
+      <c r="F235" t="s">
+        <v>384</v>
+      </c>
+      <c r="G235" t="s">
+        <v>385</v>
+      </c>
+      <c r="H235" t="s">
         <v>382</v>
       </c>
-      <c r="F235" t="s">
-        <v>383</v>
-      </c>
-      <c r="G235" t="s">
-        <v>307</v>
-      </c>
-      <c r="H235" t="s">
-        <v>384</v>
-      </c>
       <c r="I235" t="s">
         <v>19</v>
       </c>
@@ -10549,10 +10582,10 @@
         <v>1</v>
       </c>
       <c r="K235">
-        <v>20738160</v>
+        <v>4590000</v>
       </c>
       <c r="L235">
-        <v>20738160</v>
+        <v>4590000</v>
       </c>
     </row>
     <row r="236" spans="1:12">
@@ -10569,13 +10602,13 @@
         <v>297</v>
       </c>
       <c r="E236" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F236" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G236" t="s">
-        <v>387</v>
+        <v>307</v>
       </c>
       <c r="H236" t="s">
         <v>388</v>
@@ -10587,10 +10620,10 @@
         <v>1</v>
       </c>
       <c r="K236">
-        <v>720000</v>
+        <v>20738160</v>
       </c>
       <c r="L236">
-        <v>720000</v>
+        <v>20738160</v>
       </c>
     </row>
     <row r="237" spans="1:12">
@@ -10604,19 +10637,19 @@
         <v>13</v>
       </c>
       <c r="D237" t="s">
-        <v>109</v>
+        <v>297</v>
       </c>
       <c r="E237" t="s">
-        <v>129</v>
+        <v>389</v>
       </c>
       <c r="F237" t="s">
-        <v>130</v>
+        <v>390</v>
       </c>
       <c r="G237" t="s">
-        <v>131</v>
+        <v>391</v>
       </c>
       <c r="H237" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="I237" t="s">
         <v>19</v>
@@ -10625,10 +10658,10 @@
         <v>1</v>
       </c>
       <c r="K237">
-        <v>4515140</v>
+        <v>720000</v>
       </c>
       <c r="L237">
-        <v>4515140</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="238" spans="1:12">
@@ -10642,19 +10675,19 @@
         <v>13</v>
       </c>
       <c r="D238" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E238" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F238" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G238" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="H238" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="I238" t="s">
         <v>19</v>
@@ -10663,10 +10696,10 @@
         <v>1</v>
       </c>
       <c r="K238">
-        <v>2280000</v>
+        <v>4515140</v>
       </c>
       <c r="L238">
-        <v>2280000</v>
+        <v>4515140</v>
       </c>
     </row>
     <row r="239" spans="1:12">
@@ -10692,7 +10725,7 @@
         <v>143</v>
       </c>
       <c r="H239" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="I239" t="s">
         <v>19</v>
@@ -10701,10 +10734,10 @@
         <v>1</v>
       </c>
       <c r="K239">
-        <v>2015000</v>
+        <v>2280000</v>
       </c>
       <c r="L239">
-        <v>2015000</v>
+        <v>2280000</v>
       </c>
     </row>
     <row r="240" spans="1:12">
@@ -10730,7 +10763,7 @@
         <v>143</v>
       </c>
       <c r="H240" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="I240" t="s">
         <v>19</v>
@@ -10739,10 +10772,10 @@
         <v>1</v>
       </c>
       <c r="K240">
-        <v>3265000</v>
+        <v>2015000</v>
       </c>
       <c r="L240">
-        <v>3265000</v>
+        <v>2015000</v>
       </c>
     </row>
     <row r="241" spans="1:12">
@@ -10768,7 +10801,7 @@
         <v>143</v>
       </c>
       <c r="H241" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I241" t="s">
         <v>19</v>
@@ -10777,10 +10810,10 @@
         <v>1</v>
       </c>
       <c r="K241">
-        <v>1440000</v>
+        <v>3265000</v>
       </c>
       <c r="L241">
-        <v>1440000</v>
+        <v>3265000</v>
       </c>
     </row>
     <row r="242" spans="1:12">
@@ -10794,16 +10827,16 @@
         <v>13</v>
       </c>
       <c r="D242" t="s">
-        <v>176</v>
+        <v>24</v>
       </c>
       <c r="E242" t="s">
-        <v>394</v>
+        <v>141</v>
       </c>
       <c r="F242" t="s">
-        <v>395</v>
+        <v>142</v>
       </c>
       <c r="G242" t="s">
-        <v>396</v>
+        <v>143</v>
       </c>
       <c r="H242" t="s">
         <v>397</v>
@@ -10815,10 +10848,10 @@
         <v>1</v>
       </c>
       <c r="K242">
-        <v>5326766</v>
+        <v>1440000</v>
       </c>
       <c r="L242">
-        <v>5326766</v>
+        <v>1440000</v>
       </c>
     </row>
     <row r="243" spans="1:12">
@@ -10832,19 +10865,19 @@
         <v>13</v>
       </c>
       <c r="D243" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="E243" t="s">
-        <v>110</v>
+        <v>398</v>
       </c>
       <c r="F243" t="s">
-        <v>111</v>
+        <v>399</v>
       </c>
       <c r="G243" t="s">
-        <v>112</v>
+        <v>400</v>
       </c>
       <c r="H243" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="I243" t="s">
         <v>19</v>
@@ -10853,10 +10886,10 @@
         <v>1</v>
       </c>
       <c r="K243">
-        <v>2805000</v>
+        <v>5326766</v>
       </c>
       <c r="L243">
-        <v>2805000</v>
+        <v>5326766</v>
       </c>
     </row>
     <row r="244" spans="1:12">
@@ -10882,7 +10915,7 @@
         <v>112</v>
       </c>
       <c r="H244" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="I244" t="s">
         <v>19</v>
@@ -10891,10 +10924,10 @@
         <v>1</v>
       </c>
       <c r="K244">
-        <v>1650000</v>
+        <v>2805000</v>
       </c>
       <c r="L244">
-        <v>1650000</v>
+        <v>2805000</v>
       </c>
     </row>
     <row r="245" spans="1:12">
@@ -10908,19 +10941,19 @@
         <v>13</v>
       </c>
       <c r="D245" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E245" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F245" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G245" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H245" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="I245" t="s">
         <v>19</v>
@@ -10929,10 +10962,10 @@
         <v>1</v>
       </c>
       <c r="K245">
-        <v>780000</v>
+        <v>1650000</v>
       </c>
       <c r="L245">
-        <v>780000</v>
+        <v>1650000</v>
       </c>
     </row>
     <row r="246" spans="1:12">
@@ -10958,7 +10991,7 @@
         <v>107</v>
       </c>
       <c r="H246" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="I246" t="s">
         <v>19</v>
@@ -10967,10 +11000,10 @@
         <v>1</v>
       </c>
       <c r="K246">
-        <v>900000</v>
+        <v>780000</v>
       </c>
       <c r="L246">
-        <v>900000</v>
+        <v>780000</v>
       </c>
     </row>
     <row r="247" spans="1:12">
@@ -10996,7 +11029,7 @@
         <v>107</v>
       </c>
       <c r="H247" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="I247" t="s">
         <v>19</v>
@@ -11005,10 +11038,10 @@
         <v>1</v>
       </c>
       <c r="K247">
-        <v>280000</v>
+        <v>900000</v>
       </c>
       <c r="L247">
-        <v>280000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="248" spans="1:12">
@@ -11022,19 +11055,19 @@
         <v>13</v>
       </c>
       <c r="D248" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E248" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F248" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G248" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H248" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="I248" t="s">
         <v>19</v>
@@ -11043,10 +11076,10 @@
         <v>1</v>
       </c>
       <c r="K248">
-        <v>2080000</v>
+        <v>280000</v>
       </c>
       <c r="L248">
-        <v>2080000</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="249" spans="1:12">
@@ -11072,7 +11105,7 @@
         <v>112</v>
       </c>
       <c r="H249" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="I249" t="s">
         <v>19</v>
@@ -11081,10 +11114,10 @@
         <v>1</v>
       </c>
       <c r="K249">
-        <v>2400000</v>
+        <v>2080000</v>
       </c>
       <c r="L249">
-        <v>2400000</v>
+        <v>2080000</v>
       </c>
     </row>
     <row r="250" spans="1:12">
@@ -11110,7 +11143,7 @@
         <v>112</v>
       </c>
       <c r="H250" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="I250" t="s">
         <v>19</v>
@@ -11119,10 +11152,10 @@
         <v>1</v>
       </c>
       <c r="K250">
-        <v>150000</v>
+        <v>2400000</v>
       </c>
       <c r="L250">
-        <v>150000</v>
+        <v>2400000</v>
       </c>
     </row>
     <row r="251" spans="1:12">
@@ -11148,7 +11181,7 @@
         <v>112</v>
       </c>
       <c r="H251" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="I251" t="s">
         <v>19</v>
@@ -11157,10 +11190,10 @@
         <v>1</v>
       </c>
       <c r="K251">
-        <v>260000</v>
+        <v>150000</v>
       </c>
       <c r="L251">
-        <v>260000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="252" spans="1:12">
@@ -11186,7 +11219,7 @@
         <v>112</v>
       </c>
       <c r="H252" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="I252" t="s">
         <v>19</v>
@@ -11195,10 +11228,10 @@
         <v>1</v>
       </c>
       <c r="K252">
-        <v>450000</v>
+        <v>260000</v>
       </c>
       <c r="L252">
-        <v>450000</v>
+        <v>260000</v>
       </c>
     </row>
     <row r="253" spans="1:12">
@@ -11224,7 +11257,7 @@
         <v>112</v>
       </c>
       <c r="H253" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="I253" t="s">
         <v>19</v>
@@ -11233,10 +11266,10 @@
         <v>1</v>
       </c>
       <c r="K253">
-        <v>2170000</v>
+        <v>450000</v>
       </c>
       <c r="L253">
-        <v>2170000</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="254" spans="1:12">
@@ -11250,16 +11283,16 @@
         <v>13</v>
       </c>
       <c r="D254" t="s">
-        <v>297</v>
+        <v>109</v>
       </c>
       <c r="E254" t="s">
-        <v>409</v>
+        <v>110</v>
       </c>
       <c r="F254" t="s">
-        <v>410</v>
+        <v>111</v>
       </c>
       <c r="G254" t="s">
-        <v>411</v>
+        <v>112</v>
       </c>
       <c r="H254" t="s">
         <v>412</v>
@@ -11271,10 +11304,10 @@
         <v>1</v>
       </c>
       <c r="K254">
-        <v>520000</v>
+        <v>2170000</v>
       </c>
       <c r="L254">
-        <v>520000</v>
+        <v>2170000</v>
       </c>
     </row>
     <row r="255" spans="1:12">
@@ -11288,19 +11321,19 @@
         <v>13</v>
       </c>
       <c r="D255" t="s">
-        <v>109</v>
+        <v>297</v>
       </c>
       <c r="E255" t="s">
-        <v>110</v>
+        <v>413</v>
       </c>
       <c r="F255" t="s">
-        <v>111</v>
+        <v>414</v>
       </c>
       <c r="G255" t="s">
-        <v>112</v>
+        <v>415</v>
       </c>
       <c r="H255" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I255" t="s">
         <v>19</v>
@@ -11309,10 +11342,10 @@
         <v>1</v>
       </c>
       <c r="K255">
-        <v>260000</v>
+        <v>520000</v>
       </c>
       <c r="L255">
-        <v>260000</v>
+        <v>520000</v>
       </c>
     </row>
     <row r="256" spans="1:12">
@@ -11326,19 +11359,19 @@
         <v>13</v>
       </c>
       <c r="D256" t="s">
-        <v>297</v>
+        <v>109</v>
       </c>
       <c r="E256" t="s">
-        <v>409</v>
+        <v>110</v>
       </c>
       <c r="F256" t="s">
-        <v>410</v>
+        <v>111</v>
       </c>
       <c r="G256" t="s">
-        <v>411</v>
+        <v>112</v>
       </c>
       <c r="H256" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="I256" t="s">
         <v>19</v>
@@ -11347,10 +11380,10 @@
         <v>1</v>
       </c>
       <c r="K256">
-        <v>300000</v>
+        <v>260000</v>
       </c>
       <c r="L256">
-        <v>300000</v>
+        <v>260000</v>
       </c>
     </row>
     <row r="257" spans="1:12">
@@ -11364,19 +11397,19 @@
         <v>13</v>
       </c>
       <c r="D257" t="s">
-        <v>109</v>
+        <v>297</v>
       </c>
       <c r="E257" t="s">
-        <v>110</v>
+        <v>413</v>
       </c>
       <c r="F257" t="s">
-        <v>111</v>
+        <v>414</v>
       </c>
       <c r="G257" t="s">
-        <v>112</v>
+        <v>415</v>
       </c>
       <c r="H257" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="I257" t="s">
         <v>19</v>
@@ -11385,10 +11418,10 @@
         <v>1</v>
       </c>
       <c r="K257">
-        <v>150000</v>
+        <v>300000</v>
       </c>
       <c r="L257">
-        <v>150000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="258" spans="1:12">
@@ -11414,7 +11447,7 @@
         <v>112</v>
       </c>
       <c r="H258" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="I258" t="s">
         <v>19</v>
@@ -11423,10 +11456,10 @@
         <v>1</v>
       </c>
       <c r="K258">
-        <v>520000</v>
+        <v>150000</v>
       </c>
       <c r="L258">
-        <v>520000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="259" spans="1:12">
@@ -11452,7 +11485,7 @@
         <v>112</v>
       </c>
       <c r="H259" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="I259" t="s">
         <v>19</v>
@@ -11461,10 +11494,10 @@
         <v>1</v>
       </c>
       <c r="K259">
-        <v>600000</v>
+        <v>520000</v>
       </c>
       <c r="L259">
-        <v>600000</v>
+        <v>520000</v>
       </c>
     </row>
     <row r="260" spans="1:12">
@@ -11490,7 +11523,7 @@
         <v>112</v>
       </c>
       <c r="H260" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="I260" t="s">
         <v>19</v>
@@ -11499,10 +11532,10 @@
         <v>1</v>
       </c>
       <c r="K260">
-        <v>750000</v>
+        <v>600000</v>
       </c>
       <c r="L260">
-        <v>750000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="261" spans="1:12">
@@ -11528,7 +11561,7 @@
         <v>112</v>
       </c>
       <c r="H261" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I261" t="s">
         <v>19</v>
@@ -11537,10 +11570,10 @@
         <v>1</v>
       </c>
       <c r="K261">
-        <v>650000</v>
+        <v>750000</v>
       </c>
       <c r="L261">
-        <v>650000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="262" spans="1:12">
@@ -11566,7 +11599,7 @@
         <v>112</v>
       </c>
       <c r="H262" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="I262" t="s">
         <v>19</v>
@@ -11575,10 +11608,10 @@
         <v>1</v>
       </c>
       <c r="K262">
-        <v>2250000</v>
+        <v>650000</v>
       </c>
       <c r="L262">
-        <v>2250000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="263" spans="1:12">
@@ -11604,7 +11637,7 @@
         <v>112</v>
       </c>
       <c r="H263" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="I263" t="s">
         <v>19</v>
@@ -11613,10 +11646,10 @@
         <v>1</v>
       </c>
       <c r="K263">
-        <v>8275000</v>
+        <v>2250000</v>
       </c>
       <c r="L263">
-        <v>8275000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="264" spans="1:12">
@@ -11642,7 +11675,7 @@
         <v>112</v>
       </c>
       <c r="H264" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="I264" t="s">
         <v>19</v>
@@ -11651,10 +11684,10 @@
         <v>1</v>
       </c>
       <c r="K264">
-        <v>130000</v>
+        <v>8275000</v>
       </c>
       <c r="L264">
-        <v>130000</v>
+        <v>8275000</v>
       </c>
     </row>
     <row r="265" spans="1:12">
@@ -11680,7 +11713,7 @@
         <v>112</v>
       </c>
       <c r="H265" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="I265" t="s">
         <v>19</v>
@@ -11689,10 +11722,10 @@
         <v>1</v>
       </c>
       <c r="K265">
-        <v>150000</v>
+        <v>130000</v>
       </c>
       <c r="L265">
-        <v>150000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="266" spans="1:12">
@@ -11718,7 +11751,7 @@
         <v>112</v>
       </c>
       <c r="H266" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="I266" t="s">
         <v>19</v>
@@ -11727,10 +11760,10 @@
         <v>1</v>
       </c>
       <c r="K266">
-        <v>210000</v>
+        <v>150000</v>
       </c>
       <c r="L266">
-        <v>210000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="267" spans="1:12">
@@ -11756,7 +11789,7 @@
         <v>112</v>
       </c>
       <c r="H267" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="I267" t="s">
         <v>19</v>
@@ -11765,10 +11798,10 @@
         <v>1</v>
       </c>
       <c r="K267">
-        <v>150000</v>
+        <v>210000</v>
       </c>
       <c r="L267">
-        <v>150000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="268" spans="1:12">
@@ -11782,19 +11815,19 @@
         <v>13</v>
       </c>
       <c r="D268" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="E268" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F268" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G268" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H268" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="I268" t="s">
         <v>19</v>
@@ -11803,10 +11836,10 @@
         <v>1</v>
       </c>
       <c r="K268">
-        <v>28260000</v>
+        <v>150000</v>
       </c>
       <c r="L268">
-        <v>28260000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="269" spans="1:12">
@@ -11820,19 +11853,19 @@
         <v>13</v>
       </c>
       <c r="D269" t="s">
-        <v>24</v>
+        <v>327</v>
       </c>
       <c r="E269" t="s">
-        <v>105</v>
+        <v>428</v>
       </c>
       <c r="F269" t="s">
-        <v>106</v>
+        <v>429</v>
       </c>
       <c r="G269" t="s">
-        <v>107</v>
+        <v>430</v>
       </c>
       <c r="H269" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="I269" t="s">
         <v>19</v>
@@ -11841,10 +11874,10 @@
         <v>1</v>
       </c>
       <c r="K269">
-        <v>7950000</v>
+        <v>154700000</v>
       </c>
       <c r="L269">
-        <v>7950000</v>
+        <v>154700000</v>
       </c>
     </row>
     <row r="270" spans="1:12">
@@ -11870,7 +11903,7 @@
         <v>107</v>
       </c>
       <c r="H270" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="I270" t="s">
         <v>19</v>
@@ -11879,10 +11912,10 @@
         <v>1</v>
       </c>
       <c r="K270">
-        <v>420000</v>
+        <v>28260000</v>
       </c>
       <c r="L270">
-        <v>420000</v>
+        <v>28260000</v>
       </c>
     </row>
     <row r="271" spans="1:12">
@@ -11896,19 +11929,19 @@
         <v>13</v>
       </c>
       <c r="D271" t="s">
-        <v>297</v>
+        <v>24</v>
       </c>
       <c r="E271" t="s">
-        <v>427</v>
+        <v>105</v>
       </c>
       <c r="F271" t="s">
-        <v>428</v>
+        <v>106</v>
       </c>
       <c r="G271" t="s">
-        <v>429</v>
+        <v>107</v>
       </c>
       <c r="H271" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="I271" t="s">
         <v>19</v>
@@ -11917,10 +11950,10 @@
         <v>1</v>
       </c>
       <c r="K271">
-        <v>300000</v>
+        <v>7950000</v>
       </c>
       <c r="L271">
-        <v>300000</v>
+        <v>7950000</v>
       </c>
     </row>
     <row r="272" spans="1:12">
@@ -11946,7 +11979,7 @@
         <v>107</v>
       </c>
       <c r="H272" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="I272" t="s">
         <v>19</v>
@@ -11955,10 +11988,10 @@
         <v>1</v>
       </c>
       <c r="K272">
-        <v>300000</v>
+        <v>420000</v>
       </c>
       <c r="L272">
-        <v>300000</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="273" spans="1:12">
@@ -11975,16 +12008,16 @@
         <v>297</v>
       </c>
       <c r="E273" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F273" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G273" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="H273" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="I273" t="s">
         <v>19</v>
@@ -11993,10 +12026,10 @@
         <v>1</v>
       </c>
       <c r="K273">
-        <v>1152800</v>
+        <v>300000</v>
       </c>
       <c r="L273">
-        <v>1152800</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="274" spans="1:12">
@@ -12010,16 +12043,16 @@
         <v>13</v>
       </c>
       <c r="D274" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="E274" t="s">
-        <v>435</v>
+        <v>105</v>
       </c>
       <c r="F274" t="s">
-        <v>436</v>
+        <v>106</v>
       </c>
       <c r="G274" t="s">
-        <v>437</v>
+        <v>107</v>
       </c>
       <c r="H274" t="s">
         <v>438</v>
@@ -12031,10 +12064,10 @@
         <v>1</v>
       </c>
       <c r="K274">
-        <v>510700000</v>
+        <v>300000</v>
       </c>
       <c r="L274">
-        <v>510700000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="275" spans="1:12">
@@ -12048,7 +12081,7 @@
         <v>13</v>
       </c>
       <c r="D275" t="s">
-        <v>119</v>
+        <v>297</v>
       </c>
       <c r="E275" t="s">
         <v>439</v>
@@ -12069,10 +12102,124 @@
         <v>1</v>
       </c>
       <c r="K275">
+        <v>1152800</v>
+      </c>
+      <c r="L275">
+        <v>1152800</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
+      <c r="A276">
+        <v>273</v>
+      </c>
+      <c r="B276">
+        <v>626402</v>
+      </c>
+      <c r="C276" t="s">
+        <v>13</v>
+      </c>
+      <c r="D276" t="s">
+        <v>119</v>
+      </c>
+      <c r="E276" t="s">
+        <v>443</v>
+      </c>
+      <c r="F276" t="s">
+        <v>444</v>
+      </c>
+      <c r="G276" t="s">
+        <v>445</v>
+      </c>
+      <c r="H276" t="s">
+        <v>446</v>
+      </c>
+      <c r="I276" t="s">
+        <v>19</v>
+      </c>
+      <c r="J276">
+        <v>1</v>
+      </c>
+      <c r="K276">
+        <v>510700000</v>
+      </c>
+      <c r="L276">
+        <v>510700000</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
+      <c r="A277">
+        <v>274</v>
+      </c>
+      <c r="B277">
+        <v>626402</v>
+      </c>
+      <c r="C277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D277" t="s">
+        <v>119</v>
+      </c>
+      <c r="E277" t="s">
+        <v>447</v>
+      </c>
+      <c r="F277" t="s">
+        <v>448</v>
+      </c>
+      <c r="G277" t="s">
+        <v>449</v>
+      </c>
+      <c r="H277" t="s">
+        <v>450</v>
+      </c>
+      <c r="I277" t="s">
+        <v>19</v>
+      </c>
+      <c r="J277">
+        <v>1</v>
+      </c>
+      <c r="K277">
         <v>115820000</v>
       </c>
-      <c r="L275">
+      <c r="L277">
         <v>115820000</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
+      <c r="A278">
+        <v>275</v>
+      </c>
+      <c r="B278">
+        <v>626402</v>
+      </c>
+      <c r="C278" t="s">
+        <v>13</v>
+      </c>
+      <c r="D278" t="s">
+        <v>327</v>
+      </c>
+      <c r="E278" t="s">
+        <v>451</v>
+      </c>
+      <c r="F278" t="s">
+        <v>452</v>
+      </c>
+      <c r="G278" t="s">
+        <v>453</v>
+      </c>
+      <c r="H278" t="s">
+        <v>450</v>
+      </c>
+      <c r="I278" t="s">
+        <v>19</v>
+      </c>
+      <c r="J278">
+        <v>1</v>
+      </c>
+      <c r="K278">
+        <v>148500000</v>
+      </c>
+      <c r="L278">
+        <v>148500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Realisasi sd 5 Juni 2023
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2245">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -6512,6 +6512,30 @@
     <t>'626402.175.522151.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.301.0F.000985</t>
   </si>
   <si>
+    <t>2023-06-06</t>
+  </si>
+  <si>
+    <t>'00476T</t>
+  </si>
+  <si>
+    <t>'231751303012549</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang. Uang lembur PPNPN bulan Januari 2023 untuk 3 pegawai berdasarkan SPKL No B.288/BRSDM.4/KP.440/I/2023 tgl 31/1/2023 dan B.114/BRSDM.4/KP.440/I/2023 tgl 05/1/2023</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.GA.001382</t>
+  </si>
+  <si>
+    <t>'00477T</t>
+  </si>
+  <si>
+    <t>'231751303012578</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang. Uang lembur PPNPN bulan Februari 2023 untuk 3 pegawai berdasarkan SPKL No B.497/BRSDM.4/KP.440/II/2023 tgl 21/2/2023</t>
+  </si>
+  <si>
     <t>'00479T</t>
   </si>
   <si>
@@ -6593,6 +6617,24 @@
     <t>'626402.175.524119.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0B.000129</t>
   </si>
   <si>
+    <t>'00485T</t>
+  </si>
+  <si>
+    <t>'231751303012579</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang. Uang lembur PPNPN bulan Maret 2023 untuk 1 pegawai berdasarkan SPKL No B.667/BRSDM.4/KP.440/III/2023 tgl 16/3/2023</t>
+  </si>
+  <si>
+    <t>'00486T</t>
+  </si>
+  <si>
+    <t>'231751303012576</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perjadin Menghadiri Rakornis Pusat Pendidikan sesuai ST No:B.976/BRSDM.4/KP.440/V/2023 Tgl 08-05-2023 an. Wishnu C. Pratama, dkk</t>
+  </si>
+  <si>
     <t>2023-06-05</t>
   </si>
   <si>
@@ -6660,6 +6702,54 @@
   </si>
   <si>
     <t>Pembayaran belanja pegawai Pusdik uang lembur dan uang makan lembur bulan Maret 2023 untuk 8 pegawai sesuai SPKL no :B.668, 685/BRSDM.4/KP.440/III/2023 tanggal 16 dan 20 Maret 2023</t>
+  </si>
+  <si>
+    <t>'00499T</t>
+  </si>
+  <si>
+    <t>'231751303012546</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya penelitian peserta lanjutan tubel Prog S2 IPB sesuai dengan SK KPA Ses BRSDM KP Nomor 757/KPA/BRSDM/VIII/2021 Tgl 13-8-2021 an. Nurul Tri Jayanti</t>
+  </si>
+  <si>
+    <t>'00500T</t>
+  </si>
+  <si>
+    <t>'231751303012545</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya jurnal peserta lanjutan tubel Prog S3 UB, sesuai SK Ka BRSDM KP Nomor: 107/KEPBRSDM/2020 Tanggal 18 Agustus 2020 an. Afandi Saputra</t>
+  </si>
+  <si>
+    <t>'00501T</t>
+  </si>
+  <si>
+    <t>'231751303012577</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Keputusan Nomor:KEP.88/PPK/BRSDM.1/I/2023 Tgl.5 Januari 2023 (Honorarium Tim Pengelola Informasi dan Dokumentasi BRSDM Bulan Januari s/d April 2023)</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000264</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000265</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000266</t>
+  </si>
+  <si>
+    <t>'00503T</t>
+  </si>
+  <si>
+    <t>'231751701003236</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0B.000305</t>
+  </si>
+  <si>
+    <t>'626402.175.522151.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.960.101.0B.000761</t>
   </si>
 </sst>
 </file>
@@ -7001,7 +7091,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2093"/>
+  <dimension ref="A1:L2106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -83294,19 +83384,19 @@
         <v>13</v>
       </c>
       <c r="D2010" t="s">
-        <v>2156</v>
+        <v>2165</v>
       </c>
       <c r="E2010" t="s">
-        <v>2165</v>
+        <v>2166</v>
       </c>
       <c r="F2010" t="s">
-        <v>2166</v>
+        <v>2167</v>
       </c>
       <c r="G2010" t="s">
-        <v>1210</v>
+        <v>2168</v>
       </c>
       <c r="H2010" t="s">
-        <v>170</v>
+        <v>2169</v>
       </c>
       <c r="I2010" t="s">
         <v>19</v>
@@ -83315,10 +83405,10 @@
         <v>1</v>
       </c>
       <c r="K2010">
-        <v>27993000</v>
+        <v>237000</v>
       </c>
       <c r="L2010">
-        <v>27993000</v>
+        <v>237000</v>
       </c>
     </row>
     <row r="2011" spans="1:12">
@@ -83332,19 +83422,19 @@
         <v>13</v>
       </c>
       <c r="D2011" t="s">
-        <v>2156</v>
+        <v>2165</v>
       </c>
       <c r="E2011" t="s">
-        <v>2165</v>
+        <v>2170</v>
       </c>
       <c r="F2011" t="s">
-        <v>2166</v>
+        <v>2171</v>
       </c>
       <c r="G2011" t="s">
-        <v>1210</v>
+        <v>2172</v>
       </c>
       <c r="H2011" t="s">
-        <v>374</v>
+        <v>2169</v>
       </c>
       <c r="I2011" t="s">
         <v>19</v>
@@ -83353,10 +83443,10 @@
         <v>1</v>
       </c>
       <c r="K2011">
-        <v>20000000</v>
+        <v>207000</v>
       </c>
       <c r="L2011">
-        <v>20000000</v>
+        <v>207000</v>
       </c>
     </row>
     <row r="2012" spans="1:12">
@@ -83373,16 +83463,16 @@
         <v>2156</v>
       </c>
       <c r="E2012" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2012" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2012" t="s">
         <v>1210</v>
       </c>
       <c r="H2012" t="s">
-        <v>796</v>
+        <v>170</v>
       </c>
       <c r="I2012" t="s">
         <v>19</v>
@@ -83391,10 +83481,10 @@
         <v>1</v>
       </c>
       <c r="K2012">
-        <v>2798000</v>
+        <v>27993000</v>
       </c>
       <c r="L2012">
-        <v>2798000</v>
+        <v>27993000</v>
       </c>
     </row>
     <row r="2013" spans="1:12">
@@ -83411,16 +83501,16 @@
         <v>2156</v>
       </c>
       <c r="E2013" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2013" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2013" t="s">
         <v>1210</v>
       </c>
       <c r="H2013" t="s">
-        <v>173</v>
+        <v>374</v>
       </c>
       <c r="I2013" t="s">
         <v>19</v>
@@ -83429,10 +83519,10 @@
         <v>1</v>
       </c>
       <c r="K2013">
-        <v>121284</v>
+        <v>20000000</v>
       </c>
       <c r="L2013">
-        <v>121284</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="2014" spans="1:12">
@@ -83449,16 +83539,16 @@
         <v>2156</v>
       </c>
       <c r="E2014" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2014" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2014" t="s">
         <v>1210</v>
       </c>
       <c r="H2014" t="s">
-        <v>755</v>
+        <v>796</v>
       </c>
       <c r="I2014" t="s">
         <v>19</v>
@@ -83467,10 +83557,10 @@
         <v>1</v>
       </c>
       <c r="K2014">
-        <v>2327770</v>
+        <v>2798000</v>
       </c>
       <c r="L2014">
-        <v>2327770</v>
+        <v>2798000</v>
       </c>
     </row>
     <row r="2015" spans="1:12">
@@ -83487,16 +83577,16 @@
         <v>2156</v>
       </c>
       <c r="E2015" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2015" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2015" t="s">
         <v>1210</v>
       </c>
       <c r="H2015" t="s">
-        <v>895</v>
+        <v>173</v>
       </c>
       <c r="I2015" t="s">
         <v>19</v>
@@ -83505,10 +83595,10 @@
         <v>1</v>
       </c>
       <c r="K2015">
-        <v>3005000</v>
+        <v>121284</v>
       </c>
       <c r="L2015">
-        <v>3005000</v>
+        <v>121284</v>
       </c>
     </row>
     <row r="2016" spans="1:12">
@@ -83525,16 +83615,16 @@
         <v>2156</v>
       </c>
       <c r="E2016" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2016" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2016" t="s">
         <v>1210</v>
       </c>
       <c r="H2016" t="s">
-        <v>897</v>
+        <v>755</v>
       </c>
       <c r="I2016" t="s">
         <v>19</v>
@@ -83543,10 +83633,10 @@
         <v>1</v>
       </c>
       <c r="K2016">
-        <v>3012000</v>
+        <v>2327770</v>
       </c>
       <c r="L2016">
-        <v>3012000</v>
+        <v>2327770</v>
       </c>
     </row>
     <row r="2017" spans="1:12">
@@ -83563,16 +83653,16 @@
         <v>2156</v>
       </c>
       <c r="E2017" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2017" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2017" t="s">
         <v>1210</v>
       </c>
       <c r="H2017" t="s">
-        <v>814</v>
+        <v>895</v>
       </c>
       <c r="I2017" t="s">
         <v>19</v>
@@ -83581,10 +83671,10 @@
         <v>1</v>
       </c>
       <c r="K2017">
-        <v>3000000</v>
+        <v>3005000</v>
       </c>
       <c r="L2017">
-        <v>3000000</v>
+        <v>3005000</v>
       </c>
     </row>
     <row r="2018" spans="1:12">
@@ -83601,16 +83691,16 @@
         <v>2156</v>
       </c>
       <c r="E2018" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2018" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2018" t="s">
         <v>1210</v>
       </c>
       <c r="H2018" t="s">
-        <v>815</v>
+        <v>897</v>
       </c>
       <c r="I2018" t="s">
         <v>19</v>
@@ -83619,10 +83709,10 @@
         <v>1</v>
       </c>
       <c r="K2018">
-        <v>9000000</v>
+        <v>3012000</v>
       </c>
       <c r="L2018">
-        <v>9000000</v>
+        <v>3012000</v>
       </c>
     </row>
     <row r="2019" spans="1:12">
@@ -83639,16 +83729,16 @@
         <v>2156</v>
       </c>
       <c r="E2019" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2019" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2019" t="s">
         <v>1210</v>
       </c>
       <c r="H2019" t="s">
-        <v>582</v>
+        <v>814</v>
       </c>
       <c r="I2019" t="s">
         <v>19</v>
@@ -83657,10 +83747,10 @@
         <v>1</v>
       </c>
       <c r="K2019">
-        <v>1639760</v>
+        <v>3000000</v>
       </c>
       <c r="L2019">
-        <v>1639760</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="2020" spans="1:12">
@@ -83677,16 +83767,16 @@
         <v>2156</v>
       </c>
       <c r="E2020" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2020" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2020" t="s">
         <v>1210</v>
       </c>
       <c r="H2020" t="s">
-        <v>2155</v>
+        <v>815</v>
       </c>
       <c r="I2020" t="s">
         <v>19</v>
@@ -83695,10 +83785,10 @@
         <v>1</v>
       </c>
       <c r="K2020">
-        <v>150000</v>
+        <v>9000000</v>
       </c>
       <c r="L2020">
-        <v>150000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="2021" spans="1:12">
@@ -83715,16 +83805,16 @@
         <v>2156</v>
       </c>
       <c r="E2021" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2021" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2021" t="s">
         <v>1210</v>
       </c>
       <c r="H2021" t="s">
-        <v>774</v>
+        <v>582</v>
       </c>
       <c r="I2021" t="s">
         <v>19</v>
@@ -83733,10 +83823,10 @@
         <v>1</v>
       </c>
       <c r="K2021">
-        <v>520000</v>
+        <v>1639760</v>
       </c>
       <c r="L2021">
-        <v>520000</v>
+        <v>1639760</v>
       </c>
     </row>
     <row r="2022" spans="1:12">
@@ -83753,16 +83843,16 @@
         <v>2156</v>
       </c>
       <c r="E2022" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2022" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2022" t="s">
         <v>1210</v>
       </c>
       <c r="H2022" t="s">
-        <v>775</v>
+        <v>2155</v>
       </c>
       <c r="I2022" t="s">
         <v>19</v>
@@ -83771,10 +83861,10 @@
         <v>1</v>
       </c>
       <c r="K2022">
-        <v>600000</v>
+        <v>150000</v>
       </c>
       <c r="L2022">
-        <v>600000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="2023" spans="1:12">
@@ -83791,16 +83881,16 @@
         <v>2156</v>
       </c>
       <c r="E2023" t="s">
-        <v>2165</v>
+        <v>2173</v>
       </c>
       <c r="F2023" t="s">
-        <v>2166</v>
+        <v>2174</v>
       </c>
       <c r="G2023" t="s">
         <v>1210</v>
       </c>
       <c r="H2023" t="s">
-        <v>2167</v>
+        <v>774</v>
       </c>
       <c r="I2023" t="s">
         <v>19</v>
@@ -83809,10 +83899,10 @@
         <v>1</v>
       </c>
       <c r="K2023">
-        <v>25550000</v>
+        <v>520000</v>
       </c>
       <c r="L2023">
-        <v>25550000</v>
+        <v>520000</v>
       </c>
     </row>
     <row r="2024" spans="1:12">
@@ -83826,19 +83916,19 @@
         <v>13</v>
       </c>
       <c r="D2024" t="s">
-        <v>2168</v>
+        <v>2156</v>
       </c>
       <c r="E2024" t="s">
-        <v>2169</v>
+        <v>2173</v>
       </c>
       <c r="F2024" t="s">
-        <v>2170</v>
+        <v>2174</v>
       </c>
       <c r="G2024" t="s">
-        <v>2171</v>
+        <v>1210</v>
       </c>
       <c r="H2024" t="s">
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="I2024" t="s">
         <v>19</v>
@@ -83847,10 +83937,10 @@
         <v>1</v>
       </c>
       <c r="K2024">
-        <v>3333610</v>
+        <v>600000</v>
       </c>
       <c r="L2024">
-        <v>3333610</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="2025" spans="1:12">
@@ -83864,19 +83954,19 @@
         <v>13</v>
       </c>
       <c r="D2025" t="s">
-        <v>2168</v>
+        <v>2156</v>
       </c>
       <c r="E2025" t="s">
-        <v>2172</v>
+        <v>2173</v>
       </c>
       <c r="F2025" t="s">
-        <v>2173</v>
+        <v>2174</v>
       </c>
       <c r="G2025" t="s">
-        <v>2174</v>
+        <v>1210</v>
       </c>
       <c r="H2025" t="s">
-        <v>261</v>
+        <v>2175</v>
       </c>
       <c r="I2025" t="s">
         <v>19</v>
@@ -83885,10 +83975,10 @@
         <v>1</v>
       </c>
       <c r="K2025">
-        <v>5639500</v>
+        <v>25550000</v>
       </c>
       <c r="L2025">
-        <v>5639500</v>
+        <v>25550000</v>
       </c>
     </row>
     <row r="2026" spans="1:12">
@@ -83902,19 +83992,19 @@
         <v>13</v>
       </c>
       <c r="D2026" t="s">
-        <v>2156</v>
+        <v>2176</v>
       </c>
       <c r="E2026" t="s">
-        <v>2175</v>
+        <v>2177</v>
       </c>
       <c r="F2026" t="s">
-        <v>2176</v>
+        <v>2178</v>
       </c>
       <c r="G2026" t="s">
-        <v>2177</v>
+        <v>2179</v>
       </c>
       <c r="H2026" t="s">
-        <v>261</v>
+        <v>763</v>
       </c>
       <c r="I2026" t="s">
         <v>19</v>
@@ -83923,10 +84013,10 @@
         <v>1</v>
       </c>
       <c r="K2026">
-        <v>4241379</v>
+        <v>3333610</v>
       </c>
       <c r="L2026">
-        <v>4241379</v>
+        <v>3333610</v>
       </c>
     </row>
     <row r="2027" spans="1:12">
@@ -83940,19 +84030,19 @@
         <v>13</v>
       </c>
       <c r="D2027" t="s">
-        <v>2138</v>
+        <v>2176</v>
       </c>
       <c r="E2027" t="s">
-        <v>2178</v>
+        <v>2180</v>
       </c>
       <c r="F2027" t="s">
-        <v>2179</v>
+        <v>2181</v>
       </c>
       <c r="G2027" t="s">
-        <v>2180</v>
+        <v>2182</v>
       </c>
       <c r="H2027" t="s">
-        <v>342</v>
+        <v>261</v>
       </c>
       <c r="I2027" t="s">
         <v>19</v>
@@ -83961,10 +84051,10 @@
         <v>1</v>
       </c>
       <c r="K2027">
-        <v>6271000</v>
+        <v>5639500</v>
       </c>
       <c r="L2027">
-        <v>6271000</v>
+        <v>5639500</v>
       </c>
     </row>
     <row r="2028" spans="1:12">
@@ -83978,19 +84068,19 @@
         <v>13</v>
       </c>
       <c r="D2028" t="s">
-        <v>2168</v>
+        <v>2156</v>
       </c>
       <c r="E2028" t="s">
-        <v>2181</v>
+        <v>2183</v>
       </c>
       <c r="F2028" t="s">
-        <v>2182</v>
+        <v>2184</v>
       </c>
       <c r="G2028" t="s">
-        <v>2183</v>
+        <v>2185</v>
       </c>
       <c r="H2028" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="I2028" t="s">
         <v>19</v>
@@ -83999,10 +84089,10 @@
         <v>1</v>
       </c>
       <c r="K2028">
-        <v>1142000</v>
+        <v>4241379</v>
       </c>
       <c r="L2028">
-        <v>1142000</v>
+        <v>4241379</v>
       </c>
     </row>
     <row r="2029" spans="1:12">
@@ -84016,19 +84106,19 @@
         <v>13</v>
       </c>
       <c r="D2029" t="s">
-        <v>2168</v>
+        <v>2138</v>
       </c>
       <c r="E2029" t="s">
-        <v>2181</v>
+        <v>2186</v>
       </c>
       <c r="F2029" t="s">
-        <v>2182</v>
+        <v>2187</v>
       </c>
       <c r="G2029" t="s">
-        <v>2183</v>
+        <v>2188</v>
       </c>
       <c r="H2029" t="s">
-        <v>1408</v>
+        <v>342</v>
       </c>
       <c r="I2029" t="s">
         <v>19</v>
@@ -84037,10 +84127,10 @@
         <v>1</v>
       </c>
       <c r="K2029">
-        <v>1930820</v>
+        <v>6271000</v>
       </c>
       <c r="L2029">
-        <v>1930820</v>
+        <v>6271000</v>
       </c>
     </row>
     <row r="2030" spans="1:12">
@@ -84054,19 +84144,19 @@
         <v>13</v>
       </c>
       <c r="D2030" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2030" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2030" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2030" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2030" t="s">
-        <v>1509</v>
+        <v>312</v>
       </c>
       <c r="I2030" t="s">
         <v>19</v>
@@ -84075,10 +84165,10 @@
         <v>1</v>
       </c>
       <c r="K2030">
-        <v>3352000</v>
+        <v>1142000</v>
       </c>
       <c r="L2030">
-        <v>3352000</v>
+        <v>1142000</v>
       </c>
     </row>
     <row r="2031" spans="1:12">
@@ -84092,19 +84182,19 @@
         <v>13</v>
       </c>
       <c r="D2031" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2031" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2031" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2031" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2031" t="s">
-        <v>597</v>
+        <v>1408</v>
       </c>
       <c r="I2031" t="s">
         <v>19</v>
@@ -84113,10 +84203,10 @@
         <v>1</v>
       </c>
       <c r="K2031">
-        <v>1253000</v>
+        <v>1930820</v>
       </c>
       <c r="L2031">
-        <v>1253000</v>
+        <v>1930820</v>
       </c>
     </row>
     <row r="2032" spans="1:12">
@@ -84130,19 +84220,19 @@
         <v>13</v>
       </c>
       <c r="D2032" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2032" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2032" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2032" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2032" t="s">
-        <v>2184</v>
+        <v>1509</v>
       </c>
       <c r="I2032" t="s">
         <v>19</v>
@@ -84151,10 +84241,10 @@
         <v>1</v>
       </c>
       <c r="K2032">
-        <v>3000000</v>
+        <v>3352000</v>
       </c>
       <c r="L2032">
-        <v>3000000</v>
+        <v>3352000</v>
       </c>
     </row>
     <row r="2033" spans="1:12">
@@ -84168,19 +84258,19 @@
         <v>13</v>
       </c>
       <c r="D2033" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2033" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2033" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2033" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2033" t="s">
-        <v>1510</v>
+        <v>597</v>
       </c>
       <c r="I2033" t="s">
         <v>19</v>
@@ -84189,10 +84279,10 @@
         <v>1</v>
       </c>
       <c r="K2033">
-        <v>3368400</v>
+        <v>1253000</v>
       </c>
       <c r="L2033">
-        <v>3368400</v>
+        <v>1253000</v>
       </c>
     </row>
     <row r="2034" spans="1:12">
@@ -84206,19 +84296,19 @@
         <v>13</v>
       </c>
       <c r="D2034" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2034" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2034" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2034" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2034" t="s">
-        <v>321</v>
+        <v>2192</v>
       </c>
       <c r="I2034" t="s">
         <v>19</v>
@@ -84227,10 +84317,10 @@
         <v>1</v>
       </c>
       <c r="K2034">
-        <v>1125000</v>
+        <v>3000000</v>
       </c>
       <c r="L2034">
-        <v>1125000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="2035" spans="1:12">
@@ -84244,19 +84334,19 @@
         <v>13</v>
       </c>
       <c r="D2035" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2035" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2035" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2035" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2035" t="s">
-        <v>328</v>
+        <v>1510</v>
       </c>
       <c r="I2035" t="s">
         <v>19</v>
@@ -84265,10 +84355,10 @@
         <v>1</v>
       </c>
       <c r="K2035">
-        <v>1000000</v>
+        <v>3368400</v>
       </c>
       <c r="L2035">
-        <v>1000000</v>
+        <v>3368400</v>
       </c>
     </row>
     <row r="2036" spans="1:12">
@@ -84282,19 +84372,19 @@
         <v>13</v>
       </c>
       <c r="D2036" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2036" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2036" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2036" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2036" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="I2036" t="s">
         <v>19</v>
@@ -84303,10 +84393,10 @@
         <v>1</v>
       </c>
       <c r="K2036">
-        <v>1000000</v>
+        <v>1125000</v>
       </c>
       <c r="L2036">
-        <v>1000000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="2037" spans="1:12">
@@ -84320,19 +84410,19 @@
         <v>13</v>
       </c>
       <c r="D2037" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2037" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2037" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2037" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2037" t="s">
-        <v>1921</v>
+        <v>328</v>
       </c>
       <c r="I2037" t="s">
         <v>19</v>
@@ -84341,10 +84431,10 @@
         <v>1</v>
       </c>
       <c r="K2037">
-        <v>2190000</v>
+        <v>1000000</v>
       </c>
       <c r="L2037">
-        <v>2190000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="2038" spans="1:12">
@@ -84358,19 +84448,19 @@
         <v>13</v>
       </c>
       <c r="D2038" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2038" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2038" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2038" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2038" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I2038" t="s">
         <v>19</v>
@@ -84396,19 +84486,19 @@
         <v>13</v>
       </c>
       <c r="D2039" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2039" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2039" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2039" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2039" t="s">
-        <v>331</v>
+        <v>1921</v>
       </c>
       <c r="I2039" t="s">
         <v>19</v>
@@ -84417,10 +84507,10 @@
         <v>1</v>
       </c>
       <c r="K2039">
-        <v>1000000</v>
+        <v>2190000</v>
       </c>
       <c r="L2039">
-        <v>1000000</v>
+        <v>2190000</v>
       </c>
     </row>
     <row r="2040" spans="1:12">
@@ -84434,19 +84524,19 @@
         <v>13</v>
       </c>
       <c r="D2040" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2040" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2040" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2040" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2040" t="s">
-        <v>2185</v>
+        <v>330</v>
       </c>
       <c r="I2040" t="s">
         <v>19</v>
@@ -84455,10 +84545,10 @@
         <v>1</v>
       </c>
       <c r="K2040">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="L2040">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="2041" spans="1:12">
@@ -84472,19 +84562,19 @@
         <v>13</v>
       </c>
       <c r="D2041" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2041" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2041" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2041" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2041" t="s">
-        <v>1002</v>
+        <v>331</v>
       </c>
       <c r="I2041" t="s">
         <v>19</v>
@@ -84493,10 +84583,10 @@
         <v>1</v>
       </c>
       <c r="K2041">
-        <v>20000000</v>
+        <v>1000000</v>
       </c>
       <c r="L2041">
-        <v>20000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="2042" spans="1:12">
@@ -84510,19 +84600,19 @@
         <v>13</v>
       </c>
       <c r="D2042" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2042" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2042" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2042" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2042" t="s">
-        <v>332</v>
+        <v>2193</v>
       </c>
       <c r="I2042" t="s">
         <v>19</v>
@@ -84531,10 +84621,10 @@
         <v>1</v>
       </c>
       <c r="K2042">
-        <v>3000000</v>
+        <v>2000000</v>
       </c>
       <c r="L2042">
-        <v>3000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="2043" spans="1:12">
@@ -84548,19 +84638,19 @@
         <v>13</v>
       </c>
       <c r="D2043" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2043" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2043" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2043" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2043" t="s">
-        <v>334</v>
+        <v>1002</v>
       </c>
       <c r="I2043" t="s">
         <v>19</v>
@@ -84569,10 +84659,10 @@
         <v>1</v>
       </c>
       <c r="K2043">
-        <v>1745438</v>
+        <v>20000000</v>
       </c>
       <c r="L2043">
-        <v>1745438</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="2044" spans="1:12">
@@ -84586,19 +84676,19 @@
         <v>13</v>
       </c>
       <c r="D2044" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2044" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2044" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2044" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2044" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I2044" t="s">
         <v>19</v>
@@ -84607,10 +84697,10 @@
         <v>1</v>
       </c>
       <c r="K2044">
-        <v>3649462</v>
+        <v>3000000</v>
       </c>
       <c r="L2044">
-        <v>3649462</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="2045" spans="1:12">
@@ -84624,19 +84714,19 @@
         <v>13</v>
       </c>
       <c r="D2045" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2045" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2045" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2045" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2045" t="s">
-        <v>2186</v>
+        <v>334</v>
       </c>
       <c r="I2045" t="s">
         <v>19</v>
@@ -84645,10 +84735,10 @@
         <v>1</v>
       </c>
       <c r="K2045">
-        <v>300000</v>
+        <v>1745438</v>
       </c>
       <c r="L2045">
-        <v>300000</v>
+        <v>1745438</v>
       </c>
     </row>
     <row r="2046" spans="1:12">
@@ -84662,19 +84752,19 @@
         <v>13</v>
       </c>
       <c r="D2046" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2046" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2046" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2046" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2046" t="s">
-        <v>601</v>
+        <v>335</v>
       </c>
       <c r="I2046" t="s">
         <v>19</v>
@@ -84683,10 +84773,10 @@
         <v>1</v>
       </c>
       <c r="K2046">
-        <v>2830000</v>
+        <v>3649462</v>
       </c>
       <c r="L2046">
-        <v>2830000</v>
+        <v>3649462</v>
       </c>
     </row>
     <row r="2047" spans="1:12">
@@ -84700,19 +84790,19 @@
         <v>13</v>
       </c>
       <c r="D2047" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2047" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2047" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2047" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2047" t="s">
-        <v>2187</v>
+        <v>2194</v>
       </c>
       <c r="I2047" t="s">
         <v>19</v>
@@ -84721,10 +84811,10 @@
         <v>1</v>
       </c>
       <c r="K2047">
-        <v>2341299</v>
+        <v>300000</v>
       </c>
       <c r="L2047">
-        <v>2341299</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="2048" spans="1:12">
@@ -84738,19 +84828,19 @@
         <v>13</v>
       </c>
       <c r="D2048" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2048" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2048" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2048" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2048" t="s">
-        <v>341</v>
+        <v>601</v>
       </c>
       <c r="I2048" t="s">
         <v>19</v>
@@ -84759,10 +84849,10 @@
         <v>1</v>
       </c>
       <c r="K2048">
-        <v>10773800</v>
+        <v>2830000</v>
       </c>
       <c r="L2048">
-        <v>10773800</v>
+        <v>2830000</v>
       </c>
     </row>
     <row r="2049" spans="1:12">
@@ -84776,19 +84866,19 @@
         <v>13</v>
       </c>
       <c r="D2049" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2049" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2049" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2049" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2049" t="s">
-        <v>136</v>
+        <v>2195</v>
       </c>
       <c r="I2049" t="s">
         <v>19</v>
@@ -84797,10 +84887,10 @@
         <v>1</v>
       </c>
       <c r="K2049">
-        <v>1350000</v>
+        <v>2341299</v>
       </c>
       <c r="L2049">
-        <v>1350000</v>
+        <v>2341299</v>
       </c>
     </row>
     <row r="2050" spans="1:12">
@@ -84814,19 +84904,19 @@
         <v>13</v>
       </c>
       <c r="D2050" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2050" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2050" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2050" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2050" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I2050" t="s">
         <v>19</v>
@@ -84835,10 +84925,10 @@
         <v>1</v>
       </c>
       <c r="K2050">
-        <v>150000</v>
+        <v>10773800</v>
       </c>
       <c r="L2050">
-        <v>150000</v>
+        <v>10773800</v>
       </c>
     </row>
     <row r="2051" spans="1:12">
@@ -84852,19 +84942,19 @@
         <v>13</v>
       </c>
       <c r="D2051" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2051" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2051" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2051" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2051" t="s">
-        <v>603</v>
+        <v>136</v>
       </c>
       <c r="I2051" t="s">
         <v>19</v>
@@ -84873,10 +84963,10 @@
         <v>1</v>
       </c>
       <c r="K2051">
-        <v>3897000</v>
+        <v>1350000</v>
       </c>
       <c r="L2051">
-        <v>3897000</v>
+        <v>1350000</v>
       </c>
     </row>
     <row r="2052" spans="1:12">
@@ -84890,19 +84980,19 @@
         <v>13</v>
       </c>
       <c r="D2052" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2052" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2052" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2052" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2052" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I2052" t="s">
         <v>19</v>
@@ -84911,10 +85001,10 @@
         <v>1</v>
       </c>
       <c r="K2052">
-        <v>11450900</v>
+        <v>150000</v>
       </c>
       <c r="L2052">
-        <v>11450900</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="2053" spans="1:12">
@@ -84928,19 +85018,19 @@
         <v>13</v>
       </c>
       <c r="D2053" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2053" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2053" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2053" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2053" t="s">
-        <v>2188</v>
+        <v>603</v>
       </c>
       <c r="I2053" t="s">
         <v>19</v>
@@ -84949,10 +85039,10 @@
         <v>1</v>
       </c>
       <c r="K2053">
-        <v>3640000</v>
+        <v>3897000</v>
       </c>
       <c r="L2053">
-        <v>3640000</v>
+        <v>3897000</v>
       </c>
     </row>
     <row r="2054" spans="1:12">
@@ -84966,19 +85056,19 @@
         <v>13</v>
       </c>
       <c r="D2054" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2054" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2054" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2054" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2054" t="s">
-        <v>1237</v>
+        <v>345</v>
       </c>
       <c r="I2054" t="s">
         <v>19</v>
@@ -84987,10 +85077,10 @@
         <v>1</v>
       </c>
       <c r="K2054">
-        <v>6021260</v>
+        <v>11450900</v>
       </c>
       <c r="L2054">
-        <v>6021260</v>
+        <v>11450900</v>
       </c>
     </row>
     <row r="2055" spans="1:12">
@@ -85004,19 +85094,19 @@
         <v>13</v>
       </c>
       <c r="D2055" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2055" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2055" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2055" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2055" t="s">
-        <v>2189</v>
+        <v>2196</v>
       </c>
       <c r="I2055" t="s">
         <v>19</v>
@@ -85025,10 +85115,10 @@
         <v>1</v>
       </c>
       <c r="K2055">
-        <v>300000</v>
+        <v>3640000</v>
       </c>
       <c r="L2055">
-        <v>300000</v>
+        <v>3640000</v>
       </c>
     </row>
     <row r="2056" spans="1:12">
@@ -85042,19 +85132,19 @@
         <v>13</v>
       </c>
       <c r="D2056" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2056" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2056" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2056" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2056" t="s">
-        <v>1423</v>
+        <v>1237</v>
       </c>
       <c r="I2056" t="s">
         <v>19</v>
@@ -85063,10 +85153,10 @@
         <v>1</v>
       </c>
       <c r="K2056">
-        <v>450000</v>
+        <v>6021260</v>
       </c>
       <c r="L2056">
-        <v>450000</v>
+        <v>6021260</v>
       </c>
     </row>
     <row r="2057" spans="1:12">
@@ -85080,19 +85170,19 @@
         <v>13</v>
       </c>
       <c r="D2057" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2057" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2057" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2057" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2057" t="s">
-        <v>606</v>
+        <v>2197</v>
       </c>
       <c r="I2057" t="s">
         <v>19</v>
@@ -85101,10 +85191,10 @@
         <v>1</v>
       </c>
       <c r="K2057">
-        <v>750000</v>
+        <v>300000</v>
       </c>
       <c r="L2057">
-        <v>750000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="2058" spans="1:12">
@@ -85118,19 +85208,19 @@
         <v>13</v>
       </c>
       <c r="D2058" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2058" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2058" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2058" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2058" t="s">
-        <v>2190</v>
+        <v>1423</v>
       </c>
       <c r="I2058" t="s">
         <v>19</v>
@@ -85139,10 +85229,10 @@
         <v>1</v>
       </c>
       <c r="K2058">
-        <v>1350000</v>
+        <v>450000</v>
       </c>
       <c r="L2058">
-        <v>1350000</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="2059" spans="1:12">
@@ -85156,19 +85246,19 @@
         <v>13</v>
       </c>
       <c r="D2059" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="E2059" t="s">
-        <v>2181</v>
+        <v>2189</v>
       </c>
       <c r="F2059" t="s">
-        <v>2182</v>
+        <v>2190</v>
       </c>
       <c r="G2059" t="s">
-        <v>2183</v>
+        <v>2191</v>
       </c>
       <c r="H2059" t="s">
-        <v>2191</v>
+        <v>606</v>
       </c>
       <c r="I2059" t="s">
         <v>19</v>
@@ -85177,10 +85267,10 @@
         <v>1</v>
       </c>
       <c r="K2059">
-        <v>2500000</v>
+        <v>750000</v>
       </c>
       <c r="L2059">
-        <v>2500000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="2060" spans="1:12">
@@ -85194,19 +85284,19 @@
         <v>13</v>
       </c>
       <c r="D2060" t="s">
-        <v>2192</v>
+        <v>2176</v>
       </c>
       <c r="E2060" t="s">
-        <v>2193</v>
+        <v>2189</v>
       </c>
       <c r="F2060" t="s">
-        <v>2194</v>
+        <v>2190</v>
       </c>
       <c r="G2060" t="s">
-        <v>2195</v>
+        <v>2191</v>
       </c>
       <c r="H2060" t="s">
-        <v>43</v>
+        <v>2198</v>
       </c>
       <c r="I2060" t="s">
         <v>19</v>
@@ -85215,10 +85305,10 @@
         <v>1</v>
       </c>
       <c r="K2060">
-        <v>162394500</v>
+        <v>1350000</v>
       </c>
       <c r="L2060">
-        <v>162394500</v>
+        <v>1350000</v>
       </c>
     </row>
     <row r="2061" spans="1:12">
@@ -85232,19 +85322,19 @@
         <v>13</v>
       </c>
       <c r="D2061" t="s">
-        <v>2192</v>
+        <v>2176</v>
       </c>
       <c r="E2061" t="s">
-        <v>2193</v>
+        <v>2189</v>
       </c>
       <c r="F2061" t="s">
-        <v>2194</v>
+        <v>2190</v>
       </c>
       <c r="G2061" t="s">
-        <v>2195</v>
+        <v>2191</v>
       </c>
       <c r="H2061" t="s">
-        <v>44</v>
+        <v>2199</v>
       </c>
       <c r="I2061" t="s">
         <v>19</v>
@@ -85253,10 +85343,10 @@
         <v>1</v>
       </c>
       <c r="K2061">
-        <v>2536</v>
+        <v>2500000</v>
       </c>
       <c r="L2061">
-        <v>2536</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="2062" spans="1:12">
@@ -85270,19 +85360,19 @@
         <v>13</v>
       </c>
       <c r="D2062" t="s">
-        <v>2192</v>
+        <v>2165</v>
       </c>
       <c r="E2062" t="s">
-        <v>2193</v>
+        <v>2200</v>
       </c>
       <c r="F2062" t="s">
-        <v>2194</v>
+        <v>2201</v>
       </c>
       <c r="G2062" t="s">
-        <v>2195</v>
+        <v>2202</v>
       </c>
       <c r="H2062" t="s">
-        <v>45</v>
+        <v>2169</v>
       </c>
       <c r="I2062" t="s">
         <v>19</v>
@@ -85291,10 +85381,10 @@
         <v>1</v>
       </c>
       <c r="K2062">
-        <v>10583560</v>
+        <v>82000</v>
       </c>
       <c r="L2062">
-        <v>10583560</v>
+        <v>82000</v>
       </c>
     </row>
     <row r="2063" spans="1:12">
@@ -85308,19 +85398,19 @@
         <v>13</v>
       </c>
       <c r="D2063" t="s">
-        <v>2192</v>
+        <v>2165</v>
       </c>
       <c r="E2063" t="s">
-        <v>2193</v>
+        <v>2203</v>
       </c>
       <c r="F2063" t="s">
-        <v>2194</v>
+        <v>2204</v>
       </c>
       <c r="G2063" t="s">
-        <v>2195</v>
+        <v>2205</v>
       </c>
       <c r="H2063" t="s">
-        <v>46</v>
+        <v>236</v>
       </c>
       <c r="I2063" t="s">
         <v>19</v>
@@ -85329,10 +85419,10 @@
         <v>1</v>
       </c>
       <c r="K2063">
-        <v>3266244</v>
+        <v>22690740</v>
       </c>
       <c r="L2063">
-        <v>3266244</v>
+        <v>22690740</v>
       </c>
     </row>
     <row r="2064" spans="1:12">
@@ -85346,19 +85436,19 @@
         <v>13</v>
       </c>
       <c r="D2064" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2064" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
       <c r="F2064" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="G2064" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
       <c r="H2064" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I2064" t="s">
         <v>19</v>
@@ -85367,10 +85457,10 @@
         <v>1</v>
       </c>
       <c r="K2064">
-        <v>5770000</v>
+        <v>162394500</v>
       </c>
       <c r="L2064">
-        <v>5770000</v>
+        <v>162394500</v>
       </c>
     </row>
     <row r="2065" spans="1:12">
@@ -85384,19 +85474,19 @@
         <v>13</v>
       </c>
       <c r="D2065" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2065" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
       <c r="F2065" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="G2065" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
       <c r="H2065" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I2065" t="s">
         <v>19</v>
@@ -85405,10 +85495,10 @@
         <v>1</v>
       </c>
       <c r="K2065">
-        <v>10720000</v>
+        <v>2536</v>
       </c>
       <c r="L2065">
-        <v>10720000</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="2066" spans="1:12">
@@ -85422,19 +85512,19 @@
         <v>13</v>
       </c>
       <c r="D2066" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2066" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
       <c r="F2066" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="G2066" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
       <c r="H2066" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I2066" t="s">
         <v>19</v>
@@ -85443,10 +85533,10 @@
         <v>1</v>
       </c>
       <c r="K2066">
-        <v>2843062</v>
+        <v>10583560</v>
       </c>
       <c r="L2066">
-        <v>2843062</v>
+        <v>10583560</v>
       </c>
     </row>
     <row r="2067" spans="1:12">
@@ -85460,19 +85550,19 @@
         <v>13</v>
       </c>
       <c r="D2067" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2067" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
       <c r="F2067" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="G2067" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
       <c r="H2067" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I2067" t="s">
         <v>19</v>
@@ -85481,10 +85571,10 @@
         <v>1</v>
       </c>
       <c r="K2067">
-        <v>8545560</v>
+        <v>3266244</v>
       </c>
       <c r="L2067">
-        <v>8545560</v>
+        <v>3266244</v>
       </c>
     </row>
     <row r="2068" spans="1:12">
@@ -85498,19 +85588,19 @@
         <v>13</v>
       </c>
       <c r="D2068" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2068" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
       <c r="F2068" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="G2068" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
       <c r="H2068" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I2068" t="s">
         <v>19</v>
@@ -85519,10 +85609,10 @@
         <v>1</v>
       </c>
       <c r="K2068">
-        <v>4985000</v>
+        <v>5770000</v>
       </c>
       <c r="L2068">
-        <v>4985000</v>
+        <v>5770000</v>
       </c>
     </row>
     <row r="2069" spans="1:12">
@@ -85536,19 +85626,19 @@
         <v>13</v>
       </c>
       <c r="D2069" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2069" t="s">
-        <v>2196</v>
+        <v>2207</v>
       </c>
       <c r="F2069" t="s">
-        <v>2197</v>
+        <v>2208</v>
       </c>
       <c r="G2069" t="s">
-        <v>2198</v>
+        <v>2209</v>
       </c>
       <c r="H2069" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="I2069" t="s">
         <v>19</v>
@@ -85557,10 +85647,10 @@
         <v>1</v>
       </c>
       <c r="K2069">
-        <v>153281600</v>
+        <v>10720000</v>
       </c>
       <c r="L2069">
-        <v>153281600</v>
+        <v>10720000</v>
       </c>
     </row>
     <row r="2070" spans="1:12">
@@ -85574,19 +85664,19 @@
         <v>13</v>
       </c>
       <c r="D2070" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2070" t="s">
-        <v>2196</v>
+        <v>2207</v>
       </c>
       <c r="F2070" t="s">
-        <v>2197</v>
+        <v>2208</v>
       </c>
       <c r="G2070" t="s">
-        <v>2198</v>
+        <v>2209</v>
       </c>
       <c r="H2070" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="I2070" t="s">
         <v>19</v>
@@ -85595,10 +85685,10 @@
         <v>1</v>
       </c>
       <c r="K2070">
-        <v>2534</v>
+        <v>2843062</v>
       </c>
       <c r="L2070">
-        <v>2534</v>
+        <v>2843062</v>
       </c>
     </row>
     <row r="2071" spans="1:12">
@@ -85612,19 +85702,19 @@
         <v>13</v>
       </c>
       <c r="D2071" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2071" t="s">
-        <v>2196</v>
+        <v>2207</v>
       </c>
       <c r="F2071" t="s">
-        <v>2197</v>
+        <v>2208</v>
       </c>
       <c r="G2071" t="s">
-        <v>2198</v>
+        <v>2209</v>
       </c>
       <c r="H2071" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="I2071" t="s">
         <v>19</v>
@@ -85633,10 +85723,10 @@
         <v>1</v>
       </c>
       <c r="K2071">
-        <v>11090340</v>
+        <v>8545560</v>
       </c>
       <c r="L2071">
-        <v>11090340</v>
+        <v>8545560</v>
       </c>
     </row>
     <row r="2072" spans="1:12">
@@ -85650,19 +85740,19 @@
         <v>13</v>
       </c>
       <c r="D2072" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2072" t="s">
-        <v>2196</v>
+        <v>2207</v>
       </c>
       <c r="F2072" t="s">
-        <v>2197</v>
+        <v>2208</v>
       </c>
       <c r="G2072" t="s">
-        <v>2198</v>
+        <v>2209</v>
       </c>
       <c r="H2072" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I2072" t="s">
         <v>19</v>
@@ -85671,10 +85761,10 @@
         <v>1</v>
       </c>
       <c r="K2072">
-        <v>3280146</v>
+        <v>4985000</v>
       </c>
       <c r="L2072">
-        <v>3280146</v>
+        <v>4985000</v>
       </c>
     </row>
     <row r="2073" spans="1:12">
@@ -85688,19 +85778,19 @@
         <v>13</v>
       </c>
       <c r="D2073" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2073" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
       <c r="F2073" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
       <c r="G2073" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
       <c r="H2073" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I2073" t="s">
         <v>19</v>
@@ -85709,10 +85799,10 @@
         <v>1</v>
       </c>
       <c r="K2073">
-        <v>3250000</v>
+        <v>153281600</v>
       </c>
       <c r="L2073">
-        <v>3250000</v>
+        <v>153281600</v>
       </c>
     </row>
     <row r="2074" spans="1:12">
@@ -85726,19 +85816,19 @@
         <v>13</v>
       </c>
       <c r="D2074" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2074" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
       <c r="F2074" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
       <c r="G2074" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
       <c r="H2074" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I2074" t="s">
         <v>19</v>
@@ -85747,10 +85837,10 @@
         <v>1</v>
       </c>
       <c r="K2074">
-        <v>15850000</v>
+        <v>2534</v>
       </c>
       <c r="L2074">
-        <v>15850000</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="2075" spans="1:12">
@@ -85764,19 +85854,19 @@
         <v>13</v>
       </c>
       <c r="D2075" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2075" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
       <c r="F2075" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
       <c r="G2075" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
       <c r="H2075" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I2075" t="s">
         <v>19</v>
@@ -85785,10 +85875,10 @@
         <v>1</v>
       </c>
       <c r="K2075">
-        <v>3142700</v>
+        <v>11090340</v>
       </c>
       <c r="L2075">
-        <v>3142700</v>
+        <v>11090340</v>
       </c>
     </row>
     <row r="2076" spans="1:12">
@@ -85802,19 +85892,19 @@
         <v>13</v>
       </c>
       <c r="D2076" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2076" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
       <c r="F2076" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
       <c r="G2076" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
       <c r="H2076" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I2076" t="s">
         <v>19</v>
@@ -85823,10 +85913,10 @@
         <v>1</v>
       </c>
       <c r="K2076">
-        <v>7893780</v>
+        <v>3280146</v>
       </c>
       <c r="L2076">
-        <v>7893780</v>
+        <v>3280146</v>
       </c>
     </row>
     <row r="2077" spans="1:12">
@@ -85840,19 +85930,19 @@
         <v>13</v>
       </c>
       <c r="D2077" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2077" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
       <c r="F2077" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
       <c r="G2077" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
       <c r="H2077" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I2077" t="s">
         <v>19</v>
@@ -85861,10 +85951,10 @@
         <v>1</v>
       </c>
       <c r="K2077">
-        <v>3150000</v>
+        <v>3250000</v>
       </c>
       <c r="L2077">
-        <v>3150000</v>
+        <v>3250000</v>
       </c>
     </row>
     <row r="2078" spans="1:12">
@@ -85878,19 +85968,19 @@
         <v>13</v>
       </c>
       <c r="D2078" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2078" t="s">
-        <v>2199</v>
+        <v>2210</v>
       </c>
       <c r="F2078" t="s">
-        <v>2200</v>
+        <v>2211</v>
       </c>
       <c r="G2078" t="s">
-        <v>2201</v>
+        <v>2212</v>
       </c>
       <c r="H2078" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="I2078" t="s">
         <v>19</v>
@@ -85899,10 +85989,10 @@
         <v>1</v>
       </c>
       <c r="K2078">
-        <v>271970200</v>
+        <v>15850000</v>
       </c>
       <c r="L2078">
-        <v>271970200</v>
+        <v>15850000</v>
       </c>
     </row>
     <row r="2079" spans="1:12">
@@ -85916,19 +86006,19 @@
         <v>13</v>
       </c>
       <c r="D2079" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2079" t="s">
-        <v>2199</v>
+        <v>2210</v>
       </c>
       <c r="F2079" t="s">
-        <v>2200</v>
+        <v>2211</v>
       </c>
       <c r="G2079" t="s">
-        <v>2201</v>
+        <v>2212</v>
       </c>
       <c r="H2079" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I2079" t="s">
         <v>19</v>
@@ -85937,10 +86027,10 @@
         <v>1</v>
       </c>
       <c r="K2079">
-        <v>5000</v>
+        <v>3142700</v>
       </c>
       <c r="L2079">
-        <v>5000</v>
+        <v>3142700</v>
       </c>
     </row>
     <row r="2080" spans="1:12">
@@ -85954,19 +86044,19 @@
         <v>13</v>
       </c>
       <c r="D2080" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2080" t="s">
-        <v>2199</v>
+        <v>2210</v>
       </c>
       <c r="F2080" t="s">
-        <v>2200</v>
+        <v>2211</v>
       </c>
       <c r="G2080" t="s">
-        <v>2201</v>
+        <v>2212</v>
       </c>
       <c r="H2080" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I2080" t="s">
         <v>19</v>
@@ -85975,10 +86065,10 @@
         <v>1</v>
       </c>
       <c r="K2080">
-        <v>16312930</v>
+        <v>7893780</v>
       </c>
       <c r="L2080">
-        <v>16312930</v>
+        <v>7893780</v>
       </c>
     </row>
     <row r="2081" spans="1:12">
@@ -85992,19 +86082,19 @@
         <v>13</v>
       </c>
       <c r="D2081" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2081" t="s">
-        <v>2199</v>
+        <v>2210</v>
       </c>
       <c r="F2081" t="s">
-        <v>2200</v>
+        <v>2211</v>
       </c>
       <c r="G2081" t="s">
-        <v>2201</v>
+        <v>2212</v>
       </c>
       <c r="H2081" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="I2081" t="s">
         <v>19</v>
@@ -86013,10 +86103,10 @@
         <v>1</v>
       </c>
       <c r="K2081">
-        <v>5728350</v>
+        <v>3150000</v>
       </c>
       <c r="L2081">
-        <v>5728350</v>
+        <v>3150000</v>
       </c>
     </row>
     <row r="2082" spans="1:12">
@@ -86030,19 +86120,19 @@
         <v>13</v>
       </c>
       <c r="D2082" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2082" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
       <c r="F2082" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
       <c r="G2082" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
       <c r="H2082" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I2082" t="s">
         <v>19</v>
@@ -86051,10 +86141,10 @@
         <v>1</v>
       </c>
       <c r="K2082">
-        <v>7525000</v>
+        <v>271970200</v>
       </c>
       <c r="L2082">
-        <v>7525000</v>
+        <v>271970200</v>
       </c>
     </row>
     <row r="2083" spans="1:12">
@@ -86068,19 +86158,19 @@
         <v>13</v>
       </c>
       <c r="D2083" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2083" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
       <c r="F2083" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
       <c r="G2083" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
       <c r="H2083" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I2083" t="s">
         <v>19</v>
@@ -86089,10 +86179,10 @@
         <v>1</v>
       </c>
       <c r="K2083">
-        <v>24915000</v>
+        <v>5000</v>
       </c>
       <c r="L2083">
-        <v>24915000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="2084" spans="1:12">
@@ -86106,19 +86196,19 @@
         <v>13</v>
       </c>
       <c r="D2084" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2084" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
       <c r="F2084" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
       <c r="G2084" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
       <c r="H2084" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I2084" t="s">
         <v>19</v>
@@ -86127,10 +86217,10 @@
         <v>1</v>
       </c>
       <c r="K2084">
-        <v>4173278</v>
+        <v>16312930</v>
       </c>
       <c r="L2084">
-        <v>4173278</v>
+        <v>16312930</v>
       </c>
     </row>
     <row r="2085" spans="1:12">
@@ -86144,19 +86234,19 @@
         <v>13</v>
       </c>
       <c r="D2085" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2085" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
       <c r="F2085" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
       <c r="G2085" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
       <c r="H2085" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I2085" t="s">
         <v>19</v>
@@ -86165,10 +86255,10 @@
         <v>1</v>
       </c>
       <c r="K2085">
-        <v>14556420</v>
+        <v>5728350</v>
       </c>
       <c r="L2085">
-        <v>14556420</v>
+        <v>5728350</v>
       </c>
     </row>
     <row r="2086" spans="1:12">
@@ -86182,19 +86272,19 @@
         <v>13</v>
       </c>
       <c r="D2086" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2086" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
       <c r="F2086" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
       <c r="G2086" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
       <c r="H2086" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I2086" t="s">
         <v>19</v>
@@ -86203,10 +86293,10 @@
         <v>1</v>
       </c>
       <c r="K2086">
-        <v>7375000</v>
+        <v>7525000</v>
       </c>
       <c r="L2086">
-        <v>7375000</v>
+        <v>7525000</v>
       </c>
     </row>
     <row r="2087" spans="1:12">
@@ -86220,19 +86310,19 @@
         <v>13</v>
       </c>
       <c r="D2087" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2087" t="s">
-        <v>2202</v>
+        <v>2213</v>
       </c>
       <c r="F2087" t="s">
-        <v>2203</v>
+        <v>2214</v>
       </c>
       <c r="G2087" t="s">
-        <v>2204</v>
+        <v>2215</v>
       </c>
       <c r="H2087" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I2087" t="s">
         <v>19</v>
@@ -86241,10 +86331,10 @@
         <v>1</v>
       </c>
       <c r="K2087">
-        <v>1841440</v>
+        <v>24915000</v>
       </c>
       <c r="L2087">
-        <v>1841440</v>
+        <v>24915000</v>
       </c>
     </row>
     <row r="2088" spans="1:12">
@@ -86258,19 +86348,19 @@
         <v>13</v>
       </c>
       <c r="D2088" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2088" t="s">
-        <v>2202</v>
+        <v>2213</v>
       </c>
       <c r="F2088" t="s">
-        <v>2203</v>
+        <v>2214</v>
       </c>
       <c r="G2088" t="s">
-        <v>2204</v>
+        <v>2215</v>
       </c>
       <c r="H2088" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I2088" t="s">
         <v>19</v>
@@ -86279,10 +86369,10 @@
         <v>1</v>
       </c>
       <c r="K2088">
-        <v>40</v>
+        <v>4173278</v>
       </c>
       <c r="L2088">
-        <v>40</v>
+        <v>4173278</v>
       </c>
     </row>
     <row r="2089" spans="1:12">
@@ -86296,16 +86386,16 @@
         <v>13</v>
       </c>
       <c r="D2089" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2089" t="s">
-        <v>2202</v>
+        <v>2213</v>
       </c>
       <c r="F2089" t="s">
-        <v>2203</v>
+        <v>2214</v>
       </c>
       <c r="G2089" t="s">
-        <v>2204</v>
+        <v>2215</v>
       </c>
       <c r="H2089" t="s">
         <v>26</v>
@@ -86317,10 +86407,10 @@
         <v>1</v>
       </c>
       <c r="K2089">
-        <v>72420</v>
+        <v>14556420</v>
       </c>
       <c r="L2089">
-        <v>72420</v>
+        <v>14556420</v>
       </c>
     </row>
     <row r="2090" spans="1:12">
@@ -86334,16 +86424,16 @@
         <v>13</v>
       </c>
       <c r="D2090" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
       <c r="E2090" t="s">
-        <v>2202</v>
+        <v>2213</v>
       </c>
       <c r="F2090" t="s">
-        <v>2203</v>
+        <v>2214</v>
       </c>
       <c r="G2090" t="s">
-        <v>2204</v>
+        <v>2215</v>
       </c>
       <c r="H2090" t="s">
         <v>27</v>
@@ -86355,10 +86445,10 @@
         <v>1</v>
       </c>
       <c r="K2090">
-        <v>180000</v>
+        <v>7375000</v>
       </c>
       <c r="L2090">
-        <v>180000</v>
+        <v>7375000</v>
       </c>
     </row>
     <row r="2091" spans="1:12">
@@ -86372,19 +86462,19 @@
         <v>13</v>
       </c>
       <c r="D2091" t="s">
-        <v>2168</v>
+        <v>2206</v>
       </c>
       <c r="E2091" t="s">
-        <v>2205</v>
+        <v>2216</v>
       </c>
       <c r="F2091" t="s">
-        <v>2206</v>
+        <v>2217</v>
       </c>
       <c r="G2091" t="s">
-        <v>2207</v>
+        <v>2218</v>
       </c>
       <c r="H2091" t="s">
-        <v>2208</v>
+        <v>18</v>
       </c>
       <c r="I2091" t="s">
         <v>19</v>
@@ -86393,10 +86483,10 @@
         <v>1</v>
       </c>
       <c r="K2091">
-        <v>1444000</v>
+        <v>1841440</v>
       </c>
       <c r="L2091">
-        <v>1444000</v>
+        <v>1841440</v>
       </c>
     </row>
     <row r="2092" spans="1:12">
@@ -86410,19 +86500,19 @@
         <v>13</v>
       </c>
       <c r="D2092" t="s">
-        <v>2168</v>
+        <v>2206</v>
       </c>
       <c r="E2092" t="s">
-        <v>2209</v>
+        <v>2216</v>
       </c>
       <c r="F2092" t="s">
-        <v>2210</v>
+        <v>2217</v>
       </c>
       <c r="G2092" t="s">
-        <v>2211</v>
+        <v>2218</v>
       </c>
       <c r="H2092" t="s">
-        <v>2208</v>
+        <v>20</v>
       </c>
       <c r="I2092" t="s">
         <v>19</v>
@@ -86431,10 +86521,10 @@
         <v>1</v>
       </c>
       <c r="K2092">
-        <v>542000</v>
+        <v>40</v>
       </c>
       <c r="L2092">
-        <v>542000</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2093" spans="1:12">
@@ -86448,19 +86538,19 @@
         <v>13</v>
       </c>
       <c r="D2093" t="s">
-        <v>2168</v>
+        <v>2206</v>
       </c>
       <c r="E2093" t="s">
-        <v>2212</v>
+        <v>2216</v>
       </c>
       <c r="F2093" t="s">
-        <v>2213</v>
+        <v>2217</v>
       </c>
       <c r="G2093" t="s">
-        <v>2214</v>
+        <v>2218</v>
       </c>
       <c r="H2093" t="s">
-        <v>2208</v>
+        <v>26</v>
       </c>
       <c r="I2093" t="s">
         <v>19</v>
@@ -86469,10 +86559,504 @@
         <v>1</v>
       </c>
       <c r="K2093">
+        <v>72420</v>
+      </c>
+      <c r="L2093">
+        <v>72420</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:12">
+      <c r="A2094">
+        <v>2091</v>
+      </c>
+      <c r="B2094">
+        <v>626402</v>
+      </c>
+      <c r="C2094" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2094" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E2094" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F2094" t="s">
+        <v>2217</v>
+      </c>
+      <c r="G2094" t="s">
+        <v>2218</v>
+      </c>
+      <c r="H2094" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2094" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2094">
+        <v>1</v>
+      </c>
+      <c r="K2094">
+        <v>180000</v>
+      </c>
+      <c r="L2094">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:12">
+      <c r="A2095">
+        <v>2092</v>
+      </c>
+      <c r="B2095">
+        <v>626402</v>
+      </c>
+      <c r="C2095" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2095" t="s">
+        <v>2176</v>
+      </c>
+      <c r="E2095" t="s">
+        <v>2219</v>
+      </c>
+      <c r="F2095" t="s">
+        <v>2220</v>
+      </c>
+      <c r="G2095" t="s">
+        <v>2221</v>
+      </c>
+      <c r="H2095" t="s">
+        <v>2222</v>
+      </c>
+      <c r="I2095" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2095">
+        <v>1</v>
+      </c>
+      <c r="K2095">
+        <v>1444000</v>
+      </c>
+      <c r="L2095">
+        <v>1444000</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:12">
+      <c r="A2096">
+        <v>2093</v>
+      </c>
+      <c r="B2096">
+        <v>626402</v>
+      </c>
+      <c r="C2096" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2096" t="s">
+        <v>2176</v>
+      </c>
+      <c r="E2096" t="s">
+        <v>2223</v>
+      </c>
+      <c r="F2096" t="s">
+        <v>2224</v>
+      </c>
+      <c r="G2096" t="s">
+        <v>2225</v>
+      </c>
+      <c r="H2096" t="s">
+        <v>2222</v>
+      </c>
+      <c r="I2096" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2096">
+        <v>1</v>
+      </c>
+      <c r="K2096">
+        <v>542000</v>
+      </c>
+      <c r="L2096">
+        <v>542000</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:12">
+      <c r="A2097">
+        <v>2094</v>
+      </c>
+      <c r="B2097">
+        <v>626402</v>
+      </c>
+      <c r="C2097" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2097" t="s">
+        <v>2176</v>
+      </c>
+      <c r="E2097" t="s">
+        <v>2226</v>
+      </c>
+      <c r="F2097" t="s">
+        <v>2227</v>
+      </c>
+      <c r="G2097" t="s">
+        <v>2228</v>
+      </c>
+      <c r="H2097" t="s">
+        <v>2222</v>
+      </c>
+      <c r="I2097" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2097">
+        <v>1</v>
+      </c>
+      <c r="K2097">
         <v>1528000</v>
       </c>
-      <c r="L2093">
+      <c r="L2097">
         <v>1528000</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:12">
+      <c r="A2098">
+        <v>2095</v>
+      </c>
+      <c r="B2098">
+        <v>626402</v>
+      </c>
+      <c r="C2098" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2098" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E2098" t="s">
+        <v>2229</v>
+      </c>
+      <c r="F2098" t="s">
+        <v>2230</v>
+      </c>
+      <c r="G2098" t="s">
+        <v>2231</v>
+      </c>
+      <c r="H2098" t="s">
+        <v>420</v>
+      </c>
+      <c r="I2098" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2098">
+        <v>1</v>
+      </c>
+      <c r="K2098">
+        <v>15000000</v>
+      </c>
+      <c r="L2098">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:12">
+      <c r="A2099">
+        <v>2096</v>
+      </c>
+      <c r="B2099">
+        <v>626402</v>
+      </c>
+      <c r="C2099" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2099" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E2099" t="s">
+        <v>2232</v>
+      </c>
+      <c r="F2099" t="s">
+        <v>2233</v>
+      </c>
+      <c r="G2099" t="s">
+        <v>2234</v>
+      </c>
+      <c r="H2099" t="s">
+        <v>420</v>
+      </c>
+      <c r="I2099" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2099">
+        <v>1</v>
+      </c>
+      <c r="K2099">
+        <v>6000000</v>
+      </c>
+      <c r="L2099">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:12">
+      <c r="A2100">
+        <v>2097</v>
+      </c>
+      <c r="B2100">
+        <v>626402</v>
+      </c>
+      <c r="C2100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2100" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E2100" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F2100" t="s">
+        <v>2236</v>
+      </c>
+      <c r="G2100" t="s">
+        <v>2237</v>
+      </c>
+      <c r="H2100" t="s">
+        <v>2238</v>
+      </c>
+      <c r="I2100" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2100">
+        <v>1</v>
+      </c>
+      <c r="K2100">
+        <v>1600000</v>
+      </c>
+      <c r="L2100">
+        <v>1600000</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:12">
+      <c r="A2101">
+        <v>2098</v>
+      </c>
+      <c r="B2101">
+        <v>626402</v>
+      </c>
+      <c r="C2101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2101" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E2101" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F2101" t="s">
+        <v>2236</v>
+      </c>
+      <c r="G2101" t="s">
+        <v>2237</v>
+      </c>
+      <c r="H2101" t="s">
+        <v>2239</v>
+      </c>
+      <c r="I2101" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2101">
+        <v>1</v>
+      </c>
+      <c r="K2101">
+        <v>1200000</v>
+      </c>
+      <c r="L2101">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:12">
+      <c r="A2102">
+        <v>2099</v>
+      </c>
+      <c r="B2102">
+        <v>626402</v>
+      </c>
+      <c r="C2102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2102" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E2102" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F2102" t="s">
+        <v>2236</v>
+      </c>
+      <c r="G2102" t="s">
+        <v>2237</v>
+      </c>
+      <c r="H2102" t="s">
+        <v>2240</v>
+      </c>
+      <c r="I2102" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2102">
+        <v>1</v>
+      </c>
+      <c r="K2102">
+        <v>8400000</v>
+      </c>
+      <c r="L2102">
+        <v>8400000</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:12">
+      <c r="A2103">
+        <v>2100</v>
+      </c>
+      <c r="B2103">
+        <v>626402</v>
+      </c>
+      <c r="C2103" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2103" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E2103" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2103" t="s">
+        <v>2242</v>
+      </c>
+      <c r="G2103" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2103" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2103" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2103">
+        <v>1</v>
+      </c>
+      <c r="K2103">
+        <v>27850000</v>
+      </c>
+      <c r="L2103">
+        <v>27850000</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:12">
+      <c r="A2104">
+        <v>2101</v>
+      </c>
+      <c r="B2104">
+        <v>626402</v>
+      </c>
+      <c r="C2104" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2104" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E2104" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2104" t="s">
+        <v>2242</v>
+      </c>
+      <c r="G2104" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2104" t="s">
+        <v>2243</v>
+      </c>
+      <c r="I2104" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2104">
+        <v>1</v>
+      </c>
+      <c r="K2104">
+        <v>2880000</v>
+      </c>
+      <c r="L2104">
+        <v>2880000</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:12">
+      <c r="A2105">
+        <v>2102</v>
+      </c>
+      <c r="B2105">
+        <v>626402</v>
+      </c>
+      <c r="C2105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2105" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E2105" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2105" t="s">
+        <v>2242</v>
+      </c>
+      <c r="G2105" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2105" t="s">
+        <v>2244</v>
+      </c>
+      <c r="I2105" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2105">
+        <v>1</v>
+      </c>
+      <c r="K2105">
+        <v>1800000</v>
+      </c>
+      <c r="L2105">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:12">
+      <c r="A2106">
+        <v>2103</v>
+      </c>
+      <c r="B2106">
+        <v>626402</v>
+      </c>
+      <c r="C2106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2106" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E2106" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2106" t="s">
+        <v>2242</v>
+      </c>
+      <c r="G2106" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2106" t="s">
+        <v>757</v>
+      </c>
+      <c r="I2106" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2106">
+        <v>1</v>
+      </c>
+      <c r="K2106">
+        <v>400000</v>
+      </c>
+      <c r="L2106">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update plus tukin mei
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2458">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -7061,6 +7061,18 @@
     <t>Pembayaran tunjangan kinerja susulan bulan Mei tahun 2023 untuk 76 Pegawai/Anggota Polri/Prajurit TNI.</t>
   </si>
   <si>
+    <t>2023-06-12</t>
+  </si>
+  <si>
+    <t>'00530T</t>
+  </si>
+  <si>
+    <t>'231751303013325</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.3007/BRSDM.1/KP.440/VI/2023 Tanggal 5 Juni 2023</t>
+  </si>
+  <si>
     <t>'00531T</t>
   </si>
   <si>
@@ -7068,6 +7080,315 @@
   </si>
   <si>
     <t>Pembayaran tunjangan kinerja susulan bulan Mei tahun 2023 untuk 34 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00532T</t>
+  </si>
+  <si>
+    <t>'231751303013321</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2988/BRSDM.1/KP.440/V/2023 Tanggal 24 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00533T</t>
+  </si>
+  <si>
+    <t>'231751303013322</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2971/BRSDM.1/KP.440/IV/2023 Tanggal 28 April 2023</t>
+  </si>
+  <si>
+    <t>'00534T</t>
+  </si>
+  <si>
+    <t>'231751303013487</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2459/BRSDM.1/KP.440/V/2023 Tanggal 11 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00535T</t>
+  </si>
+  <si>
+    <t>'231751303013323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2362/BRSDM.1/KP.440/V/2023 Tanggal 9 Mei 2023 </t>
+  </si>
+  <si>
+    <t>'00536T</t>
+  </si>
+  <si>
+    <t>'231751303013324</t>
+  </si>
+  <si>
+    <t>'00537T</t>
+  </si>
+  <si>
+    <t>'231751701003355</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0A.000002</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0B.000043</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0B.001464</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0D.000055</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0D.000056</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0D.001465</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000095</t>
+  </si>
+  <si>
+    <t>'626402.175.522151.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000098</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000091</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000102</t>
+  </si>
+  <si>
+    <t>'00538T</t>
+  </si>
+  <si>
+    <t>'231751303013316</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2869/BRSDM.1/KP.440/V/2023 Tanggal 29 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00539T</t>
+  </si>
+  <si>
+    <t>'231751303013317</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat TUgas Nomor:B.2757/BRSDM.1/KP.440/V/2023 Tanggal 24 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00540T</t>
+  </si>
+  <si>
+    <t>'231751303013318</t>
+  </si>
+  <si>
+    <t>'00541T</t>
+  </si>
+  <si>
+    <t>'231751303013319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2459/BRSDM.1/KP.440/V/2023 Tanggal 11 Mei 2023 </t>
+  </si>
+  <si>
+    <t>'00542T</t>
+  </si>
+  <si>
+    <t>'231751303013320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2971/BRSDM.1/KP.440/IV/2023 Tanggal 28 April 2023 </t>
+  </si>
+  <si>
+    <t>'00543T</t>
+  </si>
+  <si>
+    <t>'231751303013309</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2850/BRSDM.1/KP.440/VI/2023 Tanggal 29 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00544T</t>
+  </si>
+  <si>
+    <t>'231751303013310</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.730,B.2290/BRSDM.1/KP.440/V/2023 Tanggal 4 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00545T</t>
+  </si>
+  <si>
+    <t>'231751303013311</t>
+  </si>
+  <si>
+    <t>'00546T</t>
+  </si>
+  <si>
+    <t>'231751303013312</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.739,B.2290/BRSDM.1/KP.440/V/2023 Tanggal 4,5 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00547T</t>
+  </si>
+  <si>
+    <t>'231751303013313</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.731,B.2289/BRSDM.1/KP.440/V/2023 Tanggal 4,5 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00548T</t>
+  </si>
+  <si>
+    <t>'231751303013314</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2269/BRSDM.1/KP.440/V/2023 Tanggal 5 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00549T</t>
+  </si>
+  <si>
+    <t>'231751303013315</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2286/BRSDM.1/KP.440/V/2023 Tanggal 4 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00550T</t>
+  </si>
+  <si>
+    <t>'231751303013488</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.851/BRSDM/KP.440/V/2023 Tanggal 26 Mei 2023 dan ST.No.B.782/BRSDM.5/KP.440/VI/2023.Tanggal 26 Mei 2023.</t>
+  </si>
+  <si>
+    <t>'00551T</t>
+  </si>
+  <si>
+    <t>'231751303013483</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:B.2290/BRSDM.1/KP.440/V/2023 Tanggal 4 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00553T</t>
+  </si>
+  <si>
+    <t>'231751303013411</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan bulan Mei tahun 2023 untuk 43 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00554T</t>
+  </si>
+  <si>
+    <t>'231751303013484</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.802/BRSDM.5/KP.440/V/2023 Tanggal 31 Mei 2023 dan Nomor:B.810/BRSDM.5/KP.440/VI/2023 Tanggal 05 Juni 2023</t>
+  </si>
+  <si>
+    <t>'00555T</t>
+  </si>
+  <si>
+    <t>'231751302017708</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:025681201062023 Tanggal 5 Juni 2023 Tagihan Layanan Pay TV Transvision periode Juni 2023 s.d Mei 2024 (1 Tahun)</t>
+  </si>
+  <si>
+    <t>'00556T</t>
+  </si>
+  <si>
+    <t>'231751301022673</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitasni Nomor:SK/5719/VI/2023 Tanggal 5 Juni 2023 Biaya Sewa Mesin Foto Copy Bulan Mei 2023</t>
+  </si>
+  <si>
+    <t>'00557T</t>
+  </si>
+  <si>
+    <t>'231751302017729</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:104/KWT/STSK/PT/VI/2023 Tanggl 5 Juni 2023 Biaya Pembuatan Plakat Akrilik Stanlist BRSDM</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0A.000298</t>
+  </si>
+  <si>
+    <t>'00558T</t>
+  </si>
+  <si>
+    <t>'231751303013485</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Keputusan Nomor:1,2/PPK/BRSDM.1/I/2023 Tanggal 3 Januari 2023 Honor Tenaga Profesi Social Media Specialist dan Tenaga Content Creator Bulan Mei 2023</t>
+  </si>
+  <si>
+    <t>'00559T</t>
+  </si>
+  <si>
+    <t>'231751303013486</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2989/BRSDM.1/KP.440/VI/2023 Tanggal 31 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00560T</t>
+  </si>
+  <si>
+    <t>'231751303013481</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2221/BRSDM.1/KP.440/V/2023 Tanggal 2 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00561T</t>
+  </si>
+  <si>
+    <t>'231751303013482</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2213/BRSDM.1/KP.440/V/2023 Tanggal 2 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00562T</t>
+  </si>
+  <si>
+    <t>'231751701003353</t>
+  </si>
+  <si>
+    <t>'626402.175.521241.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.102.0A.000809</t>
+  </si>
+  <si>
+    <t>'626402.175.522151.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.101.0D.001197</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.101.0A.000797</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.0A.001028</t>
+  </si>
+  <si>
+    <t>'00563T</t>
+  </si>
+  <si>
+    <t>'231751701003354</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.0B.000204</t>
   </si>
 </sst>
 </file>
@@ -7409,7 +7730,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2258"/>
+  <dimension ref="A1:L2359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -93126,31 +93447,3869 @@
         <v>13</v>
       </c>
       <c r="D2258" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2258" t="s">
+        <v>2349</v>
+      </c>
+      <c r="F2258" t="s">
+        <v>2350</v>
+      </c>
+      <c r="G2258" t="s">
+        <v>2351</v>
+      </c>
+      <c r="H2258" t="s">
+        <v>582</v>
+      </c>
+      <c r="I2258" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2258">
+        <v>1</v>
+      </c>
+      <c r="K2258">
+        <v>34352000</v>
+      </c>
+      <c r="L2258">
+        <v>34352000</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:12">
+      <c r="A2259">
+        <v>2256</v>
+      </c>
+      <c r="B2259">
+        <v>626402</v>
+      </c>
+      <c r="C2259" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2259" t="s">
         <v>2236</v>
       </c>
-      <c r="E2258" t="s">
+      <c r="E2259" t="s">
+        <v>2352</v>
+      </c>
+      <c r="F2259" t="s">
+        <v>2353</v>
+      </c>
+      <c r="G2259" t="s">
+        <v>2354</v>
+      </c>
+      <c r="H2259" t="s">
+        <v>299</v>
+      </c>
+      <c r="I2259" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2259">
+        <v>1</v>
+      </c>
+      <c r="K2259">
+        <v>204638726</v>
+      </c>
+      <c r="L2259">
+        <v>204638726</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:12">
+      <c r="A2260">
+        <v>2257</v>
+      </c>
+      <c r="B2260">
+        <v>626402</v>
+      </c>
+      <c r="C2260" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2260" t="s">
         <v>2348</v>
       </c>
-      <c r="F2258" t="s">
+      <c r="E2260" t="s">
+        <v>2355</v>
+      </c>
+      <c r="F2260" t="s">
+        <v>2356</v>
+      </c>
+      <c r="G2260" t="s">
+        <v>2357</v>
+      </c>
+      <c r="H2260" t="s">
+        <v>583</v>
+      </c>
+      <c r="I2260" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2260">
+        <v>1</v>
+      </c>
+      <c r="K2260">
+        <v>8070000</v>
+      </c>
+      <c r="L2260">
+        <v>8070000</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:12">
+      <c r="A2261">
+        <v>2258</v>
+      </c>
+      <c r="B2261">
+        <v>626402</v>
+      </c>
+      <c r="C2261" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2261" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2261" t="s">
+        <v>2358</v>
+      </c>
+      <c r="F2261" t="s">
+        <v>2359</v>
+      </c>
+      <c r="G2261" t="s">
+        <v>2360</v>
+      </c>
+      <c r="H2261" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2261" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2261">
+        <v>1</v>
+      </c>
+      <c r="K2261">
+        <v>30947680</v>
+      </c>
+      <c r="L2261">
+        <v>30947680</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:12">
+      <c r="A2262">
+        <v>2259</v>
+      </c>
+      <c r="B2262">
+        <v>626402</v>
+      </c>
+      <c r="C2262" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2262" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2262" t="s">
+        <v>2361</v>
+      </c>
+      <c r="F2262" t="s">
+        <v>2362</v>
+      </c>
+      <c r="G2262" t="s">
+        <v>2363</v>
+      </c>
+      <c r="H2262" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2262" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2262">
+        <v>1</v>
+      </c>
+      <c r="K2262">
+        <v>16089800</v>
+      </c>
+      <c r="L2262">
+        <v>16089800</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:12">
+      <c r="A2263">
+        <v>2260</v>
+      </c>
+      <c r="B2263">
+        <v>626402</v>
+      </c>
+      <c r="C2263" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2263" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2263" t="s">
+        <v>2364</v>
+      </c>
+      <c r="F2263" t="s">
+        <v>2365</v>
+      </c>
+      <c r="G2263" t="s">
+        <v>2366</v>
+      </c>
+      <c r="H2263" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2263" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2263">
+        <v>1</v>
+      </c>
+      <c r="K2263">
+        <v>767500</v>
+      </c>
+      <c r="L2263">
+        <v>767500</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:12">
+      <c r="A2264">
+        <v>2261</v>
+      </c>
+      <c r="B2264">
+        <v>626402</v>
+      </c>
+      <c r="C2264" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2264" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2264" t="s">
+        <v>2367</v>
+      </c>
+      <c r="F2264" t="s">
+        <v>2368</v>
+      </c>
+      <c r="G2264" t="s">
+        <v>2360</v>
+      </c>
+      <c r="H2264" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2264" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2264">
+        <v>1</v>
+      </c>
+      <c r="K2264">
+        <v>16702083</v>
+      </c>
+      <c r="L2264">
+        <v>16702083</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:12">
+      <c r="A2265">
+        <v>2262</v>
+      </c>
+      <c r="B2265">
+        <v>626402</v>
+      </c>
+      <c r="C2265" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2265" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2265" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2265" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2265" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2265" t="s">
+        <v>2371</v>
+      </c>
+      <c r="I2265" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2265">
+        <v>1</v>
+      </c>
+      <c r="K2265">
+        <v>150400</v>
+      </c>
+      <c r="L2265">
+        <v>150400</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:12">
+      <c r="A2266">
+        <v>2263</v>
+      </c>
+      <c r="B2266">
+        <v>626402</v>
+      </c>
+      <c r="C2266" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2266" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2266" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2266" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2266" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2266" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2266" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2266">
+        <v>1</v>
+      </c>
+      <c r="K2266">
+        <v>382400</v>
+      </c>
+      <c r="L2266">
+        <v>382400</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:12">
+      <c r="A2267">
+        <v>2264</v>
+      </c>
+      <c r="B2267">
+        <v>626402</v>
+      </c>
+      <c r="C2267" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2267" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2267" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2267" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2267" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2267" t="s">
+        <v>2372</v>
+      </c>
+      <c r="I2267" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2267">
+        <v>1</v>
+      </c>
+      <c r="K2267">
+        <v>995000</v>
+      </c>
+      <c r="L2267">
+        <v>995000</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:12">
+      <c r="A2268">
+        <v>2265</v>
+      </c>
+      <c r="B2268">
+        <v>626402</v>
+      </c>
+      <c r="C2268" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2268" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2268" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2268" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2268" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2268" t="s">
+        <v>2373</v>
+      </c>
+      <c r="I2268" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2268">
+        <v>1</v>
+      </c>
+      <c r="K2268">
+        <v>3969200</v>
+      </c>
+      <c r="L2268">
+        <v>3969200</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:12">
+      <c r="A2269">
+        <v>2266</v>
+      </c>
+      <c r="B2269">
+        <v>626402</v>
+      </c>
+      <c r="C2269" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2269" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2269" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2269" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2269" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2269" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I2269" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2269">
+        <v>1</v>
+      </c>
+      <c r="K2269">
+        <v>990000</v>
+      </c>
+      <c r="L2269">
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:12">
+      <c r="A2270">
+        <v>2267</v>
+      </c>
+      <c r="B2270">
+        <v>626402</v>
+      </c>
+      <c r="C2270" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2270" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2270" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2270" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2270" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2270" t="s">
+        <v>2375</v>
+      </c>
+      <c r="I2270" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2270">
+        <v>1</v>
+      </c>
+      <c r="K2270">
+        <v>1000000</v>
+      </c>
+      <c r="L2270">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:12">
+      <c r="A2271">
+        <v>2268</v>
+      </c>
+      <c r="B2271">
+        <v>626402</v>
+      </c>
+      <c r="C2271" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2271" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2271" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2271" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2271" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2271" t="s">
+        <v>2376</v>
+      </c>
+      <c r="I2271" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2271">
+        <v>1</v>
+      </c>
+      <c r="K2271">
+        <v>3514000</v>
+      </c>
+      <c r="L2271">
+        <v>3514000</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:12">
+      <c r="A2272">
+        <v>2269</v>
+      </c>
+      <c r="B2272">
+        <v>626402</v>
+      </c>
+      <c r="C2272" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2272" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2272" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2272" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2272" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2272" t="s">
+        <v>597</v>
+      </c>
+      <c r="I2272" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2272">
+        <v>1</v>
+      </c>
+      <c r="K2272">
+        <v>800000</v>
+      </c>
+      <c r="L2272">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:12">
+      <c r="A2273">
+        <v>2270</v>
+      </c>
+      <c r="B2273">
+        <v>626402</v>
+      </c>
+      <c r="C2273" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2273" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2273" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2273" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2273" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2273" t="s">
+        <v>2377</v>
+      </c>
+      <c r="I2273" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2273">
+        <v>1</v>
+      </c>
+      <c r="K2273">
+        <v>1200000</v>
+      </c>
+      <c r="L2273">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:12">
+      <c r="A2274">
+        <v>2271</v>
+      </c>
+      <c r="B2274">
+        <v>626402</v>
+      </c>
+      <c r="C2274" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2274" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2274" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2274" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2274" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2274" t="s">
+        <v>321</v>
+      </c>
+      <c r="I2274" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2274">
+        <v>1</v>
+      </c>
+      <c r="K2274">
+        <v>1350000</v>
+      </c>
+      <c r="L2274">
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:12">
+      <c r="A2275">
+        <v>2272</v>
+      </c>
+      <c r="B2275">
+        <v>626402</v>
+      </c>
+      <c r="C2275" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2275" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2275" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2275" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2275" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2275" t="s">
+        <v>1921</v>
+      </c>
+      <c r="I2275" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2275">
+        <v>1</v>
+      </c>
+      <c r="K2275">
+        <v>686500</v>
+      </c>
+      <c r="L2275">
+        <v>686500</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:12">
+      <c r="A2276">
+        <v>2273</v>
+      </c>
+      <c r="B2276">
+        <v>626402</v>
+      </c>
+      <c r="C2276" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2276" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2276" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2276" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2276" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2276" t="s">
+        <v>2378</v>
+      </c>
+      <c r="I2276" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2276">
+        <v>1</v>
+      </c>
+      <c r="K2276">
+        <v>1400000</v>
+      </c>
+      <c r="L2276">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:12">
+      <c r="A2277">
+        <v>2274</v>
+      </c>
+      <c r="B2277">
+        <v>626402</v>
+      </c>
+      <c r="C2277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2277" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2277" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2277" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2277" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2277" t="s">
+        <v>1478</v>
+      </c>
+      <c r="I2277" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2277">
+        <v>1</v>
+      </c>
+      <c r="K2277">
+        <v>150000</v>
+      </c>
+      <c r="L2277">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:12">
+      <c r="A2278">
+        <v>2275</v>
+      </c>
+      <c r="B2278">
+        <v>626402</v>
+      </c>
+      <c r="C2278" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2278" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2278" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2278" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2278" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2278" t="s">
+        <v>598</v>
+      </c>
+      <c r="I2278" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2278">
+        <v>1</v>
+      </c>
+      <c r="K2278">
+        <v>3545500</v>
+      </c>
+      <c r="L2278">
+        <v>3545500</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:12">
+      <c r="A2279">
+        <v>2276</v>
+      </c>
+      <c r="B2279">
+        <v>626402</v>
+      </c>
+      <c r="C2279" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2279" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2279" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2279" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2279" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2279" t="s">
+        <v>336</v>
+      </c>
+      <c r="I2279" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2279">
+        <v>1</v>
+      </c>
+      <c r="K2279">
+        <v>450000</v>
+      </c>
+      <c r="L2279">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:12">
+      <c r="A2280">
+        <v>2277</v>
+      </c>
+      <c r="B2280">
+        <v>626402</v>
+      </c>
+      <c r="C2280" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2280" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2280" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2280" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2280" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2280" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2280" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2280">
+        <v>1</v>
+      </c>
+      <c r="K2280">
+        <v>13737426</v>
+      </c>
+      <c r="L2280">
+        <v>13737426</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:12">
+      <c r="A2281">
+        <v>2278</v>
+      </c>
+      <c r="B2281">
+        <v>626402</v>
+      </c>
+      <c r="C2281" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2281" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2281" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2281" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2281" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2281" t="s">
+        <v>338</v>
+      </c>
+      <c r="I2281" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2281">
+        <v>1</v>
+      </c>
+      <c r="K2281">
+        <v>292500</v>
+      </c>
+      <c r="L2281">
+        <v>292500</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:12">
+      <c r="A2282">
+        <v>2279</v>
+      </c>
+      <c r="B2282">
+        <v>626402</v>
+      </c>
+      <c r="C2282" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2282" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2282" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2282" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2282" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2282" t="s">
+        <v>522</v>
+      </c>
+      <c r="I2282" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2282">
+        <v>1</v>
+      </c>
+      <c r="K2282">
+        <v>280000</v>
+      </c>
+      <c r="L2282">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:12">
+      <c r="A2283">
+        <v>2280</v>
+      </c>
+      <c r="B2283">
+        <v>626402</v>
+      </c>
+      <c r="C2283" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2283" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2283" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2283" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2283" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2283" t="s">
+        <v>599</v>
+      </c>
+      <c r="I2283" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2283">
+        <v>1</v>
+      </c>
+      <c r="K2283">
+        <v>433000</v>
+      </c>
+      <c r="L2283">
+        <v>433000</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:12">
+      <c r="A2284">
+        <v>2281</v>
+      </c>
+      <c r="B2284">
+        <v>626402</v>
+      </c>
+      <c r="C2284" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2284" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2284" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2284" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2284" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2284" t="s">
+        <v>2198</v>
+      </c>
+      <c r="I2284" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2284">
+        <v>1</v>
+      </c>
+      <c r="K2284">
+        <v>4593900</v>
+      </c>
+      <c r="L2284">
+        <v>4593900</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:12">
+      <c r="A2285">
+        <v>2282</v>
+      </c>
+      <c r="B2285">
+        <v>626402</v>
+      </c>
+      <c r="C2285" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2285" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2285" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2285" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2285" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2285" t="s">
+        <v>600</v>
+      </c>
+      <c r="I2285" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2285">
+        <v>1</v>
+      </c>
+      <c r="K2285">
+        <v>12606100</v>
+      </c>
+      <c r="L2285">
+        <v>12606100</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:12">
+      <c r="A2286">
+        <v>2283</v>
+      </c>
+      <c r="B2286">
+        <v>626402</v>
+      </c>
+      <c r="C2286" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2286" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2286" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2286" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2286" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2286" t="s">
+        <v>601</v>
+      </c>
+      <c r="I2286" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2286">
+        <v>1</v>
+      </c>
+      <c r="K2286">
+        <v>12600100</v>
+      </c>
+      <c r="L2286">
+        <v>12600100</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:12">
+      <c r="A2287">
+        <v>2284</v>
+      </c>
+      <c r="B2287">
+        <v>626402</v>
+      </c>
+      <c r="C2287" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2287" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2287" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2287" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2287" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2287" t="s">
+        <v>2199</v>
+      </c>
+      <c r="I2287" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2287">
+        <v>1</v>
+      </c>
+      <c r="K2287">
+        <v>4939500</v>
+      </c>
+      <c r="L2287">
+        <v>4939500</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:12">
+      <c r="A2288">
+        <v>2285</v>
+      </c>
+      <c r="B2288">
+        <v>626402</v>
+      </c>
+      <c r="C2288" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2288" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2288" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2288" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2288" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2288" t="s">
+        <v>604</v>
+      </c>
+      <c r="I2288" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2288">
+        <v>1</v>
+      </c>
+      <c r="K2288">
+        <v>1101000</v>
+      </c>
+      <c r="L2288">
+        <v>1101000</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:12">
+      <c r="A2289">
+        <v>2286</v>
+      </c>
+      <c r="B2289">
+        <v>626402</v>
+      </c>
+      <c r="C2289" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2289" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2289" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2289" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2289" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2289" t="s">
+        <v>2316</v>
+      </c>
+      <c r="I2289" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2289">
+        <v>1</v>
+      </c>
+      <c r="K2289">
+        <v>300000</v>
+      </c>
+      <c r="L2289">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:12">
+      <c r="A2290">
+        <v>2287</v>
+      </c>
+      <c r="B2290">
+        <v>626402</v>
+      </c>
+      <c r="C2290" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2290" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2290" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2290" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2290" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2290" t="s">
+        <v>606</v>
+      </c>
+      <c r="I2290" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2290">
+        <v>1</v>
+      </c>
+      <c r="K2290">
+        <v>360000</v>
+      </c>
+      <c r="L2290">
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:12">
+      <c r="A2291">
+        <v>2288</v>
+      </c>
+      <c r="B2291">
+        <v>626402</v>
+      </c>
+      <c r="C2291" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2291" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2291" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2291" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2291" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2291" t="s">
+        <v>1424</v>
+      </c>
+      <c r="I2291" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2291">
+        <v>1</v>
+      </c>
+      <c r="K2291">
+        <v>1200000</v>
+      </c>
+      <c r="L2291">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:12">
+      <c r="A2292">
+        <v>2289</v>
+      </c>
+      <c r="B2292">
+        <v>626402</v>
+      </c>
+      <c r="C2292" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2292" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2292" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2292" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2292" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2292" t="s">
+        <v>1425</v>
+      </c>
+      <c r="I2292" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2292">
+        <v>1</v>
+      </c>
+      <c r="K2292">
+        <v>8641244</v>
+      </c>
+      <c r="L2292">
+        <v>8641244</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:12">
+      <c r="A2293">
+        <v>2290</v>
+      </c>
+      <c r="B2293">
+        <v>626402</v>
+      </c>
+      <c r="C2293" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2293" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2293" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2293" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2293" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2293" t="s">
+        <v>607</v>
+      </c>
+      <c r="I2293" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2293">
+        <v>1</v>
+      </c>
+      <c r="K2293">
+        <v>8683700</v>
+      </c>
+      <c r="L2293">
+        <v>8683700</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:12">
+      <c r="A2294">
+        <v>2291</v>
+      </c>
+      <c r="B2294">
+        <v>626402</v>
+      </c>
+      <c r="C2294" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2294" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2294" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2294" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2294" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2294" t="s">
+        <v>2379</v>
+      </c>
+      <c r="I2294" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2294">
+        <v>1</v>
+      </c>
+      <c r="K2294">
+        <v>2000000</v>
+      </c>
+      <c r="L2294">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:12">
+      <c r="A2295">
+        <v>2292</v>
+      </c>
+      <c r="B2295">
+        <v>626402</v>
+      </c>
+      <c r="C2295" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2295" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2295" t="s">
+        <v>2369</v>
+      </c>
+      <c r="F2295" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G2295" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H2295" t="s">
+        <v>2380</v>
+      </c>
+      <c r="I2295" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2295">
+        <v>1</v>
+      </c>
+      <c r="K2295">
+        <v>3150000</v>
+      </c>
+      <c r="L2295">
+        <v>3150000</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:12">
+      <c r="A2296">
+        <v>2293</v>
+      </c>
+      <c r="B2296">
+        <v>626402</v>
+      </c>
+      <c r="C2296" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2296" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2296" t="s">
+        <v>2381</v>
+      </c>
+      <c r="F2296" t="s">
+        <v>2382</v>
+      </c>
+      <c r="G2296" t="s">
+        <v>2383</v>
+      </c>
+      <c r="H2296" t="s">
+        <v>582</v>
+      </c>
+      <c r="I2296" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2296">
+        <v>1</v>
+      </c>
+      <c r="K2296">
+        <v>411700</v>
+      </c>
+      <c r="L2296">
+        <v>411700</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:12">
+      <c r="A2297">
+        <v>2294</v>
+      </c>
+      <c r="B2297">
+        <v>626402</v>
+      </c>
+      <c r="C2297" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2297" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2297" t="s">
+        <v>2384</v>
+      </c>
+      <c r="F2297" t="s">
+        <v>2385</v>
+      </c>
+      <c r="G2297" t="s">
+        <v>2386</v>
+      </c>
+      <c r="H2297" t="s">
+        <v>582</v>
+      </c>
+      <c r="I2297" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2297">
+        <v>1</v>
+      </c>
+      <c r="K2297">
+        <v>12135840</v>
+      </c>
+      <c r="L2297">
+        <v>12135840</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:12">
+      <c r="A2298">
+        <v>2295</v>
+      </c>
+      <c r="B2298">
+        <v>626402</v>
+      </c>
+      <c r="C2298" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2298" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2298" t="s">
+        <v>2387</v>
+      </c>
+      <c r="F2298" t="s">
+        <v>2388</v>
+      </c>
+      <c r="G2298" t="s">
+        <v>2360</v>
+      </c>
+      <c r="H2298" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2298" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2298">
+        <v>1</v>
+      </c>
+      <c r="K2298">
+        <v>29381900</v>
+      </c>
+      <c r="L2298">
+        <v>29381900</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:12">
+      <c r="A2299">
+        <v>2296</v>
+      </c>
+      <c r="B2299">
+        <v>626402</v>
+      </c>
+      <c r="C2299" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2299" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2299" t="s">
+        <v>2389</v>
+      </c>
+      <c r="F2299" t="s">
+        <v>2390</v>
+      </c>
+      <c r="G2299" t="s">
+        <v>2391</v>
+      </c>
+      <c r="H2299" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2299" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2299">
+        <v>1</v>
+      </c>
+      <c r="K2299">
+        <v>19037070</v>
+      </c>
+      <c r="L2299">
+        <v>19037070</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:12">
+      <c r="A2300">
+        <v>2297</v>
+      </c>
+      <c r="B2300">
+        <v>626402</v>
+      </c>
+      <c r="C2300" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2300" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2300" t="s">
+        <v>2392</v>
+      </c>
+      <c r="F2300" t="s">
+        <v>2393</v>
+      </c>
+      <c r="G2300" t="s">
+        <v>2394</v>
+      </c>
+      <c r="H2300" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2300" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2300">
+        <v>1</v>
+      </c>
+      <c r="K2300">
+        <v>33523689</v>
+      </c>
+      <c r="L2300">
+        <v>33523689</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:12">
+      <c r="A2301">
+        <v>2298</v>
+      </c>
+      <c r="B2301">
+        <v>626402</v>
+      </c>
+      <c r="C2301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2301" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2301" t="s">
+        <v>2395</v>
+      </c>
+      <c r="F2301" t="s">
+        <v>2396</v>
+      </c>
+      <c r="G2301" t="s">
+        <v>2397</v>
+      </c>
+      <c r="H2301" t="s">
+        <v>2046</v>
+      </c>
+      <c r="I2301" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2301">
+        <v>1</v>
+      </c>
+      <c r="K2301">
+        <v>68484100</v>
+      </c>
+      <c r="L2301">
+        <v>68484100</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:12">
+      <c r="A2302">
+        <v>2299</v>
+      </c>
+      <c r="B2302">
+        <v>626402</v>
+      </c>
+      <c r="C2302" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2302" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2302" t="s">
+        <v>2398</v>
+      </c>
+      <c r="F2302" t="s">
+        <v>2399</v>
+      </c>
+      <c r="G2302" t="s">
+        <v>2400</v>
+      </c>
+      <c r="H2302" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2302" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2302">
+        <v>1</v>
+      </c>
+      <c r="K2302">
+        <v>4720178</v>
+      </c>
+      <c r="L2302">
+        <v>4720178</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:12">
+      <c r="A2303">
+        <v>2300</v>
+      </c>
+      <c r="B2303">
+        <v>626402</v>
+      </c>
+      <c r="C2303" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2303" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2303" t="s">
+        <v>2401</v>
+      </c>
+      <c r="F2303" t="s">
+        <v>2402</v>
+      </c>
+      <c r="G2303" t="s">
+        <v>2360</v>
+      </c>
+      <c r="H2303" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2303" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2303">
+        <v>1</v>
+      </c>
+      <c r="K2303">
+        <v>31729000</v>
+      </c>
+      <c r="L2303">
+        <v>31729000</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:12">
+      <c r="A2304">
+        <v>2301</v>
+      </c>
+      <c r="B2304">
+        <v>626402</v>
+      </c>
+      <c r="C2304" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2304" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2304" t="s">
+        <v>2403</v>
+      </c>
+      <c r="F2304" t="s">
+        <v>2404</v>
+      </c>
+      <c r="G2304" t="s">
+        <v>2405</v>
+      </c>
+      <c r="H2304" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2304" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2304">
+        <v>1</v>
+      </c>
+      <c r="K2304">
+        <v>5449686</v>
+      </c>
+      <c r="L2304">
+        <v>5449686</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:12">
+      <c r="A2305">
+        <v>2302</v>
+      </c>
+      <c r="B2305">
+        <v>626402</v>
+      </c>
+      <c r="C2305" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2305" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2305" t="s">
+        <v>2406</v>
+      </c>
+      <c r="F2305" t="s">
+        <v>2407</v>
+      </c>
+      <c r="G2305" t="s">
+        <v>2408</v>
+      </c>
+      <c r="H2305" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2305" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2305">
+        <v>1</v>
+      </c>
+      <c r="K2305">
+        <v>3357000</v>
+      </c>
+      <c r="L2305">
+        <v>3357000</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:12">
+      <c r="A2306">
+        <v>2303</v>
+      </c>
+      <c r="B2306">
+        <v>626402</v>
+      </c>
+      <c r="C2306" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2306" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2306" t="s">
+        <v>2409</v>
+      </c>
+      <c r="F2306" t="s">
+        <v>2410</v>
+      </c>
+      <c r="G2306" t="s">
+        <v>2411</v>
+      </c>
+      <c r="H2306" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I2306" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2306">
+        <v>1</v>
+      </c>
+      <c r="K2306">
+        <v>973000</v>
+      </c>
+      <c r="L2306">
+        <v>973000</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:12">
+      <c r="A2307">
+        <v>2304</v>
+      </c>
+      <c r="B2307">
+        <v>626402</v>
+      </c>
+      <c r="C2307" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2307" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2307" t="s">
+        <v>2412</v>
+      </c>
+      <c r="F2307" t="s">
+        <v>2413</v>
+      </c>
+      <c r="G2307" t="s">
+        <v>2414</v>
+      </c>
+      <c r="H2307" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2307" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2307">
+        <v>1</v>
+      </c>
+      <c r="K2307">
+        <v>1440000</v>
+      </c>
+      <c r="L2307">
+        <v>1440000</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:12">
+      <c r="A2308">
+        <v>2305</v>
+      </c>
+      <c r="B2308">
+        <v>626402</v>
+      </c>
+      <c r="C2308" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2308" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2308" t="s">
+        <v>2415</v>
+      </c>
+      <c r="F2308" t="s">
+        <v>2416</v>
+      </c>
+      <c r="G2308" t="s">
+        <v>2417</v>
+      </c>
+      <c r="H2308" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2308" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2308">
+        <v>1</v>
+      </c>
+      <c r="K2308">
+        <v>11702552</v>
+      </c>
+      <c r="L2308">
+        <v>11702552</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:12">
+      <c r="A2309">
+        <v>2306</v>
+      </c>
+      <c r="B2309">
+        <v>626402</v>
+      </c>
+      <c r="C2309" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2309" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2309" t="s">
+        <v>2418</v>
+      </c>
+      <c r="F2309" t="s">
+        <v>2419</v>
+      </c>
+      <c r="G2309" t="s">
+        <v>2420</v>
+      </c>
+      <c r="H2309" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2309" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2309">
+        <v>1</v>
+      </c>
+      <c r="K2309">
+        <v>3173000</v>
+      </c>
+      <c r="L2309">
+        <v>3173000</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:12">
+      <c r="A2310">
+        <v>2307</v>
+      </c>
+      <c r="B2310">
+        <v>626402</v>
+      </c>
+      <c r="C2310" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2310" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2310" t="s">
+        <v>2421</v>
+      </c>
+      <c r="F2310" t="s">
+        <v>2422</v>
+      </c>
+      <c r="G2310" t="s">
+        <v>2423</v>
+      </c>
+      <c r="H2310" t="s">
+        <v>307</v>
+      </c>
+      <c r="I2310" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2310">
+        <v>1</v>
+      </c>
+      <c r="K2310">
+        <v>232687713</v>
+      </c>
+      <c r="L2310">
+        <v>232687713</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:12">
+      <c r="A2311">
+        <v>2308</v>
+      </c>
+      <c r="B2311">
+        <v>626402</v>
+      </c>
+      <c r="C2311" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2311" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2311" t="s">
+        <v>2424</v>
+      </c>
+      <c r="F2311" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G2311" t="s">
+        <v>2426</v>
+      </c>
+      <c r="H2311" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2311" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2311">
+        <v>1</v>
+      </c>
+      <c r="K2311">
+        <v>13297440</v>
+      </c>
+      <c r="L2311">
+        <v>13297440</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:12">
+      <c r="A2312">
+        <v>2309</v>
+      </c>
+      <c r="B2312">
+        <v>626402</v>
+      </c>
+      <c r="C2312" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2312" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2312" t="s">
+        <v>2427</v>
+      </c>
+      <c r="F2312" t="s">
+        <v>2428</v>
+      </c>
+      <c r="G2312" t="s">
+        <v>2429</v>
+      </c>
+      <c r="H2312" t="s">
+        <v>891</v>
+      </c>
+      <c r="I2312" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2312">
+        <v>1</v>
+      </c>
+      <c r="K2312">
+        <v>5751818</v>
+      </c>
+      <c r="L2312">
+        <v>5751818</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:12">
+      <c r="A2313">
+        <v>2310</v>
+      </c>
+      <c r="B2313">
+        <v>626402</v>
+      </c>
+      <c r="C2313" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2313" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2313" t="s">
+        <v>2430</v>
+      </c>
+      <c r="F2313" t="s">
+        <v>2431</v>
+      </c>
+      <c r="G2313" t="s">
+        <v>2432</v>
+      </c>
+      <c r="H2313" t="s">
+        <v>821</v>
+      </c>
+      <c r="I2313" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2313">
+        <v>1</v>
+      </c>
+      <c r="K2313">
+        <v>10700000</v>
+      </c>
+      <c r="L2313">
+        <v>10700000</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:12">
+      <c r="A2314">
+        <v>2311</v>
+      </c>
+      <c r="B2314">
+        <v>626402</v>
+      </c>
+      <c r="C2314" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2314" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2314" t="s">
+        <v>2433</v>
+      </c>
+      <c r="F2314" t="s">
+        <v>2434</v>
+      </c>
+      <c r="G2314" t="s">
+        <v>2435</v>
+      </c>
+      <c r="H2314" t="s">
+        <v>2436</v>
+      </c>
+      <c r="I2314" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2314">
+        <v>1</v>
+      </c>
+      <c r="K2314">
+        <v>30138750</v>
+      </c>
+      <c r="L2314">
+        <v>30138750</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:12">
+      <c r="A2315">
+        <v>2312</v>
+      </c>
+      <c r="B2315">
+        <v>626402</v>
+      </c>
+      <c r="C2315" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2315" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2315" t="s">
+        <v>2437</v>
+      </c>
+      <c r="F2315" t="s">
+        <v>2438</v>
+      </c>
+      <c r="G2315" t="s">
+        <v>2439</v>
+      </c>
+      <c r="H2315" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2315" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2315">
+        <v>1</v>
+      </c>
+      <c r="K2315">
+        <v>10000000</v>
+      </c>
+      <c r="L2315">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:12">
+      <c r="A2316">
+        <v>2313</v>
+      </c>
+      <c r="B2316">
+        <v>626402</v>
+      </c>
+      <c r="C2316" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2316" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2316" t="s">
+        <v>2440</v>
+      </c>
+      <c r="F2316" t="s">
+        <v>2441</v>
+      </c>
+      <c r="G2316" t="s">
+        <v>2442</v>
+      </c>
+      <c r="H2316" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2316" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2316">
+        <v>1</v>
+      </c>
+      <c r="K2316">
+        <v>17476860</v>
+      </c>
+      <c r="L2316">
+        <v>17476860</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:12">
+      <c r="A2317">
+        <v>2314</v>
+      </c>
+      <c r="B2317">
+        <v>626402</v>
+      </c>
+      <c r="C2317" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2317" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2317" t="s">
+        <v>2443</v>
+      </c>
+      <c r="F2317" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G2317" t="s">
+        <v>2445</v>
+      </c>
+      <c r="H2317" t="s">
+        <v>773</v>
+      </c>
+      <c r="I2317" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2317">
+        <v>1</v>
+      </c>
+      <c r="K2317">
+        <v>4200000</v>
+      </c>
+      <c r="L2317">
+        <v>4200000</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:12">
+      <c r="A2318">
+        <v>2315</v>
+      </c>
+      <c r="B2318">
+        <v>626402</v>
+      </c>
+      <c r="C2318" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2318" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2318" t="s">
+        <v>2446</v>
+      </c>
+      <c r="F2318" t="s">
+        <v>2447</v>
+      </c>
+      <c r="G2318" t="s">
+        <v>2448</v>
+      </c>
+      <c r="H2318" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2318" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2318">
+        <v>1</v>
+      </c>
+      <c r="K2318">
+        <v>3604739</v>
+      </c>
+      <c r="L2318">
+        <v>3604739</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:12">
+      <c r="A2319">
+        <v>2316</v>
+      </c>
+      <c r="B2319">
+        <v>626402</v>
+      </c>
+      <c r="C2319" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2319" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2319" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2319" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2319" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2319" t="s">
+        <v>2451</v>
+      </c>
+      <c r="I2319" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2319">
+        <v>1</v>
+      </c>
+      <c r="K2319">
+        <v>255000</v>
+      </c>
+      <c r="L2319">
+        <v>255000</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:12">
+      <c r="A2320">
+        <v>2317</v>
+      </c>
+      <c r="B2320">
+        <v>626402</v>
+      </c>
+      <c r="C2320" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2320" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2320" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2320" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2320" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2320" t="s">
+        <v>2452</v>
+      </c>
+      <c r="I2320" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2320">
+        <v>1</v>
+      </c>
+      <c r="K2320">
+        <v>10800000</v>
+      </c>
+      <c r="L2320">
+        <v>10800000</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:12">
+      <c r="A2321">
+        <v>2318</v>
+      </c>
+      <c r="B2321">
+        <v>626402</v>
+      </c>
+      <c r="C2321" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2321" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2321" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2321" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2321" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2321" t="s">
+        <v>2453</v>
+      </c>
+      <c r="I2321" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2321">
+        <v>1</v>
+      </c>
+      <c r="K2321">
+        <v>1180000</v>
+      </c>
+      <c r="L2321">
+        <v>1180000</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:12">
+      <c r="A2322">
+        <v>2319</v>
+      </c>
+      <c r="B2322">
+        <v>626402</v>
+      </c>
+      <c r="C2322" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2322" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2322" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2322" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2322" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2322" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2322" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2322">
+        <v>1</v>
+      </c>
+      <c r="K2322">
+        <v>1320500</v>
+      </c>
+      <c r="L2322">
+        <v>1320500</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:12">
+      <c r="A2323">
+        <v>2320</v>
+      </c>
+      <c r="B2323">
+        <v>626402</v>
+      </c>
+      <c r="C2323" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2323" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2323" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2323" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2323" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2323" t="s">
+        <v>768</v>
+      </c>
+      <c r="I2323" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2323">
+        <v>1</v>
+      </c>
+      <c r="K2323">
+        <v>36058480</v>
+      </c>
+      <c r="L2323">
+        <v>36058480</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:12">
+      <c r="A2324">
+        <v>2321</v>
+      </c>
+      <c r="B2324">
+        <v>626402</v>
+      </c>
+      <c r="C2324" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2324" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2324" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2324" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2324" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2324" t="s">
+        <v>731</v>
+      </c>
+      <c r="I2324" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2324">
+        <v>1</v>
+      </c>
+      <c r="K2324">
+        <v>33674620</v>
+      </c>
+      <c r="L2324">
+        <v>33674620</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:12">
+      <c r="A2325">
+        <v>2322</v>
+      </c>
+      <c r="B2325">
+        <v>626402</v>
+      </c>
+      <c r="C2325" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2325" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2325" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2325" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2325" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2325" t="s">
+        <v>1546</v>
+      </c>
+      <c r="I2325" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2325">
+        <v>1</v>
+      </c>
+      <c r="K2325">
+        <v>17716440</v>
+      </c>
+      <c r="L2325">
+        <v>17716440</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:12">
+      <c r="A2326">
+        <v>2323</v>
+      </c>
+      <c r="B2326">
+        <v>626402</v>
+      </c>
+      <c r="C2326" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2326" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2326" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2326" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2326" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2326" t="s">
+        <v>909</v>
+      </c>
+      <c r="I2326" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2326">
+        <v>1</v>
+      </c>
+      <c r="K2326">
+        <v>6885000</v>
+      </c>
+      <c r="L2326">
+        <v>6885000</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:12">
+      <c r="A2327">
+        <v>2324</v>
+      </c>
+      <c r="B2327">
+        <v>626402</v>
+      </c>
+      <c r="C2327" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2327" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2327" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2327" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2327" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2327" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2327" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2327">
+        <v>1</v>
+      </c>
+      <c r="K2327">
+        <v>5656000</v>
+      </c>
+      <c r="L2327">
+        <v>5656000</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:12">
+      <c r="A2328">
+        <v>2325</v>
+      </c>
+      <c r="B2328">
+        <v>626402</v>
+      </c>
+      <c r="C2328" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2328" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2328" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2328" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2328" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2328" t="s">
+        <v>2454</v>
+      </c>
+      <c r="I2328" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2328">
+        <v>1</v>
+      </c>
+      <c r="K2328">
+        <v>16279457</v>
+      </c>
+      <c r="L2328">
+        <v>16279457</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:12">
+      <c r="A2329">
+        <v>2326</v>
+      </c>
+      <c r="B2329">
+        <v>626402</v>
+      </c>
+      <c r="C2329" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2329" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2329" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2329" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2329" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2329" t="s">
+        <v>586</v>
+      </c>
+      <c r="I2329" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2329">
+        <v>1</v>
+      </c>
+      <c r="K2329">
+        <v>300000</v>
+      </c>
+      <c r="L2329">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:12">
+      <c r="A2330">
+        <v>2327</v>
+      </c>
+      <c r="B2330">
+        <v>626402</v>
+      </c>
+      <c r="C2330" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2330" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2330" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2330" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2330" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2330" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2330" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2330">
+        <v>1</v>
+      </c>
+      <c r="K2330">
+        <v>2932200</v>
+      </c>
+      <c r="L2330">
+        <v>2932200</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:12">
+      <c r="A2331">
+        <v>2328</v>
+      </c>
+      <c r="B2331">
+        <v>626402</v>
+      </c>
+      <c r="C2331" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2331" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2331" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2331" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2331" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2331" t="s">
+        <v>910</v>
+      </c>
+      <c r="I2331" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2331">
+        <v>1</v>
+      </c>
+      <c r="K2331">
+        <v>12652560</v>
+      </c>
+      <c r="L2331">
+        <v>12652560</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:12">
+      <c r="A2332">
+        <v>2329</v>
+      </c>
+      <c r="B2332">
+        <v>626402</v>
+      </c>
+      <c r="C2332" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2332" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2332" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2332" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2332" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2332" t="s">
+        <v>2148</v>
+      </c>
+      <c r="I2332" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2332">
+        <v>1</v>
+      </c>
+      <c r="K2332">
+        <v>12052500</v>
+      </c>
+      <c r="L2332">
+        <v>12052500</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:12">
+      <c r="A2333">
+        <v>2330</v>
+      </c>
+      <c r="B2333">
+        <v>626402</v>
+      </c>
+      <c r="C2333" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2333" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2333" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2333" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2333" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2333" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2333" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2333">
+        <v>1</v>
+      </c>
+      <c r="K2333">
+        <v>9697035</v>
+      </c>
+      <c r="L2333">
+        <v>9697035</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:12">
+      <c r="A2334">
+        <v>2331</v>
+      </c>
+      <c r="B2334">
+        <v>626402</v>
+      </c>
+      <c r="C2334" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2334" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2334" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2334" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2334" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2334" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2334" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2334">
+        <v>1</v>
+      </c>
+      <c r="K2334">
+        <v>130000</v>
+      </c>
+      <c r="L2334">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:12">
+      <c r="A2335">
+        <v>2332</v>
+      </c>
+      <c r="B2335">
+        <v>626402</v>
+      </c>
+      <c r="C2335" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2335" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2335" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2335" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2335" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2335" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2335" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2335">
+        <v>1</v>
+      </c>
+      <c r="K2335">
+        <v>300000</v>
+      </c>
+      <c r="L2335">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:12">
+      <c r="A2336">
+        <v>2333</v>
+      </c>
+      <c r="B2336">
+        <v>626402</v>
+      </c>
+      <c r="C2336" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2336" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2336" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2336" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2336" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2336" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2336" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2336">
+        <v>1</v>
+      </c>
+      <c r="K2336">
+        <v>750000</v>
+      </c>
+      <c r="L2336">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:12">
+      <c r="A2337">
+        <v>2334</v>
+      </c>
+      <c r="B2337">
+        <v>626402</v>
+      </c>
+      <c r="C2337" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2337" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2337" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2337" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2337" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2337" t="s">
+        <v>911</v>
+      </c>
+      <c r="I2337" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2337">
+        <v>1</v>
+      </c>
+      <c r="K2337">
+        <v>1350000</v>
+      </c>
+      <c r="L2337">
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:12">
+      <c r="A2338">
+        <v>2335</v>
+      </c>
+      <c r="B2338">
+        <v>626402</v>
+      </c>
+      <c r="C2338" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2338" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2338" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2338" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2338" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2338" t="s">
+        <v>193</v>
+      </c>
+      <c r="I2338" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2338">
+        <v>1</v>
+      </c>
+      <c r="K2338">
+        <v>840000</v>
+      </c>
+      <c r="L2338">
+        <v>840000</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:12">
+      <c r="A2339">
+        <v>2336</v>
+      </c>
+      <c r="B2339">
+        <v>626402</v>
+      </c>
+      <c r="C2339" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2339" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2339" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F2339" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G2339" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2339" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2339" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2339">
+        <v>1</v>
+      </c>
+      <c r="K2339">
+        <v>1200000</v>
+      </c>
+      <c r="L2339">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:12">
+      <c r="A2340">
+        <v>2337</v>
+      </c>
+      <c r="B2340">
+        <v>626402</v>
+      </c>
+      <c r="C2340" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2340" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2340" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2340" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2340" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2340" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2340" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2340">
+        <v>1</v>
+      </c>
+      <c r="K2340">
+        <v>9022500</v>
+      </c>
+      <c r="L2340">
+        <v>9022500</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:12">
+      <c r="A2341">
+        <v>2338</v>
+      </c>
+      <c r="B2341">
+        <v>626402</v>
+      </c>
+      <c r="C2341" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2341" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2341" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2341" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2341" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2341" t="s">
+        <v>2457</v>
+      </c>
+      <c r="I2341" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2341">
+        <v>1</v>
+      </c>
+      <c r="K2341">
+        <v>20620280</v>
+      </c>
+      <c r="L2341">
+        <v>20620280</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:12">
+      <c r="A2342">
+        <v>2339</v>
+      </c>
+      <c r="B2342">
+        <v>626402</v>
+      </c>
+      <c r="C2342" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2342" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2342" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2342" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2342" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2342" t="s">
+        <v>582</v>
+      </c>
+      <c r="I2342" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2342">
+        <v>1</v>
+      </c>
+      <c r="K2342">
+        <v>19639260</v>
+      </c>
+      <c r="L2342">
+        <v>19639260</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:12">
+      <c r="A2343">
+        <v>2340</v>
+      </c>
+      <c r="B2343">
+        <v>626402</v>
+      </c>
+      <c r="C2343" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2343" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2343" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2343" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2343" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2343" t="s">
+        <v>584</v>
+      </c>
+      <c r="I2343" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2343">
+        <v>1</v>
+      </c>
+      <c r="K2343">
+        <v>3226000</v>
+      </c>
+      <c r="L2343">
+        <v>3226000</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:12">
+      <c r="A2344">
+        <v>2341</v>
+      </c>
+      <c r="B2344">
+        <v>626402</v>
+      </c>
+      <c r="C2344" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2344" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2344" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2344" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2344" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2344" t="s">
+        <v>729</v>
+      </c>
+      <c r="I2344" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2344">
+        <v>1</v>
+      </c>
+      <c r="K2344">
+        <v>785000</v>
+      </c>
+      <c r="L2344">
+        <v>785000</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:12">
+      <c r="A2345">
+        <v>2342</v>
+      </c>
+      <c r="B2345">
+        <v>626402</v>
+      </c>
+      <c r="C2345" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2345" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2345" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2345" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2345" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2345" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I2345" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2345">
+        <v>1</v>
+      </c>
+      <c r="K2345">
+        <v>8544680</v>
+      </c>
+      <c r="L2345">
+        <v>8544680</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:12">
+      <c r="A2346">
+        <v>2343</v>
+      </c>
+      <c r="B2346">
+        <v>626402</v>
+      </c>
+      <c r="C2346" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2346" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2346" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2346" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2346" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2346" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2346" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2346">
+        <v>1</v>
+      </c>
+      <c r="K2346">
+        <v>42630220</v>
+      </c>
+      <c r="L2346">
+        <v>42630220</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:12">
+      <c r="A2347">
+        <v>2344</v>
+      </c>
+      <c r="B2347">
+        <v>626402</v>
+      </c>
+      <c r="C2347" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2347" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2347" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2347" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2347" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2347" t="s">
+        <v>763</v>
+      </c>
+      <c r="I2347" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2347">
+        <v>1</v>
+      </c>
+      <c r="K2347">
+        <v>4224000</v>
+      </c>
+      <c r="L2347">
+        <v>4224000</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:12">
+      <c r="A2348">
+        <v>2345</v>
+      </c>
+      <c r="B2348">
+        <v>626402</v>
+      </c>
+      <c r="C2348" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2348" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2348" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2348" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2348" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2348" t="s">
+        <v>816</v>
+      </c>
+      <c r="I2348" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2348">
+        <v>1</v>
+      </c>
+      <c r="K2348">
+        <v>8472080</v>
+      </c>
+      <c r="L2348">
+        <v>8472080</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:12">
+      <c r="A2349">
+        <v>2346</v>
+      </c>
+      <c r="B2349">
+        <v>626402</v>
+      </c>
+      <c r="C2349" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2349" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2349" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2349" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2349" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2349" t="s">
+        <v>1356</v>
+      </c>
+      <c r="I2349" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2349">
+        <v>1</v>
+      </c>
+      <c r="K2349">
+        <v>6474200</v>
+      </c>
+      <c r="L2349">
+        <v>6474200</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:12">
+      <c r="A2350">
+        <v>2347</v>
+      </c>
+      <c r="B2350">
+        <v>626402</v>
+      </c>
+      <c r="C2350" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2350" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2350" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2350" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2350" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2350" t="s">
+        <v>1564</v>
+      </c>
+      <c r="I2350" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2350">
+        <v>1</v>
+      </c>
+      <c r="K2350">
+        <v>11063599</v>
+      </c>
+      <c r="L2350">
+        <v>11063599</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:12">
+      <c r="A2351">
+        <v>2348</v>
+      </c>
+      <c r="B2351">
+        <v>626402</v>
+      </c>
+      <c r="C2351" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2351" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2351" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2351" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2351" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2351" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I2351" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2351">
+        <v>1</v>
+      </c>
+      <c r="K2351">
+        <v>1656920</v>
+      </c>
+      <c r="L2351">
+        <v>1656920</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:12">
+      <c r="A2352">
         <v>2349</v>
       </c>
-      <c r="G2258" t="s">
+      <c r="B2352">
+        <v>626402</v>
+      </c>
+      <c r="C2352" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2352" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2352" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2352" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2352" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2352" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2352" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2352">
+        <v>1</v>
+      </c>
+      <c r="K2352">
+        <v>2411600</v>
+      </c>
+      <c r="L2352">
+        <v>2411600</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:12">
+      <c r="A2353">
         <v>2350</v>
       </c>
-      <c r="H2258" t="s">
-        <v>299</v>
-      </c>
-      <c r="I2258" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2258">
-        <v>1</v>
-      </c>
-      <c r="K2258">
-        <v>204638726</v>
-      </c>
-      <c r="L2258">
-        <v>204638726</v>
+      <c r="B2353">
+        <v>626402</v>
+      </c>
+      <c r="C2353" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2353" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2353" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2353" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2353" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2353" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2353" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2353">
+        <v>1</v>
+      </c>
+      <c r="K2353">
+        <v>27447287</v>
+      </c>
+      <c r="L2353">
+        <v>27447287</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:12">
+      <c r="A2354">
+        <v>2351</v>
+      </c>
+      <c r="B2354">
+        <v>626402</v>
+      </c>
+      <c r="C2354" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2354" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2354" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2354" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2354" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2354" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2354" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2354">
+        <v>1</v>
+      </c>
+      <c r="K2354">
+        <v>24556740</v>
+      </c>
+      <c r="L2354">
+        <v>24556740</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:12">
+      <c r="A2355">
+        <v>2352</v>
+      </c>
+      <c r="B2355">
+        <v>626402</v>
+      </c>
+      <c r="C2355" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2355" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2355" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2355" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2355" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2355" t="s">
+        <v>769</v>
+      </c>
+      <c r="I2355" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2355">
+        <v>1</v>
+      </c>
+      <c r="K2355">
+        <v>650000</v>
+      </c>
+      <c r="L2355">
+        <v>650000</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:12">
+      <c r="A2356">
+        <v>2353</v>
+      </c>
+      <c r="B2356">
+        <v>626402</v>
+      </c>
+      <c r="C2356" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2356" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2356" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2356" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2356" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2356" t="s">
+        <v>770</v>
+      </c>
+      <c r="I2356" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2356">
+        <v>1</v>
+      </c>
+      <c r="K2356">
+        <v>600000</v>
+      </c>
+      <c r="L2356">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:12">
+      <c r="A2357">
+        <v>2354</v>
+      </c>
+      <c r="B2357">
+        <v>626402</v>
+      </c>
+      <c r="C2357" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2357" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2357" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2357" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2357" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2357" t="s">
+        <v>400</v>
+      </c>
+      <c r="I2357" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2357">
+        <v>1</v>
+      </c>
+      <c r="K2357">
+        <v>2700000</v>
+      </c>
+      <c r="L2357">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:12">
+      <c r="A2358">
+        <v>2355</v>
+      </c>
+      <c r="B2358">
+        <v>626402</v>
+      </c>
+      <c r="C2358" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2358" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2358" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2358" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2358" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2358" t="s">
+        <v>401</v>
+      </c>
+      <c r="I2358" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2358">
+        <v>1</v>
+      </c>
+      <c r="K2358">
+        <v>1430000</v>
+      </c>
+      <c r="L2358">
+        <v>1430000</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:12">
+      <c r="A2359">
+        <v>2356</v>
+      </c>
+      <c r="B2359">
+        <v>626402</v>
+      </c>
+      <c r="C2359" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2359" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2359" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F2359" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G2359" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2359" t="s">
+        <v>773</v>
+      </c>
+      <c r="I2359" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2359">
+        <v>1</v>
+      </c>
+      <c r="K2359">
+        <v>150000</v>
+      </c>
+      <c r="L2359">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 16 juni 2023 tapi blm sama GUP8
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2490">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -7280,6 +7280,18 @@
     <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:B.2290/BRSDM.1/KP.440/V/2023 Tanggal 4 Mei 2023</t>
   </si>
   <si>
+    <t>2023-06-13</t>
+  </si>
+  <si>
+    <t>'00552T</t>
+  </si>
+  <si>
+    <t>'231751303013631</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.823/BRSDM.5/KP.440/V/2023.Tanggal 15 Mei 2023.</t>
+  </si>
+  <si>
     <t>'00553T</t>
   </si>
   <si>
@@ -7389,6 +7401,90 @@
   </si>
   <si>
     <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.0B.000204</t>
+  </si>
+  <si>
+    <t>'00564T</t>
+  </si>
+  <si>
+    <t>'231751701003393</t>
+  </si>
+  <si>
+    <t>Pertanggungjawaban Tambahan Uang Persediaan untuk Keperluan Belanja Barang.</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000890</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.102.0C.001215</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.102.0C.001216</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001403</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001404</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001405</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001407</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001409</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001410</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001411</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001412</t>
+  </si>
+  <si>
+    <t>'626402.175.521213.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.963.102.0A.001413</t>
+  </si>
+  <si>
+    <t>'626402.175.521241.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000896</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.102.0C.001222</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.102.0C.001223</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.102.0A.000814</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0C.000878</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0A.000852</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.103.0B.000838</t>
+  </si>
+  <si>
+    <t>'00568T</t>
+  </si>
+  <si>
+    <t>'231751701003394</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0A.000844</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0B.000859</t>
+  </si>
+  <si>
+    <t>'626402.175.521241.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000897</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0B.000865</t>
   </si>
 </sst>
 </file>
@@ -7730,7 +7826,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2359"/>
+  <dimension ref="A1:L2428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -95423,19 +95519,19 @@
         <v>13</v>
       </c>
       <c r="D2310" t="s">
-        <v>2249</v>
+        <v>2421</v>
       </c>
       <c r="E2310" t="s">
-        <v>2421</v>
+        <v>2422</v>
       </c>
       <c r="F2310" t="s">
-        <v>2422</v>
+        <v>2423</v>
       </c>
       <c r="G2310" t="s">
-        <v>2423</v>
+        <v>2424</v>
       </c>
       <c r="H2310" t="s">
-        <v>307</v>
+        <v>140</v>
       </c>
       <c r="I2310" t="s">
         <v>19</v>
@@ -95444,10 +95540,10 @@
         <v>1</v>
       </c>
       <c r="K2310">
-        <v>232687713</v>
+        <v>8203880</v>
       </c>
       <c r="L2310">
-        <v>232687713</v>
+        <v>8203880</v>
       </c>
     </row>
     <row r="2311" spans="1:12">
@@ -95461,19 +95557,19 @@
         <v>13</v>
       </c>
       <c r="D2311" t="s">
-        <v>2348</v>
+        <v>2249</v>
       </c>
       <c r="E2311" t="s">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="F2311" t="s">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="G2311" t="s">
-        <v>2426</v>
+        <v>2427</v>
       </c>
       <c r="H2311" t="s">
-        <v>140</v>
+        <v>307</v>
       </c>
       <c r="I2311" t="s">
         <v>19</v>
@@ -95482,10 +95578,10 @@
         <v>1</v>
       </c>
       <c r="K2311">
-        <v>13297440</v>
+        <v>232687713</v>
       </c>
       <c r="L2311">
-        <v>13297440</v>
+        <v>232687713</v>
       </c>
     </row>
     <row r="2312" spans="1:12">
@@ -95502,16 +95598,16 @@
         <v>2348</v>
       </c>
       <c r="E2312" t="s">
-        <v>2427</v>
+        <v>2428</v>
       </c>
       <c r="F2312" t="s">
-        <v>2428</v>
+        <v>2429</v>
       </c>
       <c r="G2312" t="s">
-        <v>2429</v>
+        <v>2430</v>
       </c>
       <c r="H2312" t="s">
-        <v>891</v>
+        <v>140</v>
       </c>
       <c r="I2312" t="s">
         <v>19</v>
@@ -95520,10 +95616,10 @@
         <v>1</v>
       </c>
       <c r="K2312">
-        <v>5751818</v>
+        <v>13297440</v>
       </c>
       <c r="L2312">
-        <v>5751818</v>
+        <v>13297440</v>
       </c>
     </row>
     <row r="2313" spans="1:12">
@@ -95540,16 +95636,16 @@
         <v>2348</v>
       </c>
       <c r="E2313" t="s">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="F2313" t="s">
-        <v>2431</v>
+        <v>2432</v>
       </c>
       <c r="G2313" t="s">
-        <v>2432</v>
+        <v>2433</v>
       </c>
       <c r="H2313" t="s">
-        <v>821</v>
+        <v>891</v>
       </c>
       <c r="I2313" t="s">
         <v>19</v>
@@ -95558,10 +95654,10 @@
         <v>1</v>
       </c>
       <c r="K2313">
-        <v>10700000</v>
+        <v>5751818</v>
       </c>
       <c r="L2313">
-        <v>10700000</v>
+        <v>5751818</v>
       </c>
     </row>
     <row r="2314" spans="1:12">
@@ -95578,16 +95674,16 @@
         <v>2348</v>
       </c>
       <c r="E2314" t="s">
-        <v>2433</v>
+        <v>2434</v>
       </c>
       <c r="F2314" t="s">
-        <v>2434</v>
+        <v>2435</v>
       </c>
       <c r="G2314" t="s">
-        <v>2435</v>
+        <v>2436</v>
       </c>
       <c r="H2314" t="s">
-        <v>2436</v>
+        <v>821</v>
       </c>
       <c r="I2314" t="s">
         <v>19</v>
@@ -95596,10 +95692,10 @@
         <v>1</v>
       </c>
       <c r="K2314">
-        <v>30138750</v>
+        <v>10700000</v>
       </c>
       <c r="L2314">
-        <v>30138750</v>
+        <v>10700000</v>
       </c>
     </row>
     <row r="2315" spans="1:12">
@@ -95625,7 +95721,7 @@
         <v>2439</v>
       </c>
       <c r="H2315" t="s">
-        <v>157</v>
+        <v>2440</v>
       </c>
       <c r="I2315" t="s">
         <v>19</v>
@@ -95634,10 +95730,10 @@
         <v>1</v>
       </c>
       <c r="K2315">
-        <v>10000000</v>
+        <v>30138750</v>
       </c>
       <c r="L2315">
-        <v>10000000</v>
+        <v>30138750</v>
       </c>
     </row>
     <row r="2316" spans="1:12">
@@ -95654,16 +95750,16 @@
         <v>2348</v>
       </c>
       <c r="E2316" t="s">
-        <v>2440</v>
+        <v>2441</v>
       </c>
       <c r="F2316" t="s">
-        <v>2441</v>
+        <v>2442</v>
       </c>
       <c r="G2316" t="s">
-        <v>2442</v>
+        <v>2443</v>
       </c>
       <c r="H2316" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="I2316" t="s">
         <v>19</v>
@@ -95672,10 +95768,10 @@
         <v>1</v>
       </c>
       <c r="K2316">
-        <v>17476860</v>
+        <v>10000000</v>
       </c>
       <c r="L2316">
-        <v>17476860</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="2317" spans="1:12">
@@ -95692,16 +95788,16 @@
         <v>2348</v>
       </c>
       <c r="E2317" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="F2317" t="s">
-        <v>2444</v>
+        <v>2445</v>
       </c>
       <c r="G2317" t="s">
-        <v>2445</v>
+        <v>2446</v>
       </c>
       <c r="H2317" t="s">
-        <v>773</v>
+        <v>112</v>
       </c>
       <c r="I2317" t="s">
         <v>19</v>
@@ -95710,10 +95806,10 @@
         <v>1</v>
       </c>
       <c r="K2317">
-        <v>4200000</v>
+        <v>17476860</v>
       </c>
       <c r="L2317">
-        <v>4200000</v>
+        <v>17476860</v>
       </c>
     </row>
     <row r="2318" spans="1:12">
@@ -95730,16 +95826,16 @@
         <v>2348</v>
       </c>
       <c r="E2318" t="s">
-        <v>2446</v>
+        <v>2447</v>
       </c>
       <c r="F2318" t="s">
-        <v>2447</v>
+        <v>2448</v>
       </c>
       <c r="G2318" t="s">
-        <v>2448</v>
+        <v>2449</v>
       </c>
       <c r="H2318" t="s">
-        <v>102</v>
+        <v>773</v>
       </c>
       <c r="I2318" t="s">
         <v>19</v>
@@ -95748,10 +95844,10 @@
         <v>1</v>
       </c>
       <c r="K2318">
-        <v>3604739</v>
+        <v>4200000</v>
       </c>
       <c r="L2318">
-        <v>3604739</v>
+        <v>4200000</v>
       </c>
     </row>
     <row r="2319" spans="1:12">
@@ -95765,19 +95861,19 @@
         <v>13</v>
       </c>
       <c r="D2319" t="s">
-        <v>2249</v>
+        <v>2348</v>
       </c>
       <c r="E2319" t="s">
-        <v>2449</v>
+        <v>2450</v>
       </c>
       <c r="F2319" t="s">
-        <v>2450</v>
+        <v>2451</v>
       </c>
       <c r="G2319" t="s">
-        <v>1536</v>
+        <v>2452</v>
       </c>
       <c r="H2319" t="s">
-        <v>2451</v>
+        <v>102</v>
       </c>
       <c r="I2319" t="s">
         <v>19</v>
@@ -95786,10 +95882,10 @@
         <v>1</v>
       </c>
       <c r="K2319">
-        <v>255000</v>
+        <v>3604739</v>
       </c>
       <c r="L2319">
-        <v>255000</v>
+        <v>3604739</v>
       </c>
     </row>
     <row r="2320" spans="1:12">
@@ -95806,16 +95902,16 @@
         <v>2249</v>
       </c>
       <c r="E2320" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2320" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2320" t="s">
         <v>1536</v>
       </c>
       <c r="H2320" t="s">
-        <v>2452</v>
+        <v>2455</v>
       </c>
       <c r="I2320" t="s">
         <v>19</v>
@@ -95824,10 +95920,10 @@
         <v>1</v>
       </c>
       <c r="K2320">
-        <v>10800000</v>
+        <v>255000</v>
       </c>
       <c r="L2320">
-        <v>10800000</v>
+        <v>255000</v>
       </c>
     </row>
     <row r="2321" spans="1:12">
@@ -95844,16 +95940,16 @@
         <v>2249</v>
       </c>
       <c r="E2321" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2321" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2321" t="s">
         <v>1536</v>
       </c>
       <c r="H2321" t="s">
-        <v>2453</v>
+        <v>2456</v>
       </c>
       <c r="I2321" t="s">
         <v>19</v>
@@ -95862,10 +95958,10 @@
         <v>1</v>
       </c>
       <c r="K2321">
-        <v>1180000</v>
+        <v>10800000</v>
       </c>
       <c r="L2321">
-        <v>1180000</v>
+        <v>10800000</v>
       </c>
     </row>
     <row r="2322" spans="1:12">
@@ -95882,16 +95978,16 @@
         <v>2249</v>
       </c>
       <c r="E2322" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2322" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2322" t="s">
         <v>1536</v>
       </c>
       <c r="H2322" t="s">
-        <v>102</v>
+        <v>2457</v>
       </c>
       <c r="I2322" t="s">
         <v>19</v>
@@ -95900,10 +95996,10 @@
         <v>1</v>
       </c>
       <c r="K2322">
-        <v>1320500</v>
+        <v>1180000</v>
       </c>
       <c r="L2322">
-        <v>1320500</v>
+        <v>1180000</v>
       </c>
     </row>
     <row r="2323" spans="1:12">
@@ -95920,16 +96016,16 @@
         <v>2249</v>
       </c>
       <c r="E2323" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2323" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2323" t="s">
         <v>1536</v>
       </c>
       <c r="H2323" t="s">
-        <v>768</v>
+        <v>102</v>
       </c>
       <c r="I2323" t="s">
         <v>19</v>
@@ -95938,10 +96034,10 @@
         <v>1</v>
       </c>
       <c r="K2323">
-        <v>36058480</v>
+        <v>1320500</v>
       </c>
       <c r="L2323">
-        <v>36058480</v>
+        <v>1320500</v>
       </c>
     </row>
     <row r="2324" spans="1:12">
@@ -95958,16 +96054,16 @@
         <v>2249</v>
       </c>
       <c r="E2324" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2324" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2324" t="s">
         <v>1536</v>
       </c>
       <c r="H2324" t="s">
-        <v>731</v>
+        <v>768</v>
       </c>
       <c r="I2324" t="s">
         <v>19</v>
@@ -95976,10 +96072,10 @@
         <v>1</v>
       </c>
       <c r="K2324">
-        <v>33674620</v>
+        <v>36058480</v>
       </c>
       <c r="L2324">
-        <v>33674620</v>
+        <v>36058480</v>
       </c>
     </row>
     <row r="2325" spans="1:12">
@@ -95996,16 +96092,16 @@
         <v>2249</v>
       </c>
       <c r="E2325" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2325" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2325" t="s">
         <v>1536</v>
       </c>
       <c r="H2325" t="s">
-        <v>1546</v>
+        <v>731</v>
       </c>
       <c r="I2325" t="s">
         <v>19</v>
@@ -96014,10 +96110,10 @@
         <v>1</v>
       </c>
       <c r="K2325">
-        <v>17716440</v>
+        <v>33674620</v>
       </c>
       <c r="L2325">
-        <v>17716440</v>
+        <v>33674620</v>
       </c>
     </row>
     <row r="2326" spans="1:12">
@@ -96034,16 +96130,16 @@
         <v>2249</v>
       </c>
       <c r="E2326" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2326" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2326" t="s">
         <v>1536</v>
       </c>
       <c r="H2326" t="s">
-        <v>909</v>
+        <v>1546</v>
       </c>
       <c r="I2326" t="s">
         <v>19</v>
@@ -96052,10 +96148,10 @@
         <v>1</v>
       </c>
       <c r="K2326">
-        <v>6885000</v>
+        <v>17716440</v>
       </c>
       <c r="L2326">
-        <v>6885000</v>
+        <v>17716440</v>
       </c>
     </row>
     <row r="2327" spans="1:12">
@@ -96072,16 +96168,16 @@
         <v>2249</v>
       </c>
       <c r="E2327" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2327" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2327" t="s">
         <v>1536</v>
       </c>
       <c r="H2327" t="s">
-        <v>149</v>
+        <v>909</v>
       </c>
       <c r="I2327" t="s">
         <v>19</v>
@@ -96090,10 +96186,10 @@
         <v>1</v>
       </c>
       <c r="K2327">
-        <v>5656000</v>
+        <v>6885000</v>
       </c>
       <c r="L2327">
-        <v>5656000</v>
+        <v>6885000</v>
       </c>
     </row>
     <row r="2328" spans="1:12">
@@ -96110,16 +96206,16 @@
         <v>2249</v>
       </c>
       <c r="E2328" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2328" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2328" t="s">
         <v>1536</v>
       </c>
       <c r="H2328" t="s">
-        <v>2454</v>
+        <v>149</v>
       </c>
       <c r="I2328" t="s">
         <v>19</v>
@@ -96128,10 +96224,10 @@
         <v>1</v>
       </c>
       <c r="K2328">
-        <v>16279457</v>
+        <v>5656000</v>
       </c>
       <c r="L2328">
-        <v>16279457</v>
+        <v>5656000</v>
       </c>
     </row>
     <row r="2329" spans="1:12">
@@ -96148,16 +96244,16 @@
         <v>2249</v>
       </c>
       <c r="E2329" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2329" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2329" t="s">
         <v>1536</v>
       </c>
       <c r="H2329" t="s">
-        <v>586</v>
+        <v>2458</v>
       </c>
       <c r="I2329" t="s">
         <v>19</v>
@@ -96166,10 +96262,10 @@
         <v>1</v>
       </c>
       <c r="K2329">
-        <v>300000</v>
+        <v>16279457</v>
       </c>
       <c r="L2329">
-        <v>300000</v>
+        <v>16279457</v>
       </c>
     </row>
     <row r="2330" spans="1:12">
@@ -96186,16 +96282,16 @@
         <v>2249</v>
       </c>
       <c r="E2330" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2330" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2330" t="s">
         <v>1536</v>
       </c>
       <c r="H2330" t="s">
-        <v>95</v>
+        <v>586</v>
       </c>
       <c r="I2330" t="s">
         <v>19</v>
@@ -96204,10 +96300,10 @@
         <v>1</v>
       </c>
       <c r="K2330">
-        <v>2932200</v>
+        <v>300000</v>
       </c>
       <c r="L2330">
-        <v>2932200</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="2331" spans="1:12">
@@ -96224,16 +96320,16 @@
         <v>2249</v>
       </c>
       <c r="E2331" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2331" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2331" t="s">
         <v>1536</v>
       </c>
       <c r="H2331" t="s">
-        <v>910</v>
+        <v>95</v>
       </c>
       <c r="I2331" t="s">
         <v>19</v>
@@ -96242,10 +96338,10 @@
         <v>1</v>
       </c>
       <c r="K2331">
-        <v>12652560</v>
+        <v>2932200</v>
       </c>
       <c r="L2331">
-        <v>12652560</v>
+        <v>2932200</v>
       </c>
     </row>
     <row r="2332" spans="1:12">
@@ -96262,16 +96358,16 @@
         <v>2249</v>
       </c>
       <c r="E2332" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2332" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2332" t="s">
         <v>1536</v>
       </c>
       <c r="H2332" t="s">
-        <v>2148</v>
+        <v>910</v>
       </c>
       <c r="I2332" t="s">
         <v>19</v>
@@ -96280,10 +96376,10 @@
         <v>1</v>
       </c>
       <c r="K2332">
-        <v>12052500</v>
+        <v>12652560</v>
       </c>
       <c r="L2332">
-        <v>12052500</v>
+        <v>12652560</v>
       </c>
     </row>
     <row r="2333" spans="1:12">
@@ -96300,16 +96396,16 @@
         <v>2249</v>
       </c>
       <c r="E2333" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2333" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2333" t="s">
         <v>1536</v>
       </c>
       <c r="H2333" t="s">
-        <v>197</v>
+        <v>2148</v>
       </c>
       <c r="I2333" t="s">
         <v>19</v>
@@ -96318,10 +96414,10 @@
         <v>1</v>
       </c>
       <c r="K2333">
-        <v>9697035</v>
+        <v>12052500</v>
       </c>
       <c r="L2333">
-        <v>9697035</v>
+        <v>12052500</v>
       </c>
     </row>
     <row r="2334" spans="1:12">
@@ -96338,16 +96434,16 @@
         <v>2249</v>
       </c>
       <c r="E2334" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2334" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2334" t="s">
         <v>1536</v>
       </c>
       <c r="H2334" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="I2334" t="s">
         <v>19</v>
@@ -96356,10 +96452,10 @@
         <v>1</v>
       </c>
       <c r="K2334">
-        <v>130000</v>
+        <v>9697035</v>
       </c>
       <c r="L2334">
-        <v>130000</v>
+        <v>9697035</v>
       </c>
     </row>
     <row r="2335" spans="1:12">
@@ -96376,16 +96472,16 @@
         <v>2249</v>
       </c>
       <c r="E2335" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2335" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2335" t="s">
         <v>1536</v>
       </c>
       <c r="H2335" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I2335" t="s">
         <v>19</v>
@@ -96394,10 +96490,10 @@
         <v>1</v>
       </c>
       <c r="K2335">
-        <v>300000</v>
+        <v>130000</v>
       </c>
       <c r="L2335">
-        <v>300000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="2336" spans="1:12">
@@ -96414,16 +96510,16 @@
         <v>2249</v>
       </c>
       <c r="E2336" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2336" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2336" t="s">
         <v>1536</v>
       </c>
       <c r="H2336" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I2336" t="s">
         <v>19</v>
@@ -96432,10 +96528,10 @@
         <v>1</v>
       </c>
       <c r="K2336">
-        <v>750000</v>
+        <v>300000</v>
       </c>
       <c r="L2336">
-        <v>750000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="2337" spans="1:12">
@@ -96452,16 +96548,16 @@
         <v>2249</v>
       </c>
       <c r="E2337" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2337" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2337" t="s">
         <v>1536</v>
       </c>
       <c r="H2337" t="s">
-        <v>911</v>
+        <v>190</v>
       </c>
       <c r="I2337" t="s">
         <v>19</v>
@@ -96470,10 +96566,10 @@
         <v>1</v>
       </c>
       <c r="K2337">
-        <v>1350000</v>
+        <v>750000</v>
       </c>
       <c r="L2337">
-        <v>1350000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="2338" spans="1:12">
@@ -96490,16 +96586,16 @@
         <v>2249</v>
       </c>
       <c r="E2338" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2338" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2338" t="s">
         <v>1536</v>
       </c>
       <c r="H2338" t="s">
-        <v>193</v>
+        <v>911</v>
       </c>
       <c r="I2338" t="s">
         <v>19</v>
@@ -96508,10 +96604,10 @@
         <v>1</v>
       </c>
       <c r="K2338">
-        <v>840000</v>
+        <v>1350000</v>
       </c>
       <c r="L2338">
-        <v>840000</v>
+        <v>1350000</v>
       </c>
     </row>
     <row r="2339" spans="1:12">
@@ -96528,16 +96624,16 @@
         <v>2249</v>
       </c>
       <c r="E2339" t="s">
-        <v>2449</v>
+        <v>2453</v>
       </c>
       <c r="F2339" t="s">
-        <v>2450</v>
+        <v>2454</v>
       </c>
       <c r="G2339" t="s">
         <v>1536</v>
       </c>
       <c r="H2339" t="s">
-        <v>128</v>
+        <v>193</v>
       </c>
       <c r="I2339" t="s">
         <v>19</v>
@@ -96546,10 +96642,10 @@
         <v>1</v>
       </c>
       <c r="K2339">
-        <v>1200000</v>
+        <v>840000</v>
       </c>
       <c r="L2339">
-        <v>1200000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="2340" spans="1:12">
@@ -96566,16 +96662,16 @@
         <v>2249</v>
       </c>
       <c r="E2340" t="s">
-        <v>2455</v>
+        <v>2453</v>
       </c>
       <c r="F2340" t="s">
-        <v>2456</v>
+        <v>2454</v>
       </c>
       <c r="G2340" t="s">
         <v>1536</v>
       </c>
       <c r="H2340" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="I2340" t="s">
         <v>19</v>
@@ -96584,10 +96680,10 @@
         <v>1</v>
       </c>
       <c r="K2340">
-        <v>9022500</v>
+        <v>1200000</v>
       </c>
       <c r="L2340">
-        <v>9022500</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="2341" spans="1:12">
@@ -96604,16 +96700,16 @@
         <v>2249</v>
       </c>
       <c r="E2341" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2341" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2341" t="s">
         <v>1536</v>
       </c>
       <c r="H2341" t="s">
-        <v>2457</v>
+        <v>119</v>
       </c>
       <c r="I2341" t="s">
         <v>19</v>
@@ -96622,10 +96718,10 @@
         <v>1</v>
       </c>
       <c r="K2341">
-        <v>20620280</v>
+        <v>9022500</v>
       </c>
       <c r="L2341">
-        <v>20620280</v>
+        <v>9022500</v>
       </c>
     </row>
     <row r="2342" spans="1:12">
@@ -96642,16 +96738,16 @@
         <v>2249</v>
       </c>
       <c r="E2342" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2342" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2342" t="s">
         <v>1536</v>
       </c>
       <c r="H2342" t="s">
-        <v>582</v>
+        <v>2461</v>
       </c>
       <c r="I2342" t="s">
         <v>19</v>
@@ -96660,10 +96756,10 @@
         <v>1</v>
       </c>
       <c r="K2342">
-        <v>19639260</v>
+        <v>20620280</v>
       </c>
       <c r="L2342">
-        <v>19639260</v>
+        <v>20620280</v>
       </c>
     </row>
     <row r="2343" spans="1:12">
@@ -96680,16 +96776,16 @@
         <v>2249</v>
       </c>
       <c r="E2343" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2343" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2343" t="s">
         <v>1536</v>
       </c>
       <c r="H2343" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I2343" t="s">
         <v>19</v>
@@ -96698,10 +96794,10 @@
         <v>1</v>
       </c>
       <c r="K2343">
-        <v>3226000</v>
+        <v>19639260</v>
       </c>
       <c r="L2343">
-        <v>3226000</v>
+        <v>19639260</v>
       </c>
     </row>
     <row r="2344" spans="1:12">
@@ -96718,16 +96814,16 @@
         <v>2249</v>
       </c>
       <c r="E2344" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2344" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2344" t="s">
         <v>1536</v>
       </c>
       <c r="H2344" t="s">
-        <v>729</v>
+        <v>584</v>
       </c>
       <c r="I2344" t="s">
         <v>19</v>
@@ -96736,10 +96832,10 @@
         <v>1</v>
       </c>
       <c r="K2344">
-        <v>785000</v>
+        <v>3226000</v>
       </c>
       <c r="L2344">
-        <v>785000</v>
+        <v>3226000</v>
       </c>
     </row>
     <row r="2345" spans="1:12">
@@ -96756,16 +96852,16 @@
         <v>2249</v>
       </c>
       <c r="E2345" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2345" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2345" t="s">
         <v>1536</v>
       </c>
       <c r="H2345" t="s">
-        <v>1217</v>
+        <v>729</v>
       </c>
       <c r="I2345" t="s">
         <v>19</v>
@@ -96774,10 +96870,10 @@
         <v>1</v>
       </c>
       <c r="K2345">
-        <v>8544680</v>
+        <v>785000</v>
       </c>
       <c r="L2345">
-        <v>8544680</v>
+        <v>785000</v>
       </c>
     </row>
     <row r="2346" spans="1:12">
@@ -96794,16 +96890,16 @@
         <v>2249</v>
       </c>
       <c r="E2346" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2346" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2346" t="s">
         <v>1536</v>
       </c>
       <c r="H2346" t="s">
-        <v>112</v>
+        <v>1217</v>
       </c>
       <c r="I2346" t="s">
         <v>19</v>
@@ -96812,10 +96908,10 @@
         <v>1</v>
       </c>
       <c r="K2346">
-        <v>42630220</v>
+        <v>8544680</v>
       </c>
       <c r="L2346">
-        <v>42630220</v>
+        <v>8544680</v>
       </c>
     </row>
     <row r="2347" spans="1:12">
@@ -96832,16 +96928,16 @@
         <v>2249</v>
       </c>
       <c r="E2347" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2347" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2347" t="s">
         <v>1536</v>
       </c>
       <c r="H2347" t="s">
-        <v>763</v>
+        <v>112</v>
       </c>
       <c r="I2347" t="s">
         <v>19</v>
@@ -96850,10 +96946,10 @@
         <v>1</v>
       </c>
       <c r="K2347">
-        <v>4224000</v>
+        <v>42630220</v>
       </c>
       <c r="L2347">
-        <v>4224000</v>
+        <v>42630220</v>
       </c>
     </row>
     <row r="2348" spans="1:12">
@@ -96870,16 +96966,16 @@
         <v>2249</v>
       </c>
       <c r="E2348" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2348" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2348" t="s">
         <v>1536</v>
       </c>
       <c r="H2348" t="s">
-        <v>816</v>
+        <v>763</v>
       </c>
       <c r="I2348" t="s">
         <v>19</v>
@@ -96888,10 +96984,10 @@
         <v>1</v>
       </c>
       <c r="K2348">
-        <v>8472080</v>
+        <v>4224000</v>
       </c>
       <c r="L2348">
-        <v>8472080</v>
+        <v>4224000</v>
       </c>
     </row>
     <row r="2349" spans="1:12">
@@ -96908,16 +97004,16 @@
         <v>2249</v>
       </c>
       <c r="E2349" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2349" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2349" t="s">
         <v>1536</v>
       </c>
       <c r="H2349" t="s">
-        <v>1356</v>
+        <v>816</v>
       </c>
       <c r="I2349" t="s">
         <v>19</v>
@@ -96926,10 +97022,10 @@
         <v>1</v>
       </c>
       <c r="K2349">
-        <v>6474200</v>
+        <v>8472080</v>
       </c>
       <c r="L2349">
-        <v>6474200</v>
+        <v>8472080</v>
       </c>
     </row>
     <row r="2350" spans="1:12">
@@ -96946,16 +97042,16 @@
         <v>2249</v>
       </c>
       <c r="E2350" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2350" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2350" t="s">
         <v>1536</v>
       </c>
       <c r="H2350" t="s">
-        <v>1564</v>
+        <v>1356</v>
       </c>
       <c r="I2350" t="s">
         <v>19</v>
@@ -96964,10 +97060,10 @@
         <v>1</v>
       </c>
       <c r="K2350">
-        <v>11063599</v>
+        <v>6474200</v>
       </c>
       <c r="L2350">
-        <v>11063599</v>
+        <v>6474200</v>
       </c>
     </row>
     <row r="2351" spans="1:12">
@@ -96984,16 +97080,16 @@
         <v>2249</v>
       </c>
       <c r="E2351" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2351" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2351" t="s">
         <v>1536</v>
       </c>
       <c r="H2351" t="s">
-        <v>1345</v>
+        <v>1564</v>
       </c>
       <c r="I2351" t="s">
         <v>19</v>
@@ -97002,10 +97098,10 @@
         <v>1</v>
       </c>
       <c r="K2351">
-        <v>1656920</v>
+        <v>11063599</v>
       </c>
       <c r="L2351">
-        <v>1656920</v>
+        <v>11063599</v>
       </c>
     </row>
     <row r="2352" spans="1:12">
@@ -97022,16 +97118,16 @@
         <v>2249</v>
       </c>
       <c r="E2352" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2352" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2352" t="s">
         <v>1536</v>
       </c>
       <c r="H2352" t="s">
-        <v>261</v>
+        <v>1345</v>
       </c>
       <c r="I2352" t="s">
         <v>19</v>
@@ -97040,10 +97136,10 @@
         <v>1</v>
       </c>
       <c r="K2352">
-        <v>2411600</v>
+        <v>1656920</v>
       </c>
       <c r="L2352">
-        <v>2411600</v>
+        <v>1656920</v>
       </c>
     </row>
     <row r="2353" spans="1:12">
@@ -97060,16 +97156,16 @@
         <v>2249</v>
       </c>
       <c r="E2353" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2353" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2353" t="s">
         <v>1536</v>
       </c>
       <c r="H2353" t="s">
-        <v>132</v>
+        <v>261</v>
       </c>
       <c r="I2353" t="s">
         <v>19</v>
@@ -97078,10 +97174,10 @@
         <v>1</v>
       </c>
       <c r="K2353">
-        <v>27447287</v>
+        <v>2411600</v>
       </c>
       <c r="L2353">
-        <v>27447287</v>
+        <v>2411600</v>
       </c>
     </row>
     <row r="2354" spans="1:12">
@@ -97098,16 +97194,16 @@
         <v>2249</v>
       </c>
       <c r="E2354" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2354" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2354" t="s">
         <v>1536</v>
       </c>
       <c r="H2354" t="s">
-        <v>765</v>
+        <v>132</v>
       </c>
       <c r="I2354" t="s">
         <v>19</v>
@@ -97116,10 +97212,10 @@
         <v>1</v>
       </c>
       <c r="K2354">
-        <v>24556740</v>
+        <v>27447287</v>
       </c>
       <c r="L2354">
-        <v>24556740</v>
+        <v>27447287</v>
       </c>
     </row>
     <row r="2355" spans="1:12">
@@ -97136,16 +97232,16 @@
         <v>2249</v>
       </c>
       <c r="E2355" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2355" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2355" t="s">
         <v>1536</v>
       </c>
       <c r="H2355" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="I2355" t="s">
         <v>19</v>
@@ -97154,10 +97250,10 @@
         <v>1</v>
       </c>
       <c r="K2355">
-        <v>650000</v>
+        <v>24556740</v>
       </c>
       <c r="L2355">
-        <v>650000</v>
+        <v>24556740</v>
       </c>
     </row>
     <row r="2356" spans="1:12">
@@ -97174,16 +97270,16 @@
         <v>2249</v>
       </c>
       <c r="E2356" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2356" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2356" t="s">
         <v>1536</v>
       </c>
       <c r="H2356" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I2356" t="s">
         <v>19</v>
@@ -97192,10 +97288,10 @@
         <v>1</v>
       </c>
       <c r="K2356">
-        <v>600000</v>
+        <v>650000</v>
       </c>
       <c r="L2356">
-        <v>600000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="2357" spans="1:12">
@@ -97212,16 +97308,16 @@
         <v>2249</v>
       </c>
       <c r="E2357" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2357" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2357" t="s">
         <v>1536</v>
       </c>
       <c r="H2357" t="s">
-        <v>400</v>
+        <v>770</v>
       </c>
       <c r="I2357" t="s">
         <v>19</v>
@@ -97230,10 +97326,10 @@
         <v>1</v>
       </c>
       <c r="K2357">
-        <v>2700000</v>
+        <v>600000</v>
       </c>
       <c r="L2357">
-        <v>2700000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="2358" spans="1:12">
@@ -97250,16 +97346,16 @@
         <v>2249</v>
       </c>
       <c r="E2358" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2358" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2358" t="s">
         <v>1536</v>
       </c>
       <c r="H2358" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I2358" t="s">
         <v>19</v>
@@ -97268,10 +97364,10 @@
         <v>1</v>
       </c>
       <c r="K2358">
-        <v>1430000</v>
+        <v>2700000</v>
       </c>
       <c r="L2358">
-        <v>1430000</v>
+        <v>2700000</v>
       </c>
     </row>
     <row r="2359" spans="1:12">
@@ -97288,28 +97384,2650 @@
         <v>2249</v>
       </c>
       <c r="E2359" t="s">
-        <v>2455</v>
+        <v>2459</v>
       </c>
       <c r="F2359" t="s">
-        <v>2456</v>
+        <v>2460</v>
       </c>
       <c r="G2359" t="s">
         <v>1536</v>
       </c>
       <c r="H2359" t="s">
+        <v>401</v>
+      </c>
+      <c r="I2359" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2359">
+        <v>1</v>
+      </c>
+      <c r="K2359">
+        <v>1430000</v>
+      </c>
+      <c r="L2359">
+        <v>1430000</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:12">
+      <c r="A2360">
+        <v>2357</v>
+      </c>
+      <c r="B2360">
+        <v>626402</v>
+      </c>
+      <c r="C2360" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2360" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E2360" t="s">
+        <v>2459</v>
+      </c>
+      <c r="F2360" t="s">
+        <v>2460</v>
+      </c>
+      <c r="G2360" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2360" t="s">
         <v>773</v>
       </c>
-      <c r="I2359" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2359">
-        <v>1</v>
-      </c>
-      <c r="K2359">
+      <c r="I2360" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2360">
+        <v>1</v>
+      </c>
+      <c r="K2360">
         <v>150000</v>
       </c>
-      <c r="L2359">
+      <c r="L2360">
         <v>150000</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:12">
+      <c r="A2361">
+        <v>2358</v>
+      </c>
+      <c r="B2361">
+        <v>626402</v>
+      </c>
+      <c r="C2361" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2361" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2361" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2361" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2361" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2361" t="s">
+        <v>933</v>
+      </c>
+      <c r="I2361" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2361">
+        <v>1</v>
+      </c>
+      <c r="K2361">
+        <v>7800000</v>
+      </c>
+      <c r="L2361">
+        <v>7800000</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:12">
+      <c r="A2362">
+        <v>2359</v>
+      </c>
+      <c r="B2362">
+        <v>626402</v>
+      </c>
+      <c r="C2362" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2362" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2362" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2362" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2362" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2362" t="s">
+        <v>737</v>
+      </c>
+      <c r="I2362" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2362">
+        <v>1</v>
+      </c>
+      <c r="K2362">
+        <v>1000000</v>
+      </c>
+      <c r="L2362">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:12">
+      <c r="A2363">
+        <v>2360</v>
+      </c>
+      <c r="B2363">
+        <v>626402</v>
+      </c>
+      <c r="C2363" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2363" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2363" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2363" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2363" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2363" t="s">
+        <v>738</v>
+      </c>
+      <c r="I2363" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2363">
+        <v>1</v>
+      </c>
+      <c r="K2363">
+        <v>995400</v>
+      </c>
+      <c r="L2363">
+        <v>995400</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:12">
+      <c r="A2364">
+        <v>2361</v>
+      </c>
+      <c r="B2364">
+        <v>626402</v>
+      </c>
+      <c r="C2364" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2364" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2364" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2364" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2364" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2364" t="s">
+        <v>739</v>
+      </c>
+      <c r="I2364" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2364">
+        <v>1</v>
+      </c>
+      <c r="K2364">
+        <v>998250</v>
+      </c>
+      <c r="L2364">
+        <v>998250</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:12">
+      <c r="A2365">
+        <v>2362</v>
+      </c>
+      <c r="B2365">
+        <v>626402</v>
+      </c>
+      <c r="C2365" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2365" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2365" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2365" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2365" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2365" t="s">
+        <v>740</v>
+      </c>
+      <c r="I2365" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2365">
+        <v>1</v>
+      </c>
+      <c r="K2365">
+        <v>1000000</v>
+      </c>
+      <c r="L2365">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:12">
+      <c r="A2366">
+        <v>2363</v>
+      </c>
+      <c r="B2366">
+        <v>626402</v>
+      </c>
+      <c r="C2366" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2366" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2366" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2366" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2366" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2366" t="s">
+        <v>741</v>
+      </c>
+      <c r="I2366" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2366">
+        <v>1</v>
+      </c>
+      <c r="K2366">
+        <v>992750</v>
+      </c>
+      <c r="L2366">
+        <v>992750</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:12">
+      <c r="A2367">
+        <v>2364</v>
+      </c>
+      <c r="B2367">
+        <v>626402</v>
+      </c>
+      <c r="C2367" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2367" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2367" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2367" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2367" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2367" t="s">
+        <v>742</v>
+      </c>
+      <c r="I2367" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2367">
+        <v>1</v>
+      </c>
+      <c r="K2367">
+        <v>995500</v>
+      </c>
+      <c r="L2367">
+        <v>995500</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:12">
+      <c r="A2368">
+        <v>2365</v>
+      </c>
+      <c r="B2368">
+        <v>626402</v>
+      </c>
+      <c r="C2368" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2368" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2368" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2368" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2368" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2368" t="s">
+        <v>723</v>
+      </c>
+      <c r="I2368" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2368">
+        <v>1</v>
+      </c>
+      <c r="K2368">
+        <v>1999900</v>
+      </c>
+      <c r="L2368">
+        <v>1999900</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:12">
+      <c r="A2369">
+        <v>2366</v>
+      </c>
+      <c r="B2369">
+        <v>626402</v>
+      </c>
+      <c r="C2369" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2369" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2369" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2369" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2369" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2369" t="s">
+        <v>724</v>
+      </c>
+      <c r="I2369" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2369">
+        <v>1</v>
+      </c>
+      <c r="K2369">
+        <v>1999200</v>
+      </c>
+      <c r="L2369">
+        <v>1999200</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:12">
+      <c r="A2370">
+        <v>2367</v>
+      </c>
+      <c r="B2370">
+        <v>626402</v>
+      </c>
+      <c r="C2370" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2370" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2370" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2370" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2370" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2370" t="s">
+        <v>1560</v>
+      </c>
+      <c r="I2370" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2370">
+        <v>1</v>
+      </c>
+      <c r="K2370">
+        <v>4000000</v>
+      </c>
+      <c r="L2370">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:12">
+      <c r="A2371">
+        <v>2368</v>
+      </c>
+      <c r="B2371">
+        <v>626402</v>
+      </c>
+      <c r="C2371" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2371" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2371" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2371" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2371" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2371" t="s">
+        <v>2465</v>
+      </c>
+      <c r="I2371" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2371">
+        <v>1</v>
+      </c>
+      <c r="K2371">
+        <v>2550000</v>
+      </c>
+      <c r="L2371">
+        <v>2550000</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:12">
+      <c r="A2372">
+        <v>2369</v>
+      </c>
+      <c r="B2372">
+        <v>626402</v>
+      </c>
+      <c r="C2372" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2372" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2372" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2372" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2372" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2372" t="s">
+        <v>780</v>
+      </c>
+      <c r="I2372" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2372">
+        <v>1</v>
+      </c>
+      <c r="K2372">
+        <v>5550000</v>
+      </c>
+      <c r="L2372">
+        <v>5550000</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:12">
+      <c r="A2373">
+        <v>2370</v>
+      </c>
+      <c r="B2373">
+        <v>626402</v>
+      </c>
+      <c r="C2373" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2373" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2373" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2373" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2373" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2373" t="s">
+        <v>1850</v>
+      </c>
+      <c r="I2373" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2373">
+        <v>1</v>
+      </c>
+      <c r="K2373">
+        <v>22276000</v>
+      </c>
+      <c r="L2373">
+        <v>22276000</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:12">
+      <c r="A2374">
+        <v>2371</v>
+      </c>
+      <c r="B2374">
+        <v>626402</v>
+      </c>
+      <c r="C2374" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2374" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2374" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2374" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2374" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2374" t="s">
+        <v>2466</v>
+      </c>
+      <c r="I2374" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2374">
+        <v>1</v>
+      </c>
+      <c r="K2374">
+        <v>4950000</v>
+      </c>
+      <c r="L2374">
+        <v>4950000</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:12">
+      <c r="A2375">
+        <v>2372</v>
+      </c>
+      <c r="B2375">
+        <v>626402</v>
+      </c>
+      <c r="C2375" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2375" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2375" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2375" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2375" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2375" t="s">
+        <v>2467</v>
+      </c>
+      <c r="I2375" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2375">
+        <v>1</v>
+      </c>
+      <c r="K2375">
+        <v>2810000</v>
+      </c>
+      <c r="L2375">
+        <v>2810000</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:12">
+      <c r="A2376">
+        <v>2373</v>
+      </c>
+      <c r="B2376">
+        <v>626402</v>
+      </c>
+      <c r="C2376" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2376" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2376" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2376" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2376" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2376" t="s">
+        <v>2468</v>
+      </c>
+      <c r="I2376" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2376">
+        <v>1</v>
+      </c>
+      <c r="K2376">
+        <v>500000</v>
+      </c>
+      <c r="L2376">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:12">
+      <c r="A2377">
+        <v>2374</v>
+      </c>
+      <c r="B2377">
+        <v>626402</v>
+      </c>
+      <c r="C2377" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2377" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2377" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2377" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2377" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2377" t="s">
+        <v>2469</v>
+      </c>
+      <c r="I2377" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2377">
+        <v>1</v>
+      </c>
+      <c r="K2377">
+        <v>800000</v>
+      </c>
+      <c r="L2377">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:12">
+      <c r="A2378">
+        <v>2375</v>
+      </c>
+      <c r="B2378">
+        <v>626402</v>
+      </c>
+      <c r="C2378" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2378" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2378" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2378" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2378" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2378" t="s">
+        <v>2470</v>
+      </c>
+      <c r="I2378" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2378">
+        <v>1</v>
+      </c>
+      <c r="K2378">
+        <v>3000000</v>
+      </c>
+      <c r="L2378">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:12">
+      <c r="A2379">
+        <v>2376</v>
+      </c>
+      <c r="B2379">
+        <v>626402</v>
+      </c>
+      <c r="C2379" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2379" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2379" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2379" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2379" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2379" t="s">
+        <v>2471</v>
+      </c>
+      <c r="I2379" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2379">
+        <v>1</v>
+      </c>
+      <c r="K2379">
+        <v>300000</v>
+      </c>
+      <c r="L2379">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:12">
+      <c r="A2380">
+        <v>2377</v>
+      </c>
+      <c r="B2380">
+        <v>626402</v>
+      </c>
+      <c r="C2380" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2380" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2380" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2380" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2380" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2380" t="s">
+        <v>2472</v>
+      </c>
+      <c r="I2380" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2380">
+        <v>1</v>
+      </c>
+      <c r="K2380">
+        <v>300000</v>
+      </c>
+      <c r="L2380">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:12">
+      <c r="A2381">
+        <v>2378</v>
+      </c>
+      <c r="B2381">
+        <v>626402</v>
+      </c>
+      <c r="C2381" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2381" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2381" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2381" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2381" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2381" t="s">
+        <v>2473</v>
+      </c>
+      <c r="I2381" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2381">
+        <v>1</v>
+      </c>
+      <c r="K2381">
+        <v>360000</v>
+      </c>
+      <c r="L2381">
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:12">
+      <c r="A2382">
+        <v>2379</v>
+      </c>
+      <c r="B2382">
+        <v>626402</v>
+      </c>
+      <c r="C2382" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2382" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2382" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2382" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2382" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2382" t="s">
+        <v>2474</v>
+      </c>
+      <c r="I2382" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2382">
+        <v>1</v>
+      </c>
+      <c r="K2382">
+        <v>500000</v>
+      </c>
+      <c r="L2382">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:12">
+      <c r="A2383">
+        <v>2380</v>
+      </c>
+      <c r="B2383">
+        <v>626402</v>
+      </c>
+      <c r="C2383" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2383" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2383" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2383" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2383" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2383" t="s">
+        <v>2475</v>
+      </c>
+      <c r="I2383" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2383">
+        <v>1</v>
+      </c>
+      <c r="K2383">
+        <v>400000</v>
+      </c>
+      <c r="L2383">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:12">
+      <c r="A2384">
+        <v>2381</v>
+      </c>
+      <c r="B2384">
+        <v>626402</v>
+      </c>
+      <c r="C2384" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2384" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2384" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2384" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2384" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2384" t="s">
+        <v>2476</v>
+      </c>
+      <c r="I2384" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2384">
+        <v>1</v>
+      </c>
+      <c r="K2384">
+        <v>3300000</v>
+      </c>
+      <c r="L2384">
+        <v>3300000</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:12">
+      <c r="A2385">
+        <v>2382</v>
+      </c>
+      <c r="B2385">
+        <v>626402</v>
+      </c>
+      <c r="C2385" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2385" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2385" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2385" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2385" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2385" t="s">
+        <v>2477</v>
+      </c>
+      <c r="I2385" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2385">
+        <v>1</v>
+      </c>
+      <c r="K2385">
+        <v>3600000</v>
+      </c>
+      <c r="L2385">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:12">
+      <c r="A2386">
+        <v>2383</v>
+      </c>
+      <c r="B2386">
+        <v>626402</v>
+      </c>
+      <c r="C2386" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2386" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2386" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2386" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2386" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2386" t="s">
+        <v>758</v>
+      </c>
+      <c r="I2386" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2386">
+        <v>1</v>
+      </c>
+      <c r="K2386">
+        <v>35000000</v>
+      </c>
+      <c r="L2386">
+        <v>35000000</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:12">
+      <c r="A2387">
+        <v>2384</v>
+      </c>
+      <c r="B2387">
+        <v>626402</v>
+      </c>
+      <c r="C2387" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2387" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2387" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2387" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2387" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2387" t="s">
+        <v>2478</v>
+      </c>
+      <c r="I2387" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2387">
+        <v>1</v>
+      </c>
+      <c r="K2387">
+        <v>2475000</v>
+      </c>
+      <c r="L2387">
+        <v>2475000</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:12">
+      <c r="A2388">
+        <v>2385</v>
+      </c>
+      <c r="B2388">
+        <v>626402</v>
+      </c>
+      <c r="C2388" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2388" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2388" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2388" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2388" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2388" t="s">
+        <v>2479</v>
+      </c>
+      <c r="I2388" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2388">
+        <v>1</v>
+      </c>
+      <c r="K2388">
+        <v>2055000</v>
+      </c>
+      <c r="L2388">
+        <v>2055000</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:12">
+      <c r="A2389">
+        <v>2386</v>
+      </c>
+      <c r="B2389">
+        <v>626402</v>
+      </c>
+      <c r="C2389" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2389" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2389" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2389" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2389" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2389" t="s">
+        <v>729</v>
+      </c>
+      <c r="I2389" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2389">
+        <v>1</v>
+      </c>
+      <c r="K2389">
+        <v>658400</v>
+      </c>
+      <c r="L2389">
+        <v>658400</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:12">
+      <c r="A2390">
+        <v>2387</v>
+      </c>
+      <c r="B2390">
+        <v>626402</v>
+      </c>
+      <c r="C2390" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2390" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2390" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2390" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2390" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2390" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2390" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2390">
+        <v>1</v>
+      </c>
+      <c r="K2390">
+        <v>32976940</v>
+      </c>
+      <c r="L2390">
+        <v>32976940</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:12">
+      <c r="A2391">
+        <v>2388</v>
+      </c>
+      <c r="B2391">
+        <v>626402</v>
+      </c>
+      <c r="C2391" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2391" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2391" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2391" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2391" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2391" t="s">
+        <v>816</v>
+      </c>
+      <c r="I2391" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2391">
+        <v>1</v>
+      </c>
+      <c r="K2391">
+        <v>4856020</v>
+      </c>
+      <c r="L2391">
+        <v>4856020</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:12">
+      <c r="A2392">
+        <v>2389</v>
+      </c>
+      <c r="B2392">
+        <v>626402</v>
+      </c>
+      <c r="C2392" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2392" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2392" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2392" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2392" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2392" t="s">
+        <v>1564</v>
+      </c>
+      <c r="I2392" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2392">
+        <v>1</v>
+      </c>
+      <c r="K2392">
+        <v>1050000</v>
+      </c>
+      <c r="L2392">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:12">
+      <c r="A2393">
+        <v>2390</v>
+      </c>
+      <c r="B2393">
+        <v>626402</v>
+      </c>
+      <c r="C2393" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2393" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2393" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2393" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2393" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2393" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I2393" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2393">
+        <v>1</v>
+      </c>
+      <c r="K2393">
+        <v>12952500</v>
+      </c>
+      <c r="L2393">
+        <v>12952500</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:12">
+      <c r="A2394">
+        <v>2391</v>
+      </c>
+      <c r="B2394">
+        <v>626402</v>
+      </c>
+      <c r="C2394" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2394" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2394" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2394" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2394" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2394" t="s">
+        <v>2457</v>
+      </c>
+      <c r="I2394" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2394">
+        <v>1</v>
+      </c>
+      <c r="K2394">
+        <v>15081400</v>
+      </c>
+      <c r="L2394">
+        <v>15081400</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:12">
+      <c r="A2395">
+        <v>2392</v>
+      </c>
+      <c r="B2395">
+        <v>626402</v>
+      </c>
+      <c r="C2395" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2395" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2395" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2395" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2395" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2395" t="s">
+        <v>766</v>
+      </c>
+      <c r="I2395" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2395">
+        <v>1</v>
+      </c>
+      <c r="K2395">
+        <v>20940565</v>
+      </c>
+      <c r="L2395">
+        <v>20940565</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:12">
+      <c r="A2396">
+        <v>2393</v>
+      </c>
+      <c r="B2396">
+        <v>626402</v>
+      </c>
+      <c r="C2396" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2396" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2396" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2396" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2396" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2396" t="s">
+        <v>2480</v>
+      </c>
+      <c r="I2396" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2396">
+        <v>1</v>
+      </c>
+      <c r="K2396">
+        <v>543500</v>
+      </c>
+      <c r="L2396">
+        <v>543500</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:12">
+      <c r="A2397">
+        <v>2394</v>
+      </c>
+      <c r="B2397">
+        <v>626402</v>
+      </c>
+      <c r="C2397" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2397" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2397" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2397" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2397" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2397" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2397" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2397">
+        <v>1</v>
+      </c>
+      <c r="K2397">
+        <v>159821533</v>
+      </c>
+      <c r="L2397">
+        <v>159821533</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:12">
+      <c r="A2398">
+        <v>2395</v>
+      </c>
+      <c r="B2398">
+        <v>626402</v>
+      </c>
+      <c r="C2398" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2398" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2398" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2398" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2398" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2398" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2398" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2398">
+        <v>1</v>
+      </c>
+      <c r="K2398">
+        <v>4290500</v>
+      </c>
+      <c r="L2398">
+        <v>4290500</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:12">
+      <c r="A2399">
+        <v>2396</v>
+      </c>
+      <c r="B2399">
+        <v>626402</v>
+      </c>
+      <c r="C2399" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2399" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2399" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2399" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2399" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2399" t="s">
+        <v>2481</v>
+      </c>
+      <c r="I2399" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2399">
+        <v>1</v>
+      </c>
+      <c r="K2399">
+        <v>17605160</v>
+      </c>
+      <c r="L2399">
+        <v>17605160</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:12">
+      <c r="A2400">
+        <v>2397</v>
+      </c>
+      <c r="B2400">
+        <v>626402</v>
+      </c>
+      <c r="C2400" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2400" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2400" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2400" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2400" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2400" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2400" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2400">
+        <v>1</v>
+      </c>
+      <c r="K2400">
+        <v>5308700</v>
+      </c>
+      <c r="L2400">
+        <v>5308700</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:12">
+      <c r="A2401">
+        <v>2398</v>
+      </c>
+      <c r="B2401">
+        <v>626402</v>
+      </c>
+      <c r="C2401" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2401" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2401" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2401" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2401" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2401" t="s">
+        <v>768</v>
+      </c>
+      <c r="I2401" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2401">
+        <v>1</v>
+      </c>
+      <c r="K2401">
+        <v>11499500</v>
+      </c>
+      <c r="L2401">
+        <v>11499500</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:12">
+      <c r="A2402">
+        <v>2399</v>
+      </c>
+      <c r="B2402">
+        <v>626402</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2402" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2402" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2402" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2402" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2402" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2402" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2402">
+        <v>1</v>
+      </c>
+      <c r="K2402">
+        <v>32982320</v>
+      </c>
+      <c r="L2402">
+        <v>32982320</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:12">
+      <c r="A2403">
+        <v>2400</v>
+      </c>
+      <c r="B2403">
+        <v>626402</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2403" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2403" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2403" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2403" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2403" t="s">
+        <v>586</v>
+      </c>
+      <c r="I2403" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2403">
+        <v>1</v>
+      </c>
+      <c r="K2403">
+        <v>6302000</v>
+      </c>
+      <c r="L2403">
+        <v>6302000</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:12">
+      <c r="A2404">
+        <v>2401</v>
+      </c>
+      <c r="B2404">
+        <v>626402</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2404" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2404" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2404" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2404" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2404" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2404" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2404">
+        <v>1</v>
+      </c>
+      <c r="K2404">
+        <v>7831951</v>
+      </c>
+      <c r="L2404">
+        <v>7831951</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:12">
+      <c r="A2405">
+        <v>2402</v>
+      </c>
+      <c r="B2405">
+        <v>626402</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2405" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2405" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2405" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2405" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2405" t="s">
+        <v>910</v>
+      </c>
+      <c r="I2405" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2405">
+        <v>1</v>
+      </c>
+      <c r="K2405">
+        <v>8808000</v>
+      </c>
+      <c r="L2405">
+        <v>8808000</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:12">
+      <c r="A2406">
+        <v>2403</v>
+      </c>
+      <c r="B2406">
+        <v>626402</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2406" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2406" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2406" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2406" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2406" t="s">
+        <v>2148</v>
+      </c>
+      <c r="I2406" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2406">
+        <v>1</v>
+      </c>
+      <c r="K2406">
+        <v>16452112</v>
+      </c>
+      <c r="L2406">
+        <v>16452112</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:12">
+      <c r="A2407">
+        <v>2404</v>
+      </c>
+      <c r="B2407">
+        <v>626402</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2407" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2407" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2407" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2407" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2407" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2407" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2407">
+        <v>1</v>
+      </c>
+      <c r="K2407">
+        <v>19329730</v>
+      </c>
+      <c r="L2407">
+        <v>19329730</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:12">
+      <c r="A2408">
+        <v>2405</v>
+      </c>
+      <c r="B2408">
+        <v>626402</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2408" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2408" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2408" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2408" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2408" t="s">
+        <v>2482</v>
+      </c>
+      <c r="I2408" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2408">
+        <v>1</v>
+      </c>
+      <c r="K2408">
+        <v>450000</v>
+      </c>
+      <c r="L2408">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:12">
+      <c r="A2409">
+        <v>2406</v>
+      </c>
+      <c r="B2409">
+        <v>626402</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2409" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2409" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2409" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2409" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2409" t="s">
+        <v>773</v>
+      </c>
+      <c r="I2409" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2409">
+        <v>1</v>
+      </c>
+      <c r="K2409">
+        <v>750000</v>
+      </c>
+      <c r="L2409">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:12">
+      <c r="A2410">
+        <v>2407</v>
+      </c>
+      <c r="B2410">
+        <v>626402</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2410" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2410" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2410" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2410" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2410" t="s">
+        <v>402</v>
+      </c>
+      <c r="I2410" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2410">
+        <v>1</v>
+      </c>
+      <c r="K2410">
+        <v>420000</v>
+      </c>
+      <c r="L2410">
+        <v>420000</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:12">
+      <c r="A2411">
+        <v>2408</v>
+      </c>
+      <c r="B2411">
+        <v>626402</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2411" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2411" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2411" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2411" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2411" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2411" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2411">
+        <v>1</v>
+      </c>
+      <c r="K2411">
+        <v>300000</v>
+      </c>
+      <c r="L2411">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:12">
+      <c r="A2412">
+        <v>2409</v>
+      </c>
+      <c r="B2412">
+        <v>626402</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2412" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2412" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2412" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2412" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2412" t="s">
+        <v>2483</v>
+      </c>
+      <c r="I2412" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2412">
+        <v>1</v>
+      </c>
+      <c r="K2412">
+        <v>4050000</v>
+      </c>
+      <c r="L2412">
+        <v>4050000</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:12">
+      <c r="A2413">
+        <v>2410</v>
+      </c>
+      <c r="B2413">
+        <v>626402</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2413" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2413" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2413" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2413" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2413" t="s">
+        <v>404</v>
+      </c>
+      <c r="I2413" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2413">
+        <v>1</v>
+      </c>
+      <c r="K2413">
+        <v>150000</v>
+      </c>
+      <c r="L2413">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:12">
+      <c r="A2414">
+        <v>2411</v>
+      </c>
+      <c r="B2414">
+        <v>626402</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2414" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2414" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2414" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2414" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2414" t="s">
+        <v>405</v>
+      </c>
+      <c r="I2414" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2414">
+        <v>1</v>
+      </c>
+      <c r="K2414">
+        <v>130000</v>
+      </c>
+      <c r="L2414">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:12">
+      <c r="A2415">
+        <v>2412</v>
+      </c>
+      <c r="B2415">
+        <v>626402</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2415" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2415" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F2415" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G2415" t="s">
+        <v>2464</v>
+      </c>
+      <c r="H2415" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2415" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2415">
+        <v>1</v>
+      </c>
+      <c r="K2415">
+        <v>600000</v>
+      </c>
+      <c r="L2415">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:12">
+      <c r="A2416">
+        <v>2413</v>
+      </c>
+      <c r="B2416">
+        <v>626402</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2416" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2416" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2416" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2416" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2416" t="s">
+        <v>2486</v>
+      </c>
+      <c r="I2416" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2416">
+        <v>1</v>
+      </c>
+      <c r="K2416">
+        <v>1750000</v>
+      </c>
+      <c r="L2416">
+        <v>1750000</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:12">
+      <c r="A2417">
+        <v>2414</v>
+      </c>
+      <c r="B2417">
+        <v>626402</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2417" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2417" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2417" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2417" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2417" t="s">
+        <v>2487</v>
+      </c>
+      <c r="I2417" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2417">
+        <v>1</v>
+      </c>
+      <c r="K2417">
+        <v>1800000</v>
+      </c>
+      <c r="L2417">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:12">
+      <c r="A2418">
+        <v>2415</v>
+      </c>
+      <c r="B2418">
+        <v>626402</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2418" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2418" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2418" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2418" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2418" t="s">
+        <v>780</v>
+      </c>
+      <c r="I2418" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2418">
+        <v>1</v>
+      </c>
+      <c r="K2418">
+        <v>4850000</v>
+      </c>
+      <c r="L2418">
+        <v>4850000</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:12">
+      <c r="A2419">
+        <v>2416</v>
+      </c>
+      <c r="B2419">
+        <v>626402</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2419" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2419" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2419" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2419" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2419" t="s">
+        <v>749</v>
+      </c>
+      <c r="I2419" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2419">
+        <v>1</v>
+      </c>
+      <c r="K2419">
+        <v>1000000</v>
+      </c>
+      <c r="L2419">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:12">
+      <c r="A2420">
+        <v>2417</v>
+      </c>
+      <c r="B2420">
+        <v>626402</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2420" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2420" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2420" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2420" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2420" t="s">
+        <v>750</v>
+      </c>
+      <c r="I2420" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2420">
+        <v>1</v>
+      </c>
+      <c r="K2420">
+        <v>1000000</v>
+      </c>
+      <c r="L2420">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:12">
+      <c r="A2421">
+        <v>2418</v>
+      </c>
+      <c r="B2421">
+        <v>626402</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2421" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2421" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2421" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2421" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2421" t="s">
+        <v>2488</v>
+      </c>
+      <c r="I2421" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2421">
+        <v>1</v>
+      </c>
+      <c r="K2421">
+        <v>1900000</v>
+      </c>
+      <c r="L2421">
+        <v>1900000</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:12">
+      <c r="A2422">
+        <v>2419</v>
+      </c>
+      <c r="B2422">
+        <v>626402</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2422" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2422" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2422" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2422" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2422" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I2422" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2422">
+        <v>1</v>
+      </c>
+      <c r="K2422">
+        <v>1616500</v>
+      </c>
+      <c r="L2422">
+        <v>1616500</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:12">
+      <c r="A2423">
+        <v>2420</v>
+      </c>
+      <c r="B2423">
+        <v>626402</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2423" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2423" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2423" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2423" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2423" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2423" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2423">
+        <v>1</v>
+      </c>
+      <c r="K2423">
+        <v>5374000</v>
+      </c>
+      <c r="L2423">
+        <v>5374000</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:12">
+      <c r="A2424">
+        <v>2421</v>
+      </c>
+      <c r="B2424">
+        <v>626402</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2424" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2424" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2424" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2424" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2424" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2424" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2424">
+        <v>1</v>
+      </c>
+      <c r="K2424">
+        <v>856500</v>
+      </c>
+      <c r="L2424">
+        <v>856500</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:12">
+      <c r="A2425">
+        <v>2422</v>
+      </c>
+      <c r="B2425">
+        <v>626402</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2425" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2425" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2425" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2425" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2425" t="s">
+        <v>766</v>
+      </c>
+      <c r="I2425" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2425">
+        <v>1</v>
+      </c>
+      <c r="K2425">
+        <v>450000</v>
+      </c>
+      <c r="L2425">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:12">
+      <c r="A2426">
+        <v>2423</v>
+      </c>
+      <c r="B2426">
+        <v>626402</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2426" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2426" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2426" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2426" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2426" t="s">
+        <v>2489</v>
+      </c>
+      <c r="I2426" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2426">
+        <v>1</v>
+      </c>
+      <c r="K2426">
+        <v>9372220</v>
+      </c>
+      <c r="L2426">
+        <v>9372220</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:12">
+      <c r="A2427">
+        <v>2424</v>
+      </c>
+      <c r="B2427">
+        <v>626402</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2427" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2427" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2427" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2427" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2427" t="s">
+        <v>585</v>
+      </c>
+      <c r="I2427" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2427">
+        <v>1</v>
+      </c>
+      <c r="K2427">
+        <v>2924540</v>
+      </c>
+      <c r="L2427">
+        <v>2924540</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:12">
+      <c r="A2428">
+        <v>2425</v>
+      </c>
+      <c r="B2428">
+        <v>626402</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2428" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E2428" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F2428" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G2428" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H2428" t="s">
+        <v>773</v>
+      </c>
+      <c r="I2428" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2428">
+        <v>1</v>
+      </c>
+      <c r="K2428">
+        <v>600000</v>
+      </c>
+      <c r="L2428">
+        <v>600000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE REALISASI 26 JUNI 2023
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2619">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -7824,6 +7824,54 @@
   </si>
   <si>
     <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0C.000878</t>
+  </si>
+  <si>
+    <t>'00609T</t>
+  </si>
+  <si>
+    <t>'231751303015200</t>
+  </si>
+  <si>
+    <t>'626402.175.521219.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.962.301.0G.001448</t>
+  </si>
+  <si>
+    <t>2023-06-26</t>
+  </si>
+  <si>
+    <t>'00611T</t>
+  </si>
+  <si>
+    <t>'231751303015198</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2760/BRSDM.1/KP.440/V/2023 Tanggal 24 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00612T</t>
+  </si>
+  <si>
+    <t>'231751303015199</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.3062/BRSDM.1/KP.440/VI/2023 Tanggal 7 Juni 2023,Surat Tugas Nomor:B.3149/BRSDM.1/KP.440/VI/2023 Tanggal 13 Juni 2023</t>
+  </si>
+  <si>
+    <t>'00613T</t>
+  </si>
+  <si>
+    <t>'231751303015194</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.2250,B.2250,B.2265,B.2283,B.2313/BRSDM.1/KP.440/V/2023 Tanggal 3,4,5 Mei 2023</t>
+  </si>
+  <si>
+    <t>'00615T</t>
+  </si>
+  <si>
+    <t>'231751303015201</t>
+  </si>
+  <si>
+    <t>Penggantian Uang Persediaan KKP untuk keperluan belanja barang (BPP 001 Set.BRSDM)</t>
   </si>
 </sst>
 </file>
@@ -8165,7 +8213,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2507"/>
+  <dimension ref="A1:L2515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -103369,6 +103417,310 @@
       </c>
       <c r="L2507">
         <v>1539452</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:12">
+      <c r="A2508">
+        <v>2505</v>
+      </c>
+      <c r="B2508">
+        <v>626402</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2508" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E2508" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F2508" t="s">
+        <v>2604</v>
+      </c>
+      <c r="G2508" t="s">
+        <v>1674</v>
+      </c>
+      <c r="H2508" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2508" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2508">
+        <v>1</v>
+      </c>
+      <c r="K2508">
+        <v>10000</v>
+      </c>
+      <c r="L2508">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:12">
+      <c r="A2509">
+        <v>2506</v>
+      </c>
+      <c r="B2509">
+        <v>626402</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2509" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E2509" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F2509" t="s">
+        <v>2604</v>
+      </c>
+      <c r="G2509" t="s">
+        <v>1674</v>
+      </c>
+      <c r="H2509" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2509" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2509">
+        <v>1</v>
+      </c>
+      <c r="K2509">
+        <v>728371</v>
+      </c>
+      <c r="L2509">
+        <v>728371</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:12">
+      <c r="A2510">
+        <v>2507</v>
+      </c>
+      <c r="B2510">
+        <v>626402</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2510" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E2510" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F2510" t="s">
+        <v>2604</v>
+      </c>
+      <c r="G2510" t="s">
+        <v>1674</v>
+      </c>
+      <c r="H2510" t="s">
+        <v>2605</v>
+      </c>
+      <c r="I2510" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2510">
+        <v>1</v>
+      </c>
+      <c r="K2510">
+        <v>161547</v>
+      </c>
+      <c r="L2510">
+        <v>161547</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:12">
+      <c r="A2511">
+        <v>2508</v>
+      </c>
+      <c r="B2511">
+        <v>626402</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2511" t="s">
+        <v>2606</v>
+      </c>
+      <c r="E2511" t="s">
+        <v>2607</v>
+      </c>
+      <c r="F2511" t="s">
+        <v>2608</v>
+      </c>
+      <c r="G2511" t="s">
+        <v>2609</v>
+      </c>
+      <c r="H2511" t="s">
+        <v>768</v>
+      </c>
+      <c r="I2511" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2511">
+        <v>1</v>
+      </c>
+      <c r="K2511">
+        <v>12094302</v>
+      </c>
+      <c r="L2511">
+        <v>12094302</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:12">
+      <c r="A2512">
+        <v>2509</v>
+      </c>
+      <c r="B2512">
+        <v>626402</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2512" t="s">
+        <v>2606</v>
+      </c>
+      <c r="E2512" t="s">
+        <v>2610</v>
+      </c>
+      <c r="F2512" t="s">
+        <v>2611</v>
+      </c>
+      <c r="G2512" t="s">
+        <v>2612</v>
+      </c>
+      <c r="H2512" t="s">
+        <v>729</v>
+      </c>
+      <c r="I2512" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2512">
+        <v>1</v>
+      </c>
+      <c r="K2512">
+        <v>2397500</v>
+      </c>
+      <c r="L2512">
+        <v>2397500</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:12">
+      <c r="A2513">
+        <v>2510</v>
+      </c>
+      <c r="B2513">
+        <v>626402</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2513" t="s">
+        <v>2606</v>
+      </c>
+      <c r="E2513" t="s">
+        <v>2613</v>
+      </c>
+      <c r="F2513" t="s">
+        <v>2614</v>
+      </c>
+      <c r="G2513" t="s">
+        <v>2615</v>
+      </c>
+      <c r="H2513" t="s">
+        <v>1540</v>
+      </c>
+      <c r="I2513" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2513">
+        <v>1</v>
+      </c>
+      <c r="K2513">
+        <v>780000</v>
+      </c>
+      <c r="L2513">
+        <v>780000</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:12">
+      <c r="A2514">
+        <v>2511</v>
+      </c>
+      <c r="B2514">
+        <v>626402</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2514" t="s">
+        <v>2606</v>
+      </c>
+      <c r="E2514" t="s">
+        <v>2613</v>
+      </c>
+      <c r="F2514" t="s">
+        <v>2614</v>
+      </c>
+      <c r="G2514" t="s">
+        <v>2615</v>
+      </c>
+      <c r="H2514" t="s">
+        <v>1541</v>
+      </c>
+      <c r="I2514" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2514">
+        <v>1</v>
+      </c>
+      <c r="K2514">
+        <v>750000</v>
+      </c>
+      <c r="L2514">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:12">
+      <c r="A2515">
+        <v>2512</v>
+      </c>
+      <c r="B2515">
+        <v>626402</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2515" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E2515" t="s">
+        <v>2616</v>
+      </c>
+      <c r="F2515" t="s">
+        <v>2617</v>
+      </c>
+      <c r="G2515" t="s">
+        <v>2618</v>
+      </c>
+      <c r="H2515" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2515" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2515">
+        <v>1</v>
+      </c>
+      <c r="K2515">
+        <v>17367840</v>
+      </c>
+      <c r="L2515">
+        <v>17367840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>